<commit_message>
finished version and spectrum parser
</commit_message>
<xml_diff>
--- a/doc/planning/Projektplanung_Spektrometer.xlsx
+++ b/doc/planning/Projektplanung_Spektrometer.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreas\Dropbox\YARX\10_Projekte\20_Mobile\21_iOS\1610_Spektrometer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Daten/Spektrometer/portableSpectrometer/doc/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="18960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
   </externalReferences>
   <definedNames>
     <definedName name="abc">[1]Stammdaten!$B$2:$B$9</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$GC$77</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$GC$79</definedName>
     <definedName name="Teammitglieder">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="120">
   <si>
     <t>Zeit</t>
   </si>
@@ -398,13 +398,19 @@
   <si>
     <t>​Proof of Concept</t>
   </si>
+  <si>
+    <t>Meeting Testflight</t>
+  </si>
+  <si>
+    <t>Meeting Prototyp 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1438,7 +1444,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1710,6 +1716,57 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="64" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1827,196 +1884,148 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="64" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="137">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2044,25 +2053,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Zeitplanung"/>
-      <sheetName val="Pendenzenliste"/>
       <sheetName val="Stammdaten"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Andreas Lüscher</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Raphael Bolliger</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2355,38 +2349,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:GC78"/>
+  <dimension ref="A1:GC80"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="F33" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="8" topLeftCell="EZ39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomRight" activeCell="FX51" sqref="FX51:GB51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="34" customWidth="1"/>
-    <col min="6" max="109" width="2.5703125" style="4" customWidth="1"/>
-    <col min="110" max="185" width="2.5703125" style="10" customWidth="1"/>
-    <col min="186" max="16384" width="15.5703125" style="1"/>
+    <col min="1" max="1" width="7.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="34" customWidth="1"/>
+    <col min="6" max="109" width="2.5" style="4" customWidth="1"/>
+    <col min="110" max="185" width="2.5" style="10" customWidth="1"/>
+    <col min="186" max="16384" width="15.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:185" s="12" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="116" t="s">
+    <row r="1" spans="1:185" s="12" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="133" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="135"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -2568,12 +2562,12 @@
       <c r="GB1" s="3"/>
       <c r="GC1" s="6"/>
     </row>
-    <row r="2" spans="1:185" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="125"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
+    <row r="2" spans="1:185" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="142"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="144"/>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
@@ -2755,7 +2749,7 @@
       <c r="GB2" s="50"/>
       <c r="GC2" s="13"/>
     </row>
-    <row r="3" spans="1:185" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:185" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>27</v>
       </c>
@@ -2954,852 +2948,852 @@
       <c r="GB3" s="15"/>
       <c r="GC3" s="18"/>
     </row>
-    <row r="4" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+    <row r="4" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="101" t="s">
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="102"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="102"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="102"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="102"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="102"/>
-      <c r="AC4" s="102"/>
-      <c r="AD4" s="102"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="102"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="102"/>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="102"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="102"/>
-      <c r="AM4" s="102"/>
-      <c r="AN4" s="102"/>
-      <c r="AO4" s="102" t="s">
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="119"/>
+      <c r="V4" s="119"/>
+      <c r="W4" s="119"/>
+      <c r="X4" s="119"/>
+      <c r="Y4" s="119"/>
+      <c r="Z4" s="119"/>
+      <c r="AA4" s="119"/>
+      <c r="AB4" s="119"/>
+      <c r="AC4" s="119"/>
+      <c r="AD4" s="119"/>
+      <c r="AE4" s="119"/>
+      <c r="AF4" s="119"/>
+      <c r="AG4" s="119"/>
+      <c r="AH4" s="119"/>
+      <c r="AI4" s="119"/>
+      <c r="AJ4" s="119"/>
+      <c r="AK4" s="119"/>
+      <c r="AL4" s="119"/>
+      <c r="AM4" s="119"/>
+      <c r="AN4" s="119"/>
+      <c r="AO4" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AP4" s="102"/>
-      <c r="AQ4" s="102"/>
-      <c r="AR4" s="102"/>
-      <c r="AS4" s="102"/>
-      <c r="AT4" s="102"/>
-      <c r="AU4" s="102"/>
-      <c r="AV4" s="102"/>
-      <c r="AW4" s="102"/>
-      <c r="AX4" s="102"/>
-      <c r="AY4" s="102"/>
-      <c r="AZ4" s="102"/>
-      <c r="BA4" s="102"/>
-      <c r="BB4" s="102"/>
-      <c r="BC4" s="102"/>
-      <c r="BD4" s="102"/>
-      <c r="BE4" s="102"/>
-      <c r="BF4" s="102"/>
-      <c r="BG4" s="102"/>
-      <c r="BH4" s="102"/>
-      <c r="BI4" s="102"/>
-      <c r="BJ4" s="102"/>
-      <c r="BK4" s="102"/>
-      <c r="BL4" s="102"/>
-      <c r="BM4" s="102"/>
-      <c r="BN4" s="102"/>
-      <c r="BO4" s="102"/>
-      <c r="BP4" s="102"/>
-      <c r="BQ4" s="102"/>
-      <c r="BR4" s="102"/>
-      <c r="BS4" s="102"/>
-      <c r="BT4" s="102"/>
-      <c r="BU4" s="102"/>
-      <c r="BV4" s="102"/>
-      <c r="BW4" s="102"/>
-      <c r="BX4" s="102"/>
-      <c r="BY4" s="102"/>
-      <c r="BZ4" s="102"/>
-      <c r="CA4" s="102" t="s">
+      <c r="AP4" s="119"/>
+      <c r="AQ4" s="119"/>
+      <c r="AR4" s="119"/>
+      <c r="AS4" s="119"/>
+      <c r="AT4" s="119"/>
+      <c r="AU4" s="119"/>
+      <c r="AV4" s="119"/>
+      <c r="AW4" s="119"/>
+      <c r="AX4" s="119"/>
+      <c r="AY4" s="119"/>
+      <c r="AZ4" s="119"/>
+      <c r="BA4" s="119"/>
+      <c r="BB4" s="119"/>
+      <c r="BC4" s="119"/>
+      <c r="BD4" s="119"/>
+      <c r="BE4" s="119"/>
+      <c r="BF4" s="119"/>
+      <c r="BG4" s="119"/>
+      <c r="BH4" s="119"/>
+      <c r="BI4" s="119"/>
+      <c r="BJ4" s="119"/>
+      <c r="BK4" s="119"/>
+      <c r="BL4" s="119"/>
+      <c r="BM4" s="119"/>
+      <c r="BN4" s="119"/>
+      <c r="BO4" s="119"/>
+      <c r="BP4" s="119"/>
+      <c r="BQ4" s="119"/>
+      <c r="BR4" s="119"/>
+      <c r="BS4" s="119"/>
+      <c r="BT4" s="119"/>
+      <c r="BU4" s="119"/>
+      <c r="BV4" s="119"/>
+      <c r="BW4" s="119"/>
+      <c r="BX4" s="119"/>
+      <c r="BY4" s="119"/>
+      <c r="BZ4" s="119"/>
+      <c r="CA4" s="119" t="s">
         <v>93</v>
       </c>
-      <c r="CB4" s="102"/>
-      <c r="CC4" s="102"/>
-      <c r="CD4" s="102"/>
-      <c r="CE4" s="102"/>
-      <c r="CF4" s="102"/>
-      <c r="CG4" s="102"/>
-      <c r="CH4" s="102"/>
-      <c r="CI4" s="102"/>
-      <c r="CJ4" s="102"/>
-      <c r="CK4" s="102"/>
-      <c r="CL4" s="102"/>
-      <c r="CM4" s="102"/>
-      <c r="CN4" s="102"/>
-      <c r="CO4" s="102"/>
-      <c r="CP4" s="102"/>
-      <c r="CQ4" s="102"/>
-      <c r="CR4" s="102"/>
-      <c r="CS4" s="102"/>
-      <c r="CT4" s="102"/>
-      <c r="CU4" s="102"/>
-      <c r="CV4" s="102" t="s">
+      <c r="CB4" s="119"/>
+      <c r="CC4" s="119"/>
+      <c r="CD4" s="119"/>
+      <c r="CE4" s="119"/>
+      <c r="CF4" s="119"/>
+      <c r="CG4" s="119"/>
+      <c r="CH4" s="119"/>
+      <c r="CI4" s="119"/>
+      <c r="CJ4" s="119"/>
+      <c r="CK4" s="119"/>
+      <c r="CL4" s="119"/>
+      <c r="CM4" s="119"/>
+      <c r="CN4" s="119"/>
+      <c r="CO4" s="119"/>
+      <c r="CP4" s="119"/>
+      <c r="CQ4" s="119"/>
+      <c r="CR4" s="119"/>
+      <c r="CS4" s="119"/>
+      <c r="CT4" s="119"/>
+      <c r="CU4" s="119"/>
+      <c r="CV4" s="119" t="s">
         <v>94</v>
       </c>
-      <c r="CW4" s="102"/>
-      <c r="CX4" s="102"/>
-      <c r="CY4" s="102"/>
-      <c r="CZ4" s="102"/>
-      <c r="DA4" s="102"/>
-      <c r="DB4" s="102"/>
-      <c r="DC4" s="102"/>
-      <c r="DD4" s="102"/>
-      <c r="DE4" s="102"/>
-      <c r="DF4" s="102"/>
-      <c r="DG4" s="102"/>
-      <c r="DH4" s="102"/>
-      <c r="DI4" s="102"/>
-      <c r="DJ4" s="102"/>
-      <c r="DK4" s="102"/>
-      <c r="DL4" s="102"/>
-      <c r="DM4" s="102"/>
-      <c r="DN4" s="102"/>
-      <c r="DO4" s="102"/>
-      <c r="DP4" s="102"/>
-      <c r="DQ4" s="102"/>
-      <c r="DR4" s="102"/>
-      <c r="DS4" s="102"/>
-      <c r="DT4" s="102"/>
-      <c r="DU4" s="102"/>
-      <c r="DV4" s="102"/>
-      <c r="DW4" s="102"/>
-      <c r="DX4" s="102"/>
-      <c r="DY4" s="102"/>
-      <c r="DZ4" s="102"/>
-      <c r="EA4" s="102"/>
-      <c r="EB4" s="102"/>
-      <c r="EC4" s="102"/>
-      <c r="ED4" s="102"/>
-      <c r="EE4" s="102" t="s">
+      <c r="CW4" s="119"/>
+      <c r="CX4" s="119"/>
+      <c r="CY4" s="119"/>
+      <c r="CZ4" s="119"/>
+      <c r="DA4" s="119"/>
+      <c r="DB4" s="119"/>
+      <c r="DC4" s="119"/>
+      <c r="DD4" s="119"/>
+      <c r="DE4" s="119"/>
+      <c r="DF4" s="119"/>
+      <c r="DG4" s="119"/>
+      <c r="DH4" s="119"/>
+      <c r="DI4" s="119"/>
+      <c r="DJ4" s="119"/>
+      <c r="DK4" s="119"/>
+      <c r="DL4" s="119"/>
+      <c r="DM4" s="119"/>
+      <c r="DN4" s="119"/>
+      <c r="DO4" s="119"/>
+      <c r="DP4" s="119"/>
+      <c r="DQ4" s="119"/>
+      <c r="DR4" s="119"/>
+      <c r="DS4" s="119"/>
+      <c r="DT4" s="119"/>
+      <c r="DU4" s="119"/>
+      <c r="DV4" s="119"/>
+      <c r="DW4" s="119"/>
+      <c r="DX4" s="119"/>
+      <c r="DY4" s="119"/>
+      <c r="DZ4" s="119"/>
+      <c r="EA4" s="119"/>
+      <c r="EB4" s="119"/>
+      <c r="EC4" s="119"/>
+      <c r="ED4" s="119"/>
+      <c r="EE4" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="EF4" s="102"/>
-      <c r="EG4" s="102"/>
-      <c r="EH4" s="102"/>
-      <c r="EI4" s="102"/>
-      <c r="EJ4" s="102"/>
-      <c r="EK4" s="102"/>
-      <c r="EL4" s="102"/>
-      <c r="EM4" s="102"/>
-      <c r="EN4" s="102"/>
-      <c r="EO4" s="102"/>
-      <c r="EP4" s="102"/>
-      <c r="EQ4" s="102"/>
-      <c r="ER4" s="102"/>
-      <c r="ES4" s="102"/>
-      <c r="ET4" s="102"/>
-      <c r="EU4" s="102"/>
-      <c r="EV4" s="102"/>
-      <c r="EW4" s="102"/>
-      <c r="EX4" s="102"/>
-      <c r="EY4" s="102"/>
-      <c r="EZ4" s="102"/>
-      <c r="FA4" s="102"/>
-      <c r="FB4" s="102"/>
-      <c r="FC4" s="102"/>
-      <c r="FD4" s="102"/>
-      <c r="FE4" s="102"/>
-      <c r="FF4" s="102"/>
-      <c r="FG4" s="102"/>
-      <c r="FH4" s="102"/>
-      <c r="FI4" s="102"/>
-      <c r="FJ4" s="102"/>
-      <c r="FK4" s="102"/>
-      <c r="FL4" s="102"/>
-      <c r="FM4" s="102" t="s">
+      <c r="EF4" s="119"/>
+      <c r="EG4" s="119"/>
+      <c r="EH4" s="119"/>
+      <c r="EI4" s="119"/>
+      <c r="EJ4" s="119"/>
+      <c r="EK4" s="119"/>
+      <c r="EL4" s="119"/>
+      <c r="EM4" s="119"/>
+      <c r="EN4" s="119"/>
+      <c r="EO4" s="119"/>
+      <c r="EP4" s="119"/>
+      <c r="EQ4" s="119"/>
+      <c r="ER4" s="119"/>
+      <c r="ES4" s="119"/>
+      <c r="ET4" s="119"/>
+      <c r="EU4" s="119"/>
+      <c r="EV4" s="119"/>
+      <c r="EW4" s="119"/>
+      <c r="EX4" s="119"/>
+      <c r="EY4" s="119"/>
+      <c r="EZ4" s="119"/>
+      <c r="FA4" s="119"/>
+      <c r="FB4" s="119"/>
+      <c r="FC4" s="119"/>
+      <c r="FD4" s="119"/>
+      <c r="FE4" s="119"/>
+      <c r="FF4" s="119"/>
+      <c r="FG4" s="119"/>
+      <c r="FH4" s="119"/>
+      <c r="FI4" s="119"/>
+      <c r="FJ4" s="119"/>
+      <c r="FK4" s="119"/>
+      <c r="FL4" s="119"/>
+      <c r="FM4" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="FN4" s="102"/>
-      <c r="FO4" s="102"/>
-      <c r="FP4" s="102"/>
-      <c r="FQ4" s="102"/>
-      <c r="FR4" s="102"/>
-      <c r="FS4" s="102"/>
-      <c r="FT4" s="102"/>
-      <c r="FU4" s="102"/>
-      <c r="FV4" s="102"/>
-      <c r="FW4" s="102"/>
-      <c r="FX4" s="102"/>
-      <c r="FY4" s="102"/>
-      <c r="FZ4" s="102"/>
-      <c r="GA4" s="102"/>
-      <c r="GB4" s="102"/>
-      <c r="GC4" s="103"/>
+      <c r="FN4" s="119"/>
+      <c r="FO4" s="119"/>
+      <c r="FP4" s="119"/>
+      <c r="FQ4" s="119"/>
+      <c r="FR4" s="119"/>
+      <c r="FS4" s="119"/>
+      <c r="FT4" s="119"/>
+      <c r="FU4" s="119"/>
+      <c r="FV4" s="119"/>
+      <c r="FW4" s="119"/>
+      <c r="FX4" s="119"/>
+      <c r="FY4" s="119"/>
+      <c r="FZ4" s="119"/>
+      <c r="GA4" s="119"/>
+      <c r="GB4" s="119"/>
+      <c r="GC4" s="120"/>
     </row>
-    <row r="5" spans="1:185" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="s">
+    <row r="5" spans="1:185" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="114"/>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="106">
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="123">
         <v>2016</v>
       </c>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
-      <c r="AA5" s="107"/>
-      <c r="AB5" s="107"/>
-      <c r="AC5" s="107"/>
-      <c r="AD5" s="107"/>
-      <c r="AE5" s="107"/>
-      <c r="AF5" s="107"/>
-      <c r="AG5" s="107"/>
-      <c r="AH5" s="107"/>
-      <c r="AI5" s="107"/>
-      <c r="AJ5" s="107"/>
-      <c r="AK5" s="107"/>
-      <c r="AL5" s="107"/>
-      <c r="AM5" s="107"/>
-      <c r="AN5" s="107"/>
-      <c r="AO5" s="107"/>
-      <c r="AP5" s="107"/>
-      <c r="AQ5" s="107"/>
-      <c r="AR5" s="107"/>
-      <c r="AS5" s="107"/>
-      <c r="AT5" s="107"/>
-      <c r="AU5" s="107"/>
-      <c r="AV5" s="107"/>
-      <c r="AW5" s="107"/>
-      <c r="AX5" s="107"/>
-      <c r="AY5" s="107"/>
-      <c r="AZ5" s="107"/>
-      <c r="BA5" s="107"/>
-      <c r="BB5" s="107"/>
-      <c r="BC5" s="107"/>
-      <c r="BD5" s="107"/>
-      <c r="BE5" s="107"/>
-      <c r="BF5" s="107"/>
-      <c r="BG5" s="107"/>
-      <c r="BH5" s="107"/>
-      <c r="BI5" s="107"/>
-      <c r="BJ5" s="107"/>
-      <c r="BK5" s="107"/>
-      <c r="BL5" s="107"/>
-      <c r="BM5" s="107"/>
-      <c r="BN5" s="107"/>
-      <c r="BO5" s="107"/>
-      <c r="BP5" s="107"/>
-      <c r="BQ5" s="107"/>
-      <c r="BR5" s="107"/>
-      <c r="BS5" s="107"/>
-      <c r="BT5" s="107"/>
-      <c r="BU5" s="107"/>
-      <c r="BV5" s="107"/>
-      <c r="BW5" s="107"/>
-      <c r="BX5" s="107"/>
-      <c r="BY5" s="107"/>
-      <c r="BZ5" s="107"/>
-      <c r="CA5" s="107"/>
-      <c r="CB5" s="107"/>
-      <c r="CC5" s="107"/>
-      <c r="CD5" s="107"/>
-      <c r="CE5" s="107"/>
-      <c r="CF5" s="107"/>
-      <c r="CG5" s="107"/>
-      <c r="CH5" s="107"/>
-      <c r="CI5" s="107"/>
-      <c r="CJ5" s="107"/>
-      <c r="CK5" s="107"/>
-      <c r="CL5" s="107"/>
-      <c r="CM5" s="107"/>
-      <c r="CN5" s="107"/>
-      <c r="CO5" s="107"/>
-      <c r="CP5" s="107"/>
-      <c r="CQ5" s="107"/>
-      <c r="CR5" s="107"/>
-      <c r="CS5" s="107"/>
-      <c r="CT5" s="107"/>
-      <c r="CU5" s="107"/>
-      <c r="CV5" s="107"/>
-      <c r="CW5" s="107"/>
-      <c r="CX5" s="107"/>
-      <c r="CY5" s="107"/>
-      <c r="CZ5" s="107"/>
-      <c r="DA5" s="107"/>
-      <c r="DB5" s="107"/>
-      <c r="DC5" s="107"/>
-      <c r="DD5" s="107"/>
-      <c r="DE5" s="107"/>
-      <c r="DF5" s="107">
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="124"/>
+      <c r="T5" s="124"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="124"/>
+      <c r="X5" s="124"/>
+      <c r="Y5" s="124"/>
+      <c r="Z5" s="124"/>
+      <c r="AA5" s="124"/>
+      <c r="AB5" s="124"/>
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="124"/>
+      <c r="AE5" s="124"/>
+      <c r="AF5" s="124"/>
+      <c r="AG5" s="124"/>
+      <c r="AH5" s="124"/>
+      <c r="AI5" s="124"/>
+      <c r="AJ5" s="124"/>
+      <c r="AK5" s="124"/>
+      <c r="AL5" s="124"/>
+      <c r="AM5" s="124"/>
+      <c r="AN5" s="124"/>
+      <c r="AO5" s="124"/>
+      <c r="AP5" s="124"/>
+      <c r="AQ5" s="124"/>
+      <c r="AR5" s="124"/>
+      <c r="AS5" s="124"/>
+      <c r="AT5" s="124"/>
+      <c r="AU5" s="124"/>
+      <c r="AV5" s="124"/>
+      <c r="AW5" s="124"/>
+      <c r="AX5" s="124"/>
+      <c r="AY5" s="124"/>
+      <c r="AZ5" s="124"/>
+      <c r="BA5" s="124"/>
+      <c r="BB5" s="124"/>
+      <c r="BC5" s="124"/>
+      <c r="BD5" s="124"/>
+      <c r="BE5" s="124"/>
+      <c r="BF5" s="124"/>
+      <c r="BG5" s="124"/>
+      <c r="BH5" s="124"/>
+      <c r="BI5" s="124"/>
+      <c r="BJ5" s="124"/>
+      <c r="BK5" s="124"/>
+      <c r="BL5" s="124"/>
+      <c r="BM5" s="124"/>
+      <c r="BN5" s="124"/>
+      <c r="BO5" s="124"/>
+      <c r="BP5" s="124"/>
+      <c r="BQ5" s="124"/>
+      <c r="BR5" s="124"/>
+      <c r="BS5" s="124"/>
+      <c r="BT5" s="124"/>
+      <c r="BU5" s="124"/>
+      <c r="BV5" s="124"/>
+      <c r="BW5" s="124"/>
+      <c r="BX5" s="124"/>
+      <c r="BY5" s="124"/>
+      <c r="BZ5" s="124"/>
+      <c r="CA5" s="124"/>
+      <c r="CB5" s="124"/>
+      <c r="CC5" s="124"/>
+      <c r="CD5" s="124"/>
+      <c r="CE5" s="124"/>
+      <c r="CF5" s="124"/>
+      <c r="CG5" s="124"/>
+      <c r="CH5" s="124"/>
+      <c r="CI5" s="124"/>
+      <c r="CJ5" s="124"/>
+      <c r="CK5" s="124"/>
+      <c r="CL5" s="124"/>
+      <c r="CM5" s="124"/>
+      <c r="CN5" s="124"/>
+      <c r="CO5" s="124"/>
+      <c r="CP5" s="124"/>
+      <c r="CQ5" s="124"/>
+      <c r="CR5" s="124"/>
+      <c r="CS5" s="124"/>
+      <c r="CT5" s="124"/>
+      <c r="CU5" s="124"/>
+      <c r="CV5" s="124"/>
+      <c r="CW5" s="124"/>
+      <c r="CX5" s="124"/>
+      <c r="CY5" s="124"/>
+      <c r="CZ5" s="124"/>
+      <c r="DA5" s="124"/>
+      <c r="DB5" s="124"/>
+      <c r="DC5" s="124"/>
+      <c r="DD5" s="124"/>
+      <c r="DE5" s="124"/>
+      <c r="DF5" s="124">
         <v>2017</v>
       </c>
-      <c r="DG5" s="107"/>
-      <c r="DH5" s="107"/>
-      <c r="DI5" s="107"/>
-      <c r="DJ5" s="107"/>
-      <c r="DK5" s="107"/>
-      <c r="DL5" s="107"/>
-      <c r="DM5" s="107"/>
-      <c r="DN5" s="107"/>
-      <c r="DO5" s="107"/>
-      <c r="DP5" s="107"/>
-      <c r="DQ5" s="107"/>
-      <c r="DR5" s="107"/>
-      <c r="DS5" s="107"/>
-      <c r="DT5" s="107"/>
-      <c r="DU5" s="107"/>
-      <c r="DV5" s="107"/>
-      <c r="DW5" s="107"/>
-      <c r="DX5" s="107"/>
-      <c r="DY5" s="107"/>
-      <c r="DZ5" s="107"/>
-      <c r="EA5" s="107"/>
-      <c r="EB5" s="107"/>
-      <c r="EC5" s="107"/>
-      <c r="ED5" s="107"/>
-      <c r="EE5" s="107"/>
-      <c r="EF5" s="107"/>
-      <c r="EG5" s="107"/>
-      <c r="EH5" s="107"/>
-      <c r="EI5" s="107"/>
-      <c r="EJ5" s="107"/>
-      <c r="EK5" s="107"/>
-      <c r="EL5" s="107"/>
-      <c r="EM5" s="107"/>
-      <c r="EN5" s="107"/>
-      <c r="EO5" s="107"/>
-      <c r="EP5" s="107"/>
-      <c r="EQ5" s="107"/>
-      <c r="ER5" s="107"/>
-      <c r="ES5" s="107"/>
-      <c r="ET5" s="107"/>
-      <c r="EU5" s="107"/>
-      <c r="EV5" s="107"/>
-      <c r="EW5" s="107"/>
-      <c r="EX5" s="107"/>
-      <c r="EY5" s="107"/>
-      <c r="EZ5" s="107"/>
-      <c r="FA5" s="107"/>
-      <c r="FB5" s="107"/>
-      <c r="FC5" s="107"/>
-      <c r="FD5" s="107"/>
-      <c r="FE5" s="107"/>
-      <c r="FF5" s="107"/>
-      <c r="FG5" s="107"/>
-      <c r="FH5" s="107"/>
-      <c r="FI5" s="107"/>
-      <c r="FJ5" s="107"/>
-      <c r="FK5" s="107"/>
-      <c r="FL5" s="107"/>
-      <c r="FM5" s="107"/>
-      <c r="FN5" s="107"/>
-      <c r="FO5" s="107"/>
-      <c r="FP5" s="107"/>
-      <c r="FQ5" s="107"/>
-      <c r="FR5" s="107"/>
-      <c r="FS5" s="107"/>
-      <c r="FT5" s="107"/>
-      <c r="FU5" s="107"/>
-      <c r="FV5" s="107"/>
-      <c r="FW5" s="107"/>
-      <c r="FX5" s="107"/>
-      <c r="FY5" s="107"/>
-      <c r="FZ5" s="107"/>
-      <c r="GA5" s="107"/>
-      <c r="GB5" s="107"/>
-      <c r="GC5" s="129"/>
+      <c r="DG5" s="124"/>
+      <c r="DH5" s="124"/>
+      <c r="DI5" s="124"/>
+      <c r="DJ5" s="124"/>
+      <c r="DK5" s="124"/>
+      <c r="DL5" s="124"/>
+      <c r="DM5" s="124"/>
+      <c r="DN5" s="124"/>
+      <c r="DO5" s="124"/>
+      <c r="DP5" s="124"/>
+      <c r="DQ5" s="124"/>
+      <c r="DR5" s="124"/>
+      <c r="DS5" s="124"/>
+      <c r="DT5" s="124"/>
+      <c r="DU5" s="124"/>
+      <c r="DV5" s="124"/>
+      <c r="DW5" s="124"/>
+      <c r="DX5" s="124"/>
+      <c r="DY5" s="124"/>
+      <c r="DZ5" s="124"/>
+      <c r="EA5" s="124"/>
+      <c r="EB5" s="124"/>
+      <c r="EC5" s="124"/>
+      <c r="ED5" s="124"/>
+      <c r="EE5" s="124"/>
+      <c r="EF5" s="124"/>
+      <c r="EG5" s="124"/>
+      <c r="EH5" s="124"/>
+      <c r="EI5" s="124"/>
+      <c r="EJ5" s="124"/>
+      <c r="EK5" s="124"/>
+      <c r="EL5" s="124"/>
+      <c r="EM5" s="124"/>
+      <c r="EN5" s="124"/>
+      <c r="EO5" s="124"/>
+      <c r="EP5" s="124"/>
+      <c r="EQ5" s="124"/>
+      <c r="ER5" s="124"/>
+      <c r="ES5" s="124"/>
+      <c r="ET5" s="124"/>
+      <c r="EU5" s="124"/>
+      <c r="EV5" s="124"/>
+      <c r="EW5" s="124"/>
+      <c r="EX5" s="124"/>
+      <c r="EY5" s="124"/>
+      <c r="EZ5" s="124"/>
+      <c r="FA5" s="124"/>
+      <c r="FB5" s="124"/>
+      <c r="FC5" s="124"/>
+      <c r="FD5" s="124"/>
+      <c r="FE5" s="124"/>
+      <c r="FF5" s="124"/>
+      <c r="FG5" s="124"/>
+      <c r="FH5" s="124"/>
+      <c r="FI5" s="124"/>
+      <c r="FJ5" s="124"/>
+      <c r="FK5" s="124"/>
+      <c r="FL5" s="124"/>
+      <c r="FM5" s="124"/>
+      <c r="FN5" s="124"/>
+      <c r="FO5" s="124"/>
+      <c r="FP5" s="124"/>
+      <c r="FQ5" s="124"/>
+      <c r="FR5" s="124"/>
+      <c r="FS5" s="124"/>
+      <c r="FT5" s="124"/>
+      <c r="FU5" s="124"/>
+      <c r="FV5" s="124"/>
+      <c r="FW5" s="124"/>
+      <c r="FX5" s="124"/>
+      <c r="FY5" s="124"/>
+      <c r="FZ5" s="124"/>
+      <c r="GA5" s="124"/>
+      <c r="GB5" s="124"/>
+      <c r="GC5" s="146"/>
     </row>
-    <row r="6" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+    <row r="6" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="104" t="s">
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="105"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="105" t="s">
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="105"/>
-      <c r="T6" s="105"/>
-      <c r="U6" s="105"/>
-      <c r="V6" s="105"/>
-      <c r="W6" s="105"/>
-      <c r="X6" s="105"/>
-      <c r="Y6" s="105"/>
-      <c r="Z6" s="105"/>
-      <c r="AA6" s="105"/>
-      <c r="AB6" s="105"/>
-      <c r="AC6" s="105"/>
-      <c r="AD6" s="105"/>
-      <c r="AE6" s="105"/>
-      <c r="AF6" s="105"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="105"/>
-      <c r="AL6" s="105"/>
-      <c r="AM6" s="105"/>
-      <c r="AN6" s="105"/>
-      <c r="AO6" s="105"/>
-      <c r="AP6" s="105"/>
-      <c r="AQ6" s="105"/>
-      <c r="AR6" s="105"/>
-      <c r="AS6" s="105"/>
-      <c r="AT6" s="105"/>
-      <c r="AU6" s="105"/>
-      <c r="AV6" s="105"/>
-      <c r="AW6" s="105" t="s">
+      <c r="S6" s="122"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="122"/>
+      <c r="Y6" s="122"/>
+      <c r="Z6" s="122"/>
+      <c r="AA6" s="122"/>
+      <c r="AB6" s="122"/>
+      <c r="AC6" s="122"/>
+      <c r="AD6" s="122"/>
+      <c r="AE6" s="122"/>
+      <c r="AF6" s="122"/>
+      <c r="AG6" s="122"/>
+      <c r="AH6" s="122"/>
+      <c r="AI6" s="122"/>
+      <c r="AJ6" s="122"/>
+      <c r="AK6" s="122"/>
+      <c r="AL6" s="122"/>
+      <c r="AM6" s="122"/>
+      <c r="AN6" s="122"/>
+      <c r="AO6" s="122"/>
+      <c r="AP6" s="122"/>
+      <c r="AQ6" s="122"/>
+      <c r="AR6" s="122"/>
+      <c r="AS6" s="122"/>
+      <c r="AT6" s="122"/>
+      <c r="AU6" s="122"/>
+      <c r="AV6" s="122"/>
+      <c r="AW6" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="AX6" s="105"/>
-      <c r="AY6" s="105"/>
-      <c r="AZ6" s="105"/>
-      <c r="BA6" s="105"/>
-      <c r="BB6" s="105"/>
-      <c r="BC6" s="105"/>
-      <c r="BD6" s="105"/>
-      <c r="BE6" s="105"/>
-      <c r="BF6" s="105"/>
-      <c r="BG6" s="105"/>
-      <c r="BH6" s="105"/>
-      <c r="BI6" s="105"/>
-      <c r="BJ6" s="105"/>
-      <c r="BK6" s="105"/>
-      <c r="BL6" s="105"/>
-      <c r="BM6" s="105"/>
-      <c r="BN6" s="105"/>
-      <c r="BO6" s="105"/>
-      <c r="BP6" s="105"/>
-      <c r="BQ6" s="105"/>
-      <c r="BR6" s="105"/>
-      <c r="BS6" s="105"/>
-      <c r="BT6" s="105"/>
-      <c r="BU6" s="105"/>
-      <c r="BV6" s="105"/>
-      <c r="BW6" s="105"/>
-      <c r="BX6" s="105"/>
-      <c r="BY6" s="105"/>
-      <c r="BZ6" s="105"/>
-      <c r="CA6" s="105" t="s">
+      <c r="AX6" s="122"/>
+      <c r="AY6" s="122"/>
+      <c r="AZ6" s="122"/>
+      <c r="BA6" s="122"/>
+      <c r="BB6" s="122"/>
+      <c r="BC6" s="122"/>
+      <c r="BD6" s="122"/>
+      <c r="BE6" s="122"/>
+      <c r="BF6" s="122"/>
+      <c r="BG6" s="122"/>
+      <c r="BH6" s="122"/>
+      <c r="BI6" s="122"/>
+      <c r="BJ6" s="122"/>
+      <c r="BK6" s="122"/>
+      <c r="BL6" s="122"/>
+      <c r="BM6" s="122"/>
+      <c r="BN6" s="122"/>
+      <c r="BO6" s="122"/>
+      <c r="BP6" s="122"/>
+      <c r="BQ6" s="122"/>
+      <c r="BR6" s="122"/>
+      <c r="BS6" s="122"/>
+      <c r="BT6" s="122"/>
+      <c r="BU6" s="122"/>
+      <c r="BV6" s="122"/>
+      <c r="BW6" s="122"/>
+      <c r="BX6" s="122"/>
+      <c r="BY6" s="122"/>
+      <c r="BZ6" s="122"/>
+      <c r="CA6" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="CB6" s="105"/>
-      <c r="CC6" s="105"/>
-      <c r="CD6" s="105"/>
-      <c r="CE6" s="105"/>
-      <c r="CF6" s="105"/>
-      <c r="CG6" s="105"/>
-      <c r="CH6" s="105"/>
-      <c r="CI6" s="105"/>
-      <c r="CJ6" s="105"/>
-      <c r="CK6" s="105"/>
-      <c r="CL6" s="105"/>
-      <c r="CM6" s="105"/>
-      <c r="CN6" s="105"/>
-      <c r="CO6" s="105"/>
-      <c r="CP6" s="105"/>
-      <c r="CQ6" s="105"/>
-      <c r="CR6" s="105"/>
-      <c r="CS6" s="105"/>
-      <c r="CT6" s="105"/>
-      <c r="CU6" s="105"/>
-      <c r="CV6" s="105"/>
-      <c r="CW6" s="105"/>
-      <c r="CX6" s="105"/>
-      <c r="CY6" s="105"/>
-      <c r="CZ6" s="105"/>
-      <c r="DA6" s="105"/>
-      <c r="DB6" s="105"/>
-      <c r="DC6" s="105"/>
-      <c r="DD6" s="105"/>
-      <c r="DE6" s="105"/>
-      <c r="DF6" s="105" t="s">
+      <c r="CB6" s="122"/>
+      <c r="CC6" s="122"/>
+      <c r="CD6" s="122"/>
+      <c r="CE6" s="122"/>
+      <c r="CF6" s="122"/>
+      <c r="CG6" s="122"/>
+      <c r="CH6" s="122"/>
+      <c r="CI6" s="122"/>
+      <c r="CJ6" s="122"/>
+      <c r="CK6" s="122"/>
+      <c r="CL6" s="122"/>
+      <c r="CM6" s="122"/>
+      <c r="CN6" s="122"/>
+      <c r="CO6" s="122"/>
+      <c r="CP6" s="122"/>
+      <c r="CQ6" s="122"/>
+      <c r="CR6" s="122"/>
+      <c r="CS6" s="122"/>
+      <c r="CT6" s="122"/>
+      <c r="CU6" s="122"/>
+      <c r="CV6" s="122"/>
+      <c r="CW6" s="122"/>
+      <c r="CX6" s="122"/>
+      <c r="CY6" s="122"/>
+      <c r="CZ6" s="122"/>
+      <c r="DA6" s="122"/>
+      <c r="DB6" s="122"/>
+      <c r="DC6" s="122"/>
+      <c r="DD6" s="122"/>
+      <c r="DE6" s="122"/>
+      <c r="DF6" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="DG6" s="105"/>
-      <c r="DH6" s="105"/>
-      <c r="DI6" s="105"/>
-      <c r="DJ6" s="105"/>
-      <c r="DK6" s="105"/>
-      <c r="DL6" s="105"/>
-      <c r="DM6" s="105"/>
-      <c r="DN6" s="105"/>
-      <c r="DO6" s="105"/>
-      <c r="DP6" s="105"/>
-      <c r="DQ6" s="105"/>
-      <c r="DR6" s="105"/>
-      <c r="DS6" s="105"/>
-      <c r="DT6" s="105"/>
-      <c r="DU6" s="105"/>
-      <c r="DV6" s="105"/>
-      <c r="DW6" s="105"/>
-      <c r="DX6" s="105"/>
-      <c r="DY6" s="105"/>
-      <c r="DZ6" s="105"/>
-      <c r="EA6" s="105"/>
-      <c r="EB6" s="105"/>
-      <c r="EC6" s="105"/>
-      <c r="ED6" s="105"/>
-      <c r="EE6" s="105"/>
-      <c r="EF6" s="105"/>
-      <c r="EG6" s="105"/>
-      <c r="EH6" s="105"/>
-      <c r="EI6" s="105"/>
-      <c r="EJ6" s="105"/>
-      <c r="EK6" s="105" t="s">
+      <c r="DG6" s="122"/>
+      <c r="DH6" s="122"/>
+      <c r="DI6" s="122"/>
+      <c r="DJ6" s="122"/>
+      <c r="DK6" s="122"/>
+      <c r="DL6" s="122"/>
+      <c r="DM6" s="122"/>
+      <c r="DN6" s="122"/>
+      <c r="DO6" s="122"/>
+      <c r="DP6" s="122"/>
+      <c r="DQ6" s="122"/>
+      <c r="DR6" s="122"/>
+      <c r="DS6" s="122"/>
+      <c r="DT6" s="122"/>
+      <c r="DU6" s="122"/>
+      <c r="DV6" s="122"/>
+      <c r="DW6" s="122"/>
+      <c r="DX6" s="122"/>
+      <c r="DY6" s="122"/>
+      <c r="DZ6" s="122"/>
+      <c r="EA6" s="122"/>
+      <c r="EB6" s="122"/>
+      <c r="EC6" s="122"/>
+      <c r="ED6" s="122"/>
+      <c r="EE6" s="122"/>
+      <c r="EF6" s="122"/>
+      <c r="EG6" s="122"/>
+      <c r="EH6" s="122"/>
+      <c r="EI6" s="122"/>
+      <c r="EJ6" s="122"/>
+      <c r="EK6" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="EL6" s="105"/>
-      <c r="EM6" s="105"/>
-      <c r="EN6" s="105"/>
-      <c r="EO6" s="105"/>
-      <c r="EP6" s="105"/>
-      <c r="EQ6" s="105"/>
-      <c r="ER6" s="105"/>
-      <c r="ES6" s="105"/>
-      <c r="ET6" s="105"/>
-      <c r="EU6" s="105"/>
-      <c r="EV6" s="105"/>
-      <c r="EW6" s="105"/>
-      <c r="EX6" s="105"/>
-      <c r="EY6" s="105"/>
-      <c r="EZ6" s="105"/>
-      <c r="FA6" s="105"/>
-      <c r="FB6" s="105"/>
-      <c r="FC6" s="105"/>
-      <c r="FD6" s="105"/>
-      <c r="FE6" s="105"/>
-      <c r="FF6" s="105"/>
-      <c r="FG6" s="105"/>
-      <c r="FH6" s="105"/>
-      <c r="FI6" s="105"/>
-      <c r="FJ6" s="105"/>
-      <c r="FK6" s="105"/>
-      <c r="FL6" s="105"/>
-      <c r="FM6" s="105" t="s">
+      <c r="EL6" s="122"/>
+      <c r="EM6" s="122"/>
+      <c r="EN6" s="122"/>
+      <c r="EO6" s="122"/>
+      <c r="EP6" s="122"/>
+      <c r="EQ6" s="122"/>
+      <c r="ER6" s="122"/>
+      <c r="ES6" s="122"/>
+      <c r="ET6" s="122"/>
+      <c r="EU6" s="122"/>
+      <c r="EV6" s="122"/>
+      <c r="EW6" s="122"/>
+      <c r="EX6" s="122"/>
+      <c r="EY6" s="122"/>
+      <c r="EZ6" s="122"/>
+      <c r="FA6" s="122"/>
+      <c r="FB6" s="122"/>
+      <c r="FC6" s="122"/>
+      <c r="FD6" s="122"/>
+      <c r="FE6" s="122"/>
+      <c r="FF6" s="122"/>
+      <c r="FG6" s="122"/>
+      <c r="FH6" s="122"/>
+      <c r="FI6" s="122"/>
+      <c r="FJ6" s="122"/>
+      <c r="FK6" s="122"/>
+      <c r="FL6" s="122"/>
+      <c r="FM6" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="FN6" s="105"/>
-      <c r="FO6" s="105"/>
-      <c r="FP6" s="105"/>
-      <c r="FQ6" s="105"/>
-      <c r="FR6" s="105"/>
-      <c r="FS6" s="105"/>
-      <c r="FT6" s="105"/>
-      <c r="FU6" s="105"/>
-      <c r="FV6" s="105"/>
-      <c r="FW6" s="105"/>
-      <c r="FX6" s="105"/>
-      <c r="FY6" s="105"/>
-      <c r="FZ6" s="105"/>
-      <c r="GA6" s="105"/>
-      <c r="GB6" s="105"/>
-      <c r="GC6" s="128"/>
+      <c r="FN6" s="122"/>
+      <c r="FO6" s="122"/>
+      <c r="FP6" s="122"/>
+      <c r="FQ6" s="122"/>
+      <c r="FR6" s="122"/>
+      <c r="FS6" s="122"/>
+      <c r="FT6" s="122"/>
+      <c r="FU6" s="122"/>
+      <c r="FV6" s="122"/>
+      <c r="FW6" s="122"/>
+      <c r="FX6" s="122"/>
+      <c r="FY6" s="122"/>
+      <c r="FZ6" s="122"/>
+      <c r="GA6" s="122"/>
+      <c r="GB6" s="122"/>
+      <c r="GC6" s="145"/>
     </row>
-    <row r="7" spans="1:185" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+    <row r="7" spans="1:185" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="106" t="s">
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
-      <c r="I7" s="107"/>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="111" t="s">
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="107"/>
-      <c r="O7" s="107"/>
-      <c r="P7" s="107"/>
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="111" t="s">
+      <c r="N7" s="124"/>
+      <c r="O7" s="124"/>
+      <c r="P7" s="124"/>
+      <c r="Q7" s="124"/>
+      <c r="R7" s="124"/>
+      <c r="S7" s="129"/>
+      <c r="T7" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="107"/>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="112"/>
-      <c r="AA7" s="111" t="s">
+      <c r="U7" s="124"/>
+      <c r="V7" s="124"/>
+      <c r="W7" s="124"/>
+      <c r="X7" s="124"/>
+      <c r="Y7" s="124"/>
+      <c r="Z7" s="129"/>
+      <c r="AA7" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="AB7" s="107"/>
-      <c r="AC7" s="107"/>
-      <c r="AD7" s="107"/>
-      <c r="AE7" s="107"/>
-      <c r="AF7" s="107"/>
-      <c r="AG7" s="112"/>
-      <c r="AH7" s="111" t="s">
+      <c r="AB7" s="124"/>
+      <c r="AC7" s="124"/>
+      <c r="AD7" s="124"/>
+      <c r="AE7" s="124"/>
+      <c r="AF7" s="124"/>
+      <c r="AG7" s="129"/>
+      <c r="AH7" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="AI7" s="107"/>
-      <c r="AJ7" s="107"/>
-      <c r="AK7" s="107"/>
-      <c r="AL7" s="107"/>
-      <c r="AM7" s="107"/>
-      <c r="AN7" s="112"/>
-      <c r="AO7" s="111" t="s">
+      <c r="AI7" s="124"/>
+      <c r="AJ7" s="124"/>
+      <c r="AK7" s="124"/>
+      <c r="AL7" s="124"/>
+      <c r="AM7" s="124"/>
+      <c r="AN7" s="129"/>
+      <c r="AO7" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="AP7" s="107"/>
-      <c r="AQ7" s="107"/>
-      <c r="AR7" s="107"/>
-      <c r="AS7" s="107"/>
-      <c r="AT7" s="107"/>
-      <c r="AU7" s="112"/>
-      <c r="AV7" s="111" t="s">
+      <c r="AP7" s="124"/>
+      <c r="AQ7" s="124"/>
+      <c r="AR7" s="124"/>
+      <c r="AS7" s="124"/>
+      <c r="AT7" s="124"/>
+      <c r="AU7" s="129"/>
+      <c r="AV7" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="AW7" s="107"/>
-      <c r="AX7" s="107"/>
-      <c r="AY7" s="107"/>
-      <c r="AZ7" s="107"/>
-      <c r="BA7" s="107"/>
-      <c r="BB7" s="112"/>
-      <c r="BC7" s="111" t="s">
+      <c r="AW7" s="124"/>
+      <c r="AX7" s="124"/>
+      <c r="AY7" s="124"/>
+      <c r="AZ7" s="124"/>
+      <c r="BA7" s="124"/>
+      <c r="BB7" s="129"/>
+      <c r="BC7" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="BD7" s="107"/>
-      <c r="BE7" s="107"/>
-      <c r="BF7" s="107"/>
-      <c r="BG7" s="107"/>
-      <c r="BH7" s="107"/>
-      <c r="BI7" s="112"/>
-      <c r="BJ7" s="111" t="s">
+      <c r="BD7" s="124"/>
+      <c r="BE7" s="124"/>
+      <c r="BF7" s="124"/>
+      <c r="BG7" s="124"/>
+      <c r="BH7" s="124"/>
+      <c r="BI7" s="129"/>
+      <c r="BJ7" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="BK7" s="107"/>
-      <c r="BL7" s="107"/>
-      <c r="BM7" s="107"/>
-      <c r="BN7" s="107"/>
-      <c r="BO7" s="107"/>
-      <c r="BP7" s="112"/>
-      <c r="BQ7" s="111" t="s">
+      <c r="BK7" s="124"/>
+      <c r="BL7" s="124"/>
+      <c r="BM7" s="124"/>
+      <c r="BN7" s="124"/>
+      <c r="BO7" s="124"/>
+      <c r="BP7" s="129"/>
+      <c r="BQ7" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="BR7" s="107"/>
-      <c r="BS7" s="107"/>
-      <c r="BT7" s="107"/>
-      <c r="BU7" s="107"/>
-      <c r="BV7" s="107"/>
-      <c r="BW7" s="112"/>
-      <c r="BX7" s="111" t="s">
+      <c r="BR7" s="124"/>
+      <c r="BS7" s="124"/>
+      <c r="BT7" s="124"/>
+      <c r="BU7" s="124"/>
+      <c r="BV7" s="124"/>
+      <c r="BW7" s="129"/>
+      <c r="BX7" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="BY7" s="107"/>
-      <c r="BZ7" s="107"/>
-      <c r="CA7" s="107"/>
-      <c r="CB7" s="107"/>
-      <c r="CC7" s="107"/>
-      <c r="CD7" s="112"/>
-      <c r="CE7" s="111" t="s">
+      <c r="BY7" s="124"/>
+      <c r="BZ7" s="124"/>
+      <c r="CA7" s="124"/>
+      <c r="CB7" s="124"/>
+      <c r="CC7" s="124"/>
+      <c r="CD7" s="129"/>
+      <c r="CE7" s="128" t="s">
         <v>16</v>
       </c>
-      <c r="CF7" s="107"/>
-      <c r="CG7" s="107"/>
-      <c r="CH7" s="107"/>
-      <c r="CI7" s="107"/>
-      <c r="CJ7" s="107"/>
-      <c r="CK7" s="112"/>
-      <c r="CL7" s="111" t="s">
+      <c r="CF7" s="124"/>
+      <c r="CG7" s="124"/>
+      <c r="CH7" s="124"/>
+      <c r="CI7" s="124"/>
+      <c r="CJ7" s="124"/>
+      <c r="CK7" s="129"/>
+      <c r="CL7" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="CM7" s="107"/>
-      <c r="CN7" s="107"/>
-      <c r="CO7" s="107"/>
-      <c r="CP7" s="107"/>
-      <c r="CQ7" s="107"/>
-      <c r="CR7" s="112"/>
-      <c r="CS7" s="111" t="s">
+      <c r="CM7" s="124"/>
+      <c r="CN7" s="124"/>
+      <c r="CO7" s="124"/>
+      <c r="CP7" s="124"/>
+      <c r="CQ7" s="124"/>
+      <c r="CR7" s="129"/>
+      <c r="CS7" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="CT7" s="107"/>
-      <c r="CU7" s="107"/>
-      <c r="CV7" s="107"/>
-      <c r="CW7" s="107"/>
-      <c r="CX7" s="107"/>
-      <c r="CY7" s="112"/>
-      <c r="CZ7" s="111" t="s">
+      <c r="CT7" s="124"/>
+      <c r="CU7" s="124"/>
+      <c r="CV7" s="124"/>
+      <c r="CW7" s="124"/>
+      <c r="CX7" s="124"/>
+      <c r="CY7" s="129"/>
+      <c r="CZ7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="DA7" s="107"/>
-      <c r="DB7" s="107"/>
-      <c r="DC7" s="107"/>
-      <c r="DD7" s="107"/>
-      <c r="DE7" s="107"/>
-      <c r="DF7" s="107"/>
-      <c r="DG7" s="111" t="s">
+      <c r="DA7" s="124"/>
+      <c r="DB7" s="124"/>
+      <c r="DC7" s="124"/>
+      <c r="DD7" s="124"/>
+      <c r="DE7" s="124"/>
+      <c r="DF7" s="124"/>
+      <c r="DG7" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="DH7" s="107"/>
-      <c r="DI7" s="107"/>
-      <c r="DJ7" s="107"/>
-      <c r="DK7" s="107"/>
-      <c r="DL7" s="107"/>
-      <c r="DM7" s="112"/>
-      <c r="DN7" s="107" t="s">
+      <c r="DH7" s="124"/>
+      <c r="DI7" s="124"/>
+      <c r="DJ7" s="124"/>
+      <c r="DK7" s="124"/>
+      <c r="DL7" s="124"/>
+      <c r="DM7" s="129"/>
+      <c r="DN7" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="DO7" s="107"/>
-      <c r="DP7" s="107"/>
-      <c r="DQ7" s="107"/>
-      <c r="DR7" s="107"/>
-      <c r="DS7" s="107"/>
-      <c r="DT7" s="107"/>
-      <c r="DU7" s="111" t="s">
+      <c r="DO7" s="124"/>
+      <c r="DP7" s="124"/>
+      <c r="DQ7" s="124"/>
+      <c r="DR7" s="124"/>
+      <c r="DS7" s="124"/>
+      <c r="DT7" s="124"/>
+      <c r="DU7" s="128" t="s">
         <v>52</v>
       </c>
-      <c r="DV7" s="107"/>
-      <c r="DW7" s="107"/>
-      <c r="DX7" s="107"/>
-      <c r="DY7" s="107"/>
-      <c r="DZ7" s="107"/>
-      <c r="EA7" s="112"/>
-      <c r="EB7" s="107" t="s">
+      <c r="DV7" s="124"/>
+      <c r="DW7" s="124"/>
+      <c r="DX7" s="124"/>
+      <c r="DY7" s="124"/>
+      <c r="DZ7" s="124"/>
+      <c r="EA7" s="129"/>
+      <c r="EB7" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="EC7" s="107"/>
-      <c r="ED7" s="107"/>
-      <c r="EE7" s="107"/>
-      <c r="EF7" s="107"/>
-      <c r="EG7" s="107"/>
-      <c r="EH7" s="107"/>
-      <c r="EI7" s="111" t="s">
+      <c r="EC7" s="124"/>
+      <c r="ED7" s="124"/>
+      <c r="EE7" s="124"/>
+      <c r="EF7" s="124"/>
+      <c r="EG7" s="124"/>
+      <c r="EH7" s="124"/>
+      <c r="EI7" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="EJ7" s="107"/>
-      <c r="EK7" s="107"/>
-      <c r="EL7" s="107"/>
-      <c r="EM7" s="107"/>
-      <c r="EN7" s="107"/>
-      <c r="EO7" s="112"/>
-      <c r="EP7" s="107" t="s">
+      <c r="EJ7" s="124"/>
+      <c r="EK7" s="124"/>
+      <c r="EL7" s="124"/>
+      <c r="EM7" s="124"/>
+      <c r="EN7" s="124"/>
+      <c r="EO7" s="129"/>
+      <c r="EP7" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="EQ7" s="107"/>
-      <c r="ER7" s="107"/>
-      <c r="ES7" s="107"/>
-      <c r="ET7" s="107"/>
-      <c r="EU7" s="107"/>
-      <c r="EV7" s="107"/>
-      <c r="EW7" s="111" t="s">
+      <c r="EQ7" s="124"/>
+      <c r="ER7" s="124"/>
+      <c r="ES7" s="124"/>
+      <c r="ET7" s="124"/>
+      <c r="EU7" s="124"/>
+      <c r="EV7" s="124"/>
+      <c r="EW7" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="EX7" s="107"/>
-      <c r="EY7" s="107"/>
-      <c r="EZ7" s="107"/>
-      <c r="FA7" s="107"/>
-      <c r="FB7" s="107"/>
-      <c r="FC7" s="112"/>
-      <c r="FD7" s="107" t="s">
+      <c r="EX7" s="124"/>
+      <c r="EY7" s="124"/>
+      <c r="EZ7" s="124"/>
+      <c r="FA7" s="124"/>
+      <c r="FB7" s="124"/>
+      <c r="FC7" s="129"/>
+      <c r="FD7" s="124" t="s">
         <v>57</v>
       </c>
-      <c r="FE7" s="107"/>
-      <c r="FF7" s="107"/>
-      <c r="FG7" s="107"/>
-      <c r="FH7" s="107"/>
-      <c r="FI7" s="107"/>
-      <c r="FJ7" s="107"/>
-      <c r="FK7" s="111" t="s">
+      <c r="FE7" s="124"/>
+      <c r="FF7" s="124"/>
+      <c r="FG7" s="124"/>
+      <c r="FH7" s="124"/>
+      <c r="FI7" s="124"/>
+      <c r="FJ7" s="124"/>
+      <c r="FK7" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="FL7" s="107"/>
-      <c r="FM7" s="107"/>
-      <c r="FN7" s="107"/>
-      <c r="FO7" s="107"/>
-      <c r="FP7" s="107"/>
-      <c r="FQ7" s="112"/>
-      <c r="FR7" s="107" t="s">
+      <c r="FL7" s="124"/>
+      <c r="FM7" s="124"/>
+      <c r="FN7" s="124"/>
+      <c r="FO7" s="124"/>
+      <c r="FP7" s="124"/>
+      <c r="FQ7" s="129"/>
+      <c r="FR7" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="FS7" s="107"/>
-      <c r="FT7" s="107"/>
-      <c r="FU7" s="107"/>
-      <c r="FV7" s="107"/>
-      <c r="FW7" s="107"/>
-      <c r="FX7" s="107"/>
-      <c r="FY7" s="111" t="s">
+      <c r="FS7" s="124"/>
+      <c r="FT7" s="124"/>
+      <c r="FU7" s="124"/>
+      <c r="FV7" s="124"/>
+      <c r="FW7" s="124"/>
+      <c r="FX7" s="124"/>
+      <c r="FY7" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="FZ7" s="107"/>
-      <c r="GA7" s="107"/>
-      <c r="GB7" s="107"/>
-      <c r="GC7" s="129"/>
+      <c r="FZ7" s="124"/>
+      <c r="GA7" s="124"/>
+      <c r="GB7" s="124"/>
+      <c r="GC7" s="146"/>
     </row>
-    <row r="8" spans="1:185" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="108" t="s">
+    <row r="8" spans="1:185" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="110"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="127"/>
       <c r="F8" s="25">
         <v>19</v>
       </c>
@@ -4341,7 +4335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A9" s="33"/>
       <c r="B9" s="9"/>
       <c r="C9" s="7"/>
@@ -4527,7 +4521,7 @@
       <c r="GB9" s="7"/>
       <c r="GC9" s="8"/>
     </row>
-    <row r="10" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
         <v>32</v>
       </c>
@@ -4720,7 +4714,7 @@
       <c r="GB10" s="40"/>
       <c r="GC10" s="45"/>
     </row>
-    <row r="11" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="31"/>
       <c r="B11" s="48" t="s">
         <v>96</v>
@@ -4911,7 +4905,7 @@
       <c r="GB11" s="11"/>
       <c r="GC11" s="24"/>
     </row>
-    <row r="12" spans="1:185" s="61" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:185" s="61" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
       <c r="B12" s="54"/>
       <c r="C12" s="55"/>
@@ -5098,7 +5092,7 @@
       <c r="GB12" s="56"/>
       <c r="GC12" s="60"/>
     </row>
-    <row r="13" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A13" s="46"/>
       <c r="B13" s="9" t="s">
         <v>68</v>
@@ -5288,7 +5282,7 @@
       <c r="GB13" s="11"/>
       <c r="GC13" s="24"/>
     </row>
-    <row r="14" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="31"/>
       <c r="B14" s="48"/>
       <c r="C14" s="11"/>
@@ -5475,7 +5469,7 @@
       <c r="GB14" s="11"/>
       <c r="GC14" s="24"/>
     </row>
-    <row r="15" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
       <c r="B15" s="9" t="s">
         <v>69</v>
@@ -5665,7 +5659,7 @@
       <c r="GB15" s="11"/>
       <c r="GC15" s="24"/>
     </row>
-    <row r="16" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="31"/>
       <c r="B16" s="48"/>
       <c r="C16" s="11"/>
@@ -5852,7 +5846,7 @@
       <c r="GB16" s="11"/>
       <c r="GC16" s="24"/>
     </row>
-    <row r="17" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A17" s="46"/>
       <c r="B17" s="9" t="s">
         <v>70</v>
@@ -6042,7 +6036,7 @@
       <c r="GB17" s="11"/>
       <c r="GC17" s="24"/>
     </row>
-    <row r="18" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A18" s="33"/>
       <c r="B18" s="9"/>
       <c r="C18" s="7"/>
@@ -6228,7 +6222,7 @@
       <c r="GB18" s="11"/>
       <c r="GC18" s="24"/>
     </row>
-    <row r="19" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="43" t="s">
         <v>33</v>
       </c>
@@ -6421,7 +6415,7 @@
       <c r="GB19" s="40"/>
       <c r="GC19" s="45"/>
     </row>
-    <row r="20" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A20" s="46"/>
       <c r="B20" s="9" t="s">
         <v>71</v>
@@ -6611,7 +6605,7 @@
       <c r="GB20" s="11"/>
       <c r="GC20" s="24"/>
     </row>
-    <row r="21" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46"/>
       <c r="B21" s="9"/>
       <c r="C21" s="47"/>
@@ -6797,7 +6791,7 @@
       <c r="GB21" s="11"/>
       <c r="GC21" s="24"/>
     </row>
-    <row r="22" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A22" s="46"/>
       <c r="B22" s="9" t="s">
         <v>73</v>
@@ -6987,7 +6981,7 @@
       <c r="GB22" s="11"/>
       <c r="GC22" s="24"/>
     </row>
-    <row r="23" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="46"/>
       <c r="B23" s="9"/>
       <c r="C23" s="47"/>
@@ -7173,7 +7167,7 @@
       <c r="GB23" s="11"/>
       <c r="GC23" s="24"/>
     </row>
-    <row r="24" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A24" s="46"/>
       <c r="B24" s="9" t="s">
         <v>72</v>
@@ -7363,7 +7357,7 @@
       <c r="GB24" s="11"/>
       <c r="GC24" s="24"/>
     </row>
-    <row r="25" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A25" s="33"/>
       <c r="B25" s="9"/>
       <c r="C25" s="7"/>
@@ -7549,7 +7543,7 @@
       <c r="GB25" s="11"/>
       <c r="GC25" s="24"/>
     </row>
-    <row r="26" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
         <v>34</v>
       </c>
@@ -7742,7 +7736,7 @@
       <c r="GB26" s="40"/>
       <c r="GC26" s="45"/>
     </row>
-    <row r="27" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="31"/>
       <c r="B27" s="48" t="s">
         <v>74</v>
@@ -7933,7 +7927,7 @@
       <c r="GB27" s="11"/>
       <c r="GC27" s="24"/>
     </row>
-    <row r="28" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31"/>
       <c r="B28" s="48"/>
       <c r="C28" s="11"/>
@@ -8120,7 +8114,7 @@
       <c r="GB28" s="11"/>
       <c r="GC28" s="24"/>
     </row>
-    <row r="29" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
       <c r="B29" s="48" t="s">
         <v>77</v>
@@ -8311,7 +8305,7 @@
       <c r="GB29" s="11"/>
       <c r="GC29" s="24"/>
     </row>
-    <row r="30" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="48"/>
       <c r="C30" s="11"/>
@@ -8498,7 +8492,7 @@
       <c r="GB30" s="11"/>
       <c r="GC30" s="24"/>
     </row>
-    <row r="31" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A31" s="46"/>
       <c r="B31" s="9" t="s">
         <v>91</v>
@@ -8688,7 +8682,7 @@
       <c r="GB31" s="11"/>
       <c r="GC31" s="24"/>
     </row>
-    <row r="32" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A32" s="33"/>
       <c r="B32" s="9"/>
       <c r="C32" s="7"/>
@@ -8874,7 +8868,7 @@
       <c r="GB32" s="11"/>
       <c r="GC32" s="24"/>
     </row>
-    <row r="33" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="43" t="s">
         <v>35</v>
       </c>
@@ -9067,7 +9061,7 @@
       <c r="GB33" s="40"/>
       <c r="GC33" s="45"/>
     </row>
-    <row r="34" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
       <c r="B34" s="48" t="s">
         <v>78</v>
@@ -9258,7 +9252,7 @@
       <c r="GB34" s="11"/>
       <c r="GC34" s="24"/>
     </row>
-    <row r="35" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
       <c r="B35" s="48"/>
       <c r="C35" s="49"/>
@@ -9445,7 +9439,7 @@
       <c r="GB35" s="11"/>
       <c r="GC35" s="24"/>
     </row>
-    <row r="36" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="31"/>
       <c r="B36" s="48" t="s">
         <v>88</v>
@@ -9636,7 +9630,7 @@
       <c r="GB36" s="11"/>
       <c r="GC36" s="24"/>
     </row>
-    <row r="37" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
       <c r="B37" s="48"/>
       <c r="C37" s="49"/>
@@ -9823,7 +9817,7 @@
       <c r="GB37" s="11"/>
       <c r="GC37" s="24"/>
     </row>
-    <row r="38" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="43" t="s">
         <v>36</v>
       </c>
@@ -10016,7 +10010,7 @@
       <c r="GB38" s="40"/>
       <c r="GC38" s="45"/>
     </row>
-    <row r="39" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
       <c r="B39" s="2" t="s">
         <v>87</v>
@@ -10207,7 +10201,7 @@
       <c r="GB39" s="11"/>
       <c r="GC39" s="24"/>
     </row>
-    <row r="40" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="31"/>
       <c r="C40" s="49"/>
       <c r="D40" s="11"/>
@@ -10393,7 +10387,7 @@
       <c r="GB40" s="11"/>
       <c r="GC40" s="24"/>
     </row>
-    <row r="41" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="31"/>
       <c r="B41" s="48" t="s">
         <v>86</v>
@@ -10584,7 +10578,7 @@
       <c r="GB41" s="11"/>
       <c r="GC41" s="24"/>
     </row>
-    <row r="42" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="31"/>
       <c r="B42" s="48"/>
       <c r="C42" s="49"/>
@@ -10771,7 +10765,7 @@
       <c r="GB42" s="11"/>
       <c r="GC42" s="24"/>
     </row>
-    <row r="43" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="43" t="s">
         <v>37</v>
       </c>
@@ -10964,7 +10958,7 @@
       <c r="GB43" s="40"/>
       <c r="GC43" s="45"/>
     </row>
-    <row r="44" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="31"/>
       <c r="B44" s="48" t="s">
         <v>89</v>
@@ -11155,7 +11149,7 @@
       <c r="GB44" s="11"/>
       <c r="GC44" s="24"/>
     </row>
-    <row r="45" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
       <c r="B45" s="48"/>
       <c r="C45" s="49"/>
@@ -11342,7 +11336,7 @@
       <c r="GB45" s="11"/>
       <c r="GC45" s="24"/>
     </row>
-    <row r="46" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="31"/>
       <c r="B46" s="48" t="s">
         <v>79</v>
@@ -11533,7 +11527,7 @@
       <c r="GB46" s="11"/>
       <c r="GC46" s="24"/>
     </row>
-    <row r="47" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="31"/>
       <c r="B47" s="48"/>
       <c r="C47" s="49"/>
@@ -11720,7 +11714,7 @@
       <c r="GB47" s="11"/>
       <c r="GC47" s="24"/>
     </row>
-    <row r="48" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="43" t="s">
         <v>83</v>
       </c>
@@ -11911,7 +11905,7 @@
       <c r="GB48" s="40"/>
       <c r="GC48" s="45"/>
     </row>
-    <row r="49" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="31"/>
       <c r="B49" s="48" t="s">
         <v>85</v>
@@ -12102,7 +12096,7 @@
       <c r="GB49" s="11"/>
       <c r="GC49" s="24"/>
     </row>
-    <row r="50" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="31"/>
       <c r="B50" s="48"/>
       <c r="C50" s="49"/>
@@ -12289,7 +12283,7 @@
       <c r="GB50" s="11"/>
       <c r="GC50" s="24"/>
     </row>
-    <row r="51" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:185" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="31"/>
       <c r="B51" s="48" t="s">
         <v>90</v>
@@ -12480,7 +12474,7 @@
       <c r="GB51" s="83"/>
       <c r="GC51" s="89"/>
     </row>
-    <row r="52" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A52" s="33"/>
       <c r="B52" s="9"/>
       <c r="C52" s="7"/>
@@ -12666,7 +12660,7 @@
       <c r="GB52" s="11"/>
       <c r="GC52" s="24"/>
     </row>
-    <row r="53" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="43" t="s">
         <v>36</v>
       </c>
@@ -12857,7 +12851,7 @@
       <c r="GB53" s="40"/>
       <c r="GC53" s="45"/>
     </row>
-    <row r="54" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
       <c r="B54" s="9" t="s">
         <v>38</v>
@@ -13047,7 +13041,7 @@
       <c r="GB54" s="11"/>
       <c r="GC54" s="24"/>
     </row>
-    <row r="55" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="33"/>
       <c r="B55" s="9"/>
       <c r="C55" s="7"/>
@@ -13233,7 +13227,7 @@
       <c r="GB55" s="11"/>
       <c r="GC55" s="24"/>
     </row>
-    <row r="56" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A56" s="33"/>
       <c r="B56" s="9" t="s">
         <v>44</v>
@@ -13423,7 +13417,7 @@
       <c r="GB56" s="11"/>
       <c r="GC56" s="24"/>
     </row>
-    <row r="57" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="33"/>
       <c r="B57" s="9"/>
       <c r="C57" s="7"/>
@@ -13609,7 +13603,7 @@
       <c r="GB57" s="11"/>
       <c r="GC57" s="24"/>
     </row>
-    <row r="58" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A58" s="33"/>
       <c r="B58" s="9" t="s">
         <v>46</v>
@@ -13799,7 +13793,7 @@
       <c r="GB58" s="11"/>
       <c r="GC58" s="24"/>
     </row>
-    <row r="59" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A59" s="33"/>
       <c r="B59" s="9"/>
       <c r="C59" s="7"/>
@@ -13985,7 +13979,7 @@
       <c r="GB59" s="11"/>
       <c r="GC59" s="24"/>
     </row>
-    <row r="60" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:185" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="43" t="s">
         <v>37</v>
       </c>
@@ -14176,7 +14170,7 @@
       <c r="GB60" s="40"/>
       <c r="GC60" s="45"/>
     </row>
-    <row r="61" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A61" s="33"/>
       <c r="B61" s="9" t="s">
         <v>61</v>
@@ -14366,7 +14360,7 @@
       <c r="GB61" s="11"/>
       <c r="GC61" s="24"/>
     </row>
-    <row r="62" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="32"/>
       <c r="B62" s="48"/>
       <c r="C62" s="11"/>
@@ -14553,7 +14547,7 @@
       <c r="GB62" s="11"/>
       <c r="GC62" s="24"/>
     </row>
-    <row r="63" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A63" s="33"/>
       <c r="B63" s="9" t="s">
         <v>40</v>
@@ -14743,7 +14737,7 @@
       <c r="GB63" s="11"/>
       <c r="GC63" s="24"/>
     </row>
-    <row r="64" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
       <c r="B64" s="48"/>
       <c r="C64" s="11"/>
@@ -14930,7 +14924,7 @@
       <c r="GB64" s="11"/>
       <c r="GC64" s="24"/>
     </row>
-    <row r="65" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A65" s="33"/>
       <c r="B65" s="9" t="s">
         <v>62</v>
@@ -15120,7 +15114,7 @@
       <c r="GB65" s="11"/>
       <c r="GC65" s="24"/>
     </row>
-    <row r="66" spans="1:185" s="2" customFormat="1" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
       <c r="B66" s="48"/>
       <c r="C66" s="11"/>
@@ -15307,7 +15301,7 @@
       <c r="GB66" s="11"/>
       <c r="GC66" s="24"/>
     </row>
-    <row r="67" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A67" s="33"/>
       <c r="B67" s="9" t="s">
         <v>80</v>
@@ -15497,10 +15491,14 @@
       <c r="GB67" s="11"/>
       <c r="GC67" s="24"/>
     </row>
-    <row r="68" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A68" s="33"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="7"/>
+      <c r="B68" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C68" s="47">
+        <v>42720</v>
+      </c>
       <c r="D68" s="7"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -15596,7 +15594,7 @@
       <c r="CS68" s="23"/>
       <c r="CT68" s="11"/>
       <c r="CU68" s="11"/>
-      <c r="CV68" s="67"/>
+      <c r="CV68" s="90"/>
       <c r="CW68" s="11"/>
       <c r="CX68" s="11"/>
       <c r="CY68" s="22"/>
@@ -15683,12 +15681,14 @@
       <c r="GB68" s="11"/>
       <c r="GC68" s="24"/>
     </row>
-    <row r="69" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A69" s="33"/>
       <c r="B69" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="C69" s="47">
+        <v>42776</v>
+      </c>
       <c r="D69" s="7"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
@@ -15784,24 +15784,24 @@
       <c r="CS69" s="23"/>
       <c r="CT69" s="11"/>
       <c r="CU69" s="11"/>
-      <c r="CV69" s="67"/>
+      <c r="CV69" s="90"/>
       <c r="CW69" s="11"/>
       <c r="CX69" s="11"/>
       <c r="CY69" s="22"/>
-      <c r="CZ69" s="51"/>
-      <c r="DA69" s="51"/>
-      <c r="DB69" s="51"/>
-      <c r="DC69" s="51"/>
-      <c r="DD69" s="51"/>
-      <c r="DE69" s="51"/>
-      <c r="DF69" s="51"/>
-      <c r="DG69" s="63"/>
-      <c r="DH69" s="51"/>
-      <c r="DI69" s="51"/>
-      <c r="DJ69" s="51"/>
-      <c r="DK69" s="51"/>
-      <c r="DL69" s="51"/>
-      <c r="DM69" s="64"/>
+      <c r="CZ69" s="11"/>
+      <c r="DA69" s="11"/>
+      <c r="DB69" s="11"/>
+      <c r="DC69" s="11"/>
+      <c r="DD69" s="11"/>
+      <c r="DE69" s="11"/>
+      <c r="DF69" s="11"/>
+      <c r="DG69" s="23"/>
+      <c r="DH69" s="11"/>
+      <c r="DI69" s="11"/>
+      <c r="DJ69" s="11"/>
+      <c r="DK69" s="11"/>
+      <c r="DL69" s="11"/>
+      <c r="DM69" s="22"/>
       <c r="DN69" s="11"/>
       <c r="DO69" s="11"/>
       <c r="DP69" s="11"/>
@@ -15871,7 +15871,7 @@
       <c r="GB69" s="11"/>
       <c r="GC69" s="24"/>
     </row>
-    <row r="70" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A70" s="33"/>
       <c r="B70" s="9"/>
       <c r="C70" s="7"/>
@@ -16057,10 +16057,10 @@
       <c r="GB70" s="11"/>
       <c r="GC70" s="24"/>
     </row>
-    <row r="71" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A71" s="33"/>
       <c r="B71" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -16162,20 +16162,20 @@
       <c r="CW71" s="11"/>
       <c r="CX71" s="11"/>
       <c r="CY71" s="22"/>
-      <c r="CZ71" s="11"/>
-      <c r="DA71" s="11"/>
-      <c r="DB71" s="11"/>
-      <c r="DC71" s="11"/>
-      <c r="DD71" s="11"/>
-      <c r="DE71" s="11"/>
-      <c r="DF71" s="11"/>
-      <c r="DG71" s="23"/>
-      <c r="DH71" s="11"/>
-      <c r="DI71" s="11"/>
-      <c r="DJ71" s="11"/>
-      <c r="DK71" s="11"/>
-      <c r="DL71" s="11"/>
-      <c r="DM71" s="22"/>
+      <c r="CZ71" s="51"/>
+      <c r="DA71" s="51"/>
+      <c r="DB71" s="51"/>
+      <c r="DC71" s="51"/>
+      <c r="DD71" s="51"/>
+      <c r="DE71" s="51"/>
+      <c r="DF71" s="51"/>
+      <c r="DG71" s="63"/>
+      <c r="DH71" s="51"/>
+      <c r="DI71" s="51"/>
+      <c r="DJ71" s="51"/>
+      <c r="DK71" s="51"/>
+      <c r="DL71" s="51"/>
+      <c r="DM71" s="64"/>
       <c r="DN71" s="11"/>
       <c r="DO71" s="11"/>
       <c r="DP71" s="11"/>
@@ -16245,7 +16245,7 @@
       <c r="GB71" s="11"/>
       <c r="GC71" s="24"/>
     </row>
-    <row r="72" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="33"/>
       <c r="B72" s="9"/>
       <c r="C72" s="7"/>
@@ -16431,10 +16431,10 @@
       <c r="GB72" s="11"/>
       <c r="GC72" s="24"/>
     </row>
-    <row r="73" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A73" s="33"/>
       <c r="B73" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -16529,13 +16529,13 @@
       <c r="CP73" s="11"/>
       <c r="CQ73" s="11"/>
       <c r="CR73" s="11"/>
-      <c r="CS73" s="23"/>
-      <c r="CT73" s="11"/>
-      <c r="CU73" s="11"/>
-      <c r="CV73" s="67"/>
-      <c r="CW73" s="11"/>
-      <c r="CX73" s="11"/>
-      <c r="CY73" s="22"/>
+      <c r="CS73" s="63"/>
+      <c r="CT73" s="51"/>
+      <c r="CU73" s="51"/>
+      <c r="CV73" s="90"/>
+      <c r="CW73" s="51"/>
+      <c r="CX73" s="51"/>
+      <c r="CY73" s="64"/>
       <c r="CZ73" s="51"/>
       <c r="DA73" s="51"/>
       <c r="DB73" s="51"/>
@@ -16550,36 +16550,36 @@
       <c r="DK73" s="51"/>
       <c r="DL73" s="51"/>
       <c r="DM73" s="64"/>
-      <c r="DN73" s="11"/>
-      <c r="DO73" s="11"/>
-      <c r="DP73" s="11"/>
-      <c r="DQ73" s="11"/>
-      <c r="DR73" s="11"/>
-      <c r="DS73" s="11"/>
-      <c r="DT73" s="11"/>
-      <c r="DU73" s="23"/>
-      <c r="DV73" s="11"/>
-      <c r="DW73" s="11"/>
-      <c r="DX73" s="11"/>
-      <c r="DY73" s="11"/>
-      <c r="DZ73" s="11"/>
-      <c r="EA73" s="22"/>
-      <c r="EB73" s="11"/>
-      <c r="EC73" s="11"/>
-      <c r="ED73" s="73"/>
-      <c r="EE73" s="11"/>
-      <c r="EF73" s="11"/>
-      <c r="EG73" s="11"/>
-      <c r="EH73" s="11"/>
-      <c r="EI73" s="23"/>
-      <c r="EJ73" s="11"/>
-      <c r="EK73" s="11"/>
-      <c r="EL73" s="11"/>
-      <c r="EM73" s="11"/>
-      <c r="EN73" s="11"/>
-      <c r="EO73" s="22"/>
-      <c r="EP73" s="11"/>
-      <c r="EQ73" s="11"/>
+      <c r="DN73" s="51"/>
+      <c r="DO73" s="51"/>
+      <c r="DP73" s="51"/>
+      <c r="DQ73" s="51"/>
+      <c r="DR73" s="51"/>
+      <c r="DS73" s="51"/>
+      <c r="DT73" s="51"/>
+      <c r="DU73" s="63"/>
+      <c r="DV73" s="51"/>
+      <c r="DW73" s="51"/>
+      <c r="DX73" s="51"/>
+      <c r="DY73" s="51"/>
+      <c r="DZ73" s="51"/>
+      <c r="EA73" s="64"/>
+      <c r="EB73" s="51"/>
+      <c r="EC73" s="51"/>
+      <c r="ED73" s="147"/>
+      <c r="EE73" s="51"/>
+      <c r="EF73" s="51"/>
+      <c r="EG73" s="51"/>
+      <c r="EH73" s="51"/>
+      <c r="EI73" s="63"/>
+      <c r="EJ73" s="51"/>
+      <c r="EK73" s="51"/>
+      <c r="EL73" s="51"/>
+      <c r="EM73" s="51"/>
+      <c r="EN73" s="51"/>
+      <c r="EO73" s="64"/>
+      <c r="EP73" s="51"/>
+      <c r="EQ73" s="51"/>
       <c r="ER73" s="11"/>
       <c r="ES73" s="11"/>
       <c r="ET73" s="11"/>
@@ -16619,7 +16619,7 @@
       <c r="GB73" s="11"/>
       <c r="GC73" s="24"/>
     </row>
-    <row r="74" spans="1:185" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="33"/>
       <c r="B74" s="9"/>
       <c r="C74" s="7"/>
@@ -16805,10 +16805,10 @@
       <c r="GB74" s="11"/>
       <c r="GC74" s="24"/>
     </row>
-    <row r="75" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A75" s="33"/>
       <c r="B75" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -16910,20 +16910,20 @@
       <c r="CW75" s="11"/>
       <c r="CX75" s="11"/>
       <c r="CY75" s="22"/>
-      <c r="CZ75" s="11"/>
-      <c r="DA75" s="11"/>
-      <c r="DB75" s="11"/>
-      <c r="DC75" s="11"/>
-      <c r="DD75" s="11"/>
-      <c r="DE75" s="11"/>
-      <c r="DF75" s="11"/>
-      <c r="DG75" s="23"/>
-      <c r="DH75" s="11"/>
-      <c r="DI75" s="11"/>
-      <c r="DJ75" s="11"/>
-      <c r="DK75" s="11"/>
-      <c r="DL75" s="11"/>
-      <c r="DM75" s="22"/>
+      <c r="CZ75" s="51"/>
+      <c r="DA75" s="51"/>
+      <c r="DB75" s="51"/>
+      <c r="DC75" s="51"/>
+      <c r="DD75" s="51"/>
+      <c r="DE75" s="51"/>
+      <c r="DF75" s="51"/>
+      <c r="DG75" s="63"/>
+      <c r="DH75" s="51"/>
+      <c r="DI75" s="51"/>
+      <c r="DJ75" s="51"/>
+      <c r="DK75" s="51"/>
+      <c r="DL75" s="51"/>
+      <c r="DM75" s="64"/>
       <c r="DN75" s="11"/>
       <c r="DO75" s="11"/>
       <c r="DP75" s="11"/>
@@ -16993,7 +16993,7 @@
       <c r="GB75" s="11"/>
       <c r="GC75" s="24"/>
     </row>
-    <row r="76" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="33"/>
       <c r="B76" s="9"/>
       <c r="C76" s="7"/>
@@ -17179,9 +17179,11 @@
       <c r="GB76" s="11"/>
       <c r="GC76" s="24"/>
     </row>
-    <row r="77" spans="1:185" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A77" s="33"/>
-      <c r="B77" s="9"/>
+      <c r="B77" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="F77" s="11"/>
@@ -17365,206 +17367,578 @@
       <c r="GB77" s="11"/>
       <c r="GC77" s="24"/>
     </row>
-    <row r="78" spans="1:185" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="95" t="s">
+    <row r="78" spans="1:185" x14ac:dyDescent="0.2">
+      <c r="A78" s="33"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="23"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="22"/>
+      <c r="T78" s="11"/>
+      <c r="U78" s="11"/>
+      <c r="V78" s="11"/>
+      <c r="W78" s="11"/>
+      <c r="X78" s="11"/>
+      <c r="Y78" s="11"/>
+      <c r="Z78" s="11"/>
+      <c r="AA78" s="23"/>
+      <c r="AB78" s="11"/>
+      <c r="AC78" s="11"/>
+      <c r="AD78" s="11"/>
+      <c r="AE78" s="11"/>
+      <c r="AF78" s="11"/>
+      <c r="AG78" s="22"/>
+      <c r="AH78" s="11"/>
+      <c r="AI78" s="11"/>
+      <c r="AJ78" s="11"/>
+      <c r="AK78" s="11"/>
+      <c r="AL78" s="11"/>
+      <c r="AM78" s="11"/>
+      <c r="AN78" s="11"/>
+      <c r="AO78" s="76"/>
+      <c r="AP78" s="11"/>
+      <c r="AQ78" s="11"/>
+      <c r="AR78" s="11"/>
+      <c r="AS78" s="11"/>
+      <c r="AT78" s="11"/>
+      <c r="AU78" s="22"/>
+      <c r="AV78" s="11"/>
+      <c r="AW78" s="11"/>
+      <c r="AX78" s="11"/>
+      <c r="AY78" s="11"/>
+      <c r="AZ78" s="11"/>
+      <c r="BA78" s="11"/>
+      <c r="BB78" s="11"/>
+      <c r="BC78" s="23"/>
+      <c r="BD78" s="11"/>
+      <c r="BE78" s="11"/>
+      <c r="BF78" s="11"/>
+      <c r="BG78" s="11"/>
+      <c r="BH78" s="11"/>
+      <c r="BI78" s="22"/>
+      <c r="BJ78" s="11"/>
+      <c r="BK78" s="11"/>
+      <c r="BL78" s="11"/>
+      <c r="BM78" s="11"/>
+      <c r="BN78" s="11"/>
+      <c r="BO78" s="11"/>
+      <c r="BP78" s="11"/>
+      <c r="BQ78" s="23"/>
+      <c r="BR78" s="11"/>
+      <c r="BS78" s="11"/>
+      <c r="BT78" s="11"/>
+      <c r="BU78" s="11"/>
+      <c r="BV78" s="11"/>
+      <c r="BW78" s="22"/>
+      <c r="BX78" s="11"/>
+      <c r="BY78" s="11"/>
+      <c r="BZ78" s="73"/>
+      <c r="CA78" s="11"/>
+      <c r="CB78" s="11"/>
+      <c r="CC78" s="11"/>
+      <c r="CD78" s="11"/>
+      <c r="CE78" s="23"/>
+      <c r="CF78" s="11"/>
+      <c r="CG78" s="11"/>
+      <c r="CH78" s="11"/>
+      <c r="CI78" s="11"/>
+      <c r="CJ78" s="11"/>
+      <c r="CK78" s="22"/>
+      <c r="CL78" s="11"/>
+      <c r="CM78" s="11"/>
+      <c r="CN78" s="11"/>
+      <c r="CO78" s="11"/>
+      <c r="CP78" s="11"/>
+      <c r="CQ78" s="11"/>
+      <c r="CR78" s="11"/>
+      <c r="CS78" s="23"/>
+      <c r="CT78" s="11"/>
+      <c r="CU78" s="11"/>
+      <c r="CV78" s="67"/>
+      <c r="CW78" s="11"/>
+      <c r="CX78" s="11"/>
+      <c r="CY78" s="22"/>
+      <c r="CZ78" s="11"/>
+      <c r="DA78" s="11"/>
+      <c r="DB78" s="11"/>
+      <c r="DC78" s="11"/>
+      <c r="DD78" s="11"/>
+      <c r="DE78" s="11"/>
+      <c r="DF78" s="11"/>
+      <c r="DG78" s="23"/>
+      <c r="DH78" s="11"/>
+      <c r="DI78" s="11"/>
+      <c r="DJ78" s="11"/>
+      <c r="DK78" s="11"/>
+      <c r="DL78" s="11"/>
+      <c r="DM78" s="22"/>
+      <c r="DN78" s="11"/>
+      <c r="DO78" s="11"/>
+      <c r="DP78" s="11"/>
+      <c r="DQ78" s="11"/>
+      <c r="DR78" s="11"/>
+      <c r="DS78" s="11"/>
+      <c r="DT78" s="11"/>
+      <c r="DU78" s="23"/>
+      <c r="DV78" s="11"/>
+      <c r="DW78" s="11"/>
+      <c r="DX78" s="11"/>
+      <c r="DY78" s="11"/>
+      <c r="DZ78" s="11"/>
+      <c r="EA78" s="22"/>
+      <c r="EB78" s="11"/>
+      <c r="EC78" s="11"/>
+      <c r="ED78" s="73"/>
+      <c r="EE78" s="11"/>
+      <c r="EF78" s="11"/>
+      <c r="EG78" s="11"/>
+      <c r="EH78" s="11"/>
+      <c r="EI78" s="23"/>
+      <c r="EJ78" s="11"/>
+      <c r="EK78" s="11"/>
+      <c r="EL78" s="11"/>
+      <c r="EM78" s="11"/>
+      <c r="EN78" s="11"/>
+      <c r="EO78" s="22"/>
+      <c r="EP78" s="11"/>
+      <c r="EQ78" s="11"/>
+      <c r="ER78" s="11"/>
+      <c r="ES78" s="11"/>
+      <c r="ET78" s="11"/>
+      <c r="EU78" s="11"/>
+      <c r="EV78" s="11"/>
+      <c r="EW78" s="23"/>
+      <c r="EX78" s="11"/>
+      <c r="EY78" s="11"/>
+      <c r="EZ78" s="11"/>
+      <c r="FA78" s="11"/>
+      <c r="FB78" s="11"/>
+      <c r="FC78" s="22"/>
+      <c r="FD78" s="11"/>
+      <c r="FE78" s="11"/>
+      <c r="FF78" s="11"/>
+      <c r="FG78" s="11"/>
+      <c r="FH78" s="11"/>
+      <c r="FI78" s="11"/>
+      <c r="FJ78" s="11"/>
+      <c r="FK78" s="23"/>
+      <c r="FL78" s="11"/>
+      <c r="FM78" s="67"/>
+      <c r="FN78" s="11"/>
+      <c r="FO78" s="11"/>
+      <c r="FP78" s="11"/>
+      <c r="FQ78" s="22"/>
+      <c r="FR78" s="11"/>
+      <c r="FS78" s="11"/>
+      <c r="FT78" s="11"/>
+      <c r="FU78" s="11"/>
+      <c r="FV78" s="11"/>
+      <c r="FW78" s="11"/>
+      <c r="FX78" s="11"/>
+      <c r="FY78" s="23"/>
+      <c r="FZ78" s="11"/>
+      <c r="GA78" s="11"/>
+      <c r="GB78" s="11"/>
+      <c r="GC78" s="24"/>
+    </row>
+    <row r="79" spans="1:185" x14ac:dyDescent="0.2">
+      <c r="A79" s="33"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="11"/>
+      <c r="L79" s="11"/>
+      <c r="M79" s="23"/>
+      <c r="N79" s="11"/>
+      <c r="O79" s="11"/>
+      <c r="P79" s="11"/>
+      <c r="Q79" s="11"/>
+      <c r="R79" s="11"/>
+      <c r="S79" s="22"/>
+      <c r="T79" s="11"/>
+      <c r="U79" s="11"/>
+      <c r="V79" s="11"/>
+      <c r="W79" s="11"/>
+      <c r="X79" s="11"/>
+      <c r="Y79" s="11"/>
+      <c r="Z79" s="11"/>
+      <c r="AA79" s="23"/>
+      <c r="AB79" s="11"/>
+      <c r="AC79" s="11"/>
+      <c r="AD79" s="11"/>
+      <c r="AE79" s="11"/>
+      <c r="AF79" s="11"/>
+      <c r="AG79" s="22"/>
+      <c r="AH79" s="11"/>
+      <c r="AI79" s="11"/>
+      <c r="AJ79" s="11"/>
+      <c r="AK79" s="11"/>
+      <c r="AL79" s="11"/>
+      <c r="AM79" s="11"/>
+      <c r="AN79" s="11"/>
+      <c r="AO79" s="76"/>
+      <c r="AP79" s="11"/>
+      <c r="AQ79" s="11"/>
+      <c r="AR79" s="11"/>
+      <c r="AS79" s="11"/>
+      <c r="AT79" s="11"/>
+      <c r="AU79" s="22"/>
+      <c r="AV79" s="11"/>
+      <c r="AW79" s="11"/>
+      <c r="AX79" s="11"/>
+      <c r="AY79" s="11"/>
+      <c r="AZ79" s="11"/>
+      <c r="BA79" s="11"/>
+      <c r="BB79" s="11"/>
+      <c r="BC79" s="23"/>
+      <c r="BD79" s="11"/>
+      <c r="BE79" s="11"/>
+      <c r="BF79" s="11"/>
+      <c r="BG79" s="11"/>
+      <c r="BH79" s="11"/>
+      <c r="BI79" s="22"/>
+      <c r="BJ79" s="11"/>
+      <c r="BK79" s="11"/>
+      <c r="BL79" s="11"/>
+      <c r="BM79" s="11"/>
+      <c r="BN79" s="11"/>
+      <c r="BO79" s="11"/>
+      <c r="BP79" s="11"/>
+      <c r="BQ79" s="23"/>
+      <c r="BR79" s="11"/>
+      <c r="BS79" s="11"/>
+      <c r="BT79" s="11"/>
+      <c r="BU79" s="11"/>
+      <c r="BV79" s="11"/>
+      <c r="BW79" s="22"/>
+      <c r="BX79" s="11"/>
+      <c r="BY79" s="11"/>
+      <c r="BZ79" s="73"/>
+      <c r="CA79" s="11"/>
+      <c r="CB79" s="11"/>
+      <c r="CC79" s="11"/>
+      <c r="CD79" s="11"/>
+      <c r="CE79" s="23"/>
+      <c r="CF79" s="11"/>
+      <c r="CG79" s="11"/>
+      <c r="CH79" s="11"/>
+      <c r="CI79" s="11"/>
+      <c r="CJ79" s="11"/>
+      <c r="CK79" s="22"/>
+      <c r="CL79" s="11"/>
+      <c r="CM79" s="11"/>
+      <c r="CN79" s="11"/>
+      <c r="CO79" s="11"/>
+      <c r="CP79" s="11"/>
+      <c r="CQ79" s="11"/>
+      <c r="CR79" s="11"/>
+      <c r="CS79" s="23"/>
+      <c r="CT79" s="11"/>
+      <c r="CU79" s="11"/>
+      <c r="CV79" s="67"/>
+      <c r="CW79" s="11"/>
+      <c r="CX79" s="11"/>
+      <c r="CY79" s="22"/>
+      <c r="CZ79" s="11"/>
+      <c r="DA79" s="11"/>
+      <c r="DB79" s="11"/>
+      <c r="DC79" s="11"/>
+      <c r="DD79" s="11"/>
+      <c r="DE79" s="11"/>
+      <c r="DF79" s="11"/>
+      <c r="DG79" s="23"/>
+      <c r="DH79" s="11"/>
+      <c r="DI79" s="11"/>
+      <c r="DJ79" s="11"/>
+      <c r="DK79" s="11"/>
+      <c r="DL79" s="11"/>
+      <c r="DM79" s="22"/>
+      <c r="DN79" s="11"/>
+      <c r="DO79" s="11"/>
+      <c r="DP79" s="11"/>
+      <c r="DQ79" s="11"/>
+      <c r="DR79" s="11"/>
+      <c r="DS79" s="11"/>
+      <c r="DT79" s="11"/>
+      <c r="DU79" s="23"/>
+      <c r="DV79" s="11"/>
+      <c r="DW79" s="11"/>
+      <c r="DX79" s="11"/>
+      <c r="DY79" s="11"/>
+      <c r="DZ79" s="11"/>
+      <c r="EA79" s="22"/>
+      <c r="EB79" s="11"/>
+      <c r="EC79" s="11"/>
+      <c r="ED79" s="73"/>
+      <c r="EE79" s="11"/>
+      <c r="EF79" s="11"/>
+      <c r="EG79" s="11"/>
+      <c r="EH79" s="11"/>
+      <c r="EI79" s="23"/>
+      <c r="EJ79" s="11"/>
+      <c r="EK79" s="11"/>
+      <c r="EL79" s="11"/>
+      <c r="EM79" s="11"/>
+      <c r="EN79" s="11"/>
+      <c r="EO79" s="22"/>
+      <c r="EP79" s="11"/>
+      <c r="EQ79" s="11"/>
+      <c r="ER79" s="11"/>
+      <c r="ES79" s="11"/>
+      <c r="ET79" s="11"/>
+      <c r="EU79" s="11"/>
+      <c r="EV79" s="11"/>
+      <c r="EW79" s="23"/>
+      <c r="EX79" s="11"/>
+      <c r="EY79" s="11"/>
+      <c r="EZ79" s="11"/>
+      <c r="FA79" s="11"/>
+      <c r="FB79" s="11"/>
+      <c r="FC79" s="22"/>
+      <c r="FD79" s="11"/>
+      <c r="FE79" s="11"/>
+      <c r="FF79" s="11"/>
+      <c r="FG79" s="11"/>
+      <c r="FH79" s="11"/>
+      <c r="FI79" s="11"/>
+      <c r="FJ79" s="11"/>
+      <c r="FK79" s="23"/>
+      <c r="FL79" s="11"/>
+      <c r="FM79" s="67"/>
+      <c r="FN79" s="11"/>
+      <c r="FO79" s="11"/>
+      <c r="FP79" s="11"/>
+      <c r="FQ79" s="22"/>
+      <c r="FR79" s="11"/>
+      <c r="FS79" s="11"/>
+      <c r="FT79" s="11"/>
+      <c r="FU79" s="11"/>
+      <c r="FV79" s="11"/>
+      <c r="FW79" s="11"/>
+      <c r="FX79" s="11"/>
+      <c r="FY79" s="23"/>
+      <c r="FZ79" s="11"/>
+      <c r="GA79" s="11"/>
+      <c r="GB79" s="11"/>
+      <c r="GC79" s="24"/>
+    </row>
+    <row r="80" spans="1:185" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="96"/>
-      <c r="C78" s="96"/>
-      <c r="D78" s="96"/>
-      <c r="E78" s="97"/>
-      <c r="F78" s="98" t="s">
+      <c r="B80" s="113"/>
+      <c r="C80" s="113"/>
+      <c r="D80" s="113"/>
+      <c r="E80" s="114"/>
+      <c r="F80" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="G78" s="92"/>
-      <c r="H78" s="92"/>
-      <c r="I78" s="92"/>
-      <c r="J78" s="92"/>
-      <c r="K78" s="92"/>
-      <c r="L78" s="92"/>
-      <c r="M78" s="92"/>
-      <c r="N78" s="92"/>
-      <c r="O78" s="92"/>
-      <c r="P78" s="92"/>
-      <c r="Q78" s="92"/>
-      <c r="R78" s="92"/>
-      <c r="S78" s="92"/>
-      <c r="T78" s="92"/>
-      <c r="U78" s="92"/>
-      <c r="V78" s="92"/>
-      <c r="W78" s="92"/>
-      <c r="X78" s="92"/>
-      <c r="Y78" s="92"/>
-      <c r="Z78" s="92"/>
-      <c r="AA78" s="92"/>
-      <c r="AB78" s="92"/>
-      <c r="AC78" s="92"/>
-      <c r="AD78" s="92"/>
-      <c r="AE78" s="92"/>
-      <c r="AF78" s="92"/>
-      <c r="AG78" s="92"/>
-      <c r="AH78" s="92"/>
-      <c r="AI78" s="92"/>
-      <c r="AJ78" s="92"/>
-      <c r="AK78" s="92"/>
-      <c r="AL78" s="92"/>
-      <c r="AM78" s="92"/>
-      <c r="AN78" s="99"/>
-      <c r="AO78" s="100" t="s">
+      <c r="G80" s="109"/>
+      <c r="H80" s="109"/>
+      <c r="I80" s="109"/>
+      <c r="J80" s="109"/>
+      <c r="K80" s="109"/>
+      <c r="L80" s="109"/>
+      <c r="M80" s="109"/>
+      <c r="N80" s="109"/>
+      <c r="O80" s="109"/>
+      <c r="P80" s="109"/>
+      <c r="Q80" s="109"/>
+      <c r="R80" s="109"/>
+      <c r="S80" s="109"/>
+      <c r="T80" s="109"/>
+      <c r="U80" s="109"/>
+      <c r="V80" s="109"/>
+      <c r="W80" s="109"/>
+      <c r="X80" s="109"/>
+      <c r="Y80" s="109"/>
+      <c r="Z80" s="109"/>
+      <c r="AA80" s="109"/>
+      <c r="AB80" s="109"/>
+      <c r="AC80" s="109"/>
+      <c r="AD80" s="109"/>
+      <c r="AE80" s="109"/>
+      <c r="AF80" s="109"/>
+      <c r="AG80" s="109"/>
+      <c r="AH80" s="109"/>
+      <c r="AI80" s="109"/>
+      <c r="AJ80" s="109"/>
+      <c r="AK80" s="109"/>
+      <c r="AL80" s="109"/>
+      <c r="AM80" s="109"/>
+      <c r="AN80" s="116"/>
+      <c r="AO80" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="AP78" s="92"/>
-      <c r="AQ78" s="92"/>
-      <c r="AR78" s="92"/>
-      <c r="AS78" s="92"/>
-      <c r="AT78" s="92"/>
-      <c r="AU78" s="92"/>
-      <c r="AV78" s="92"/>
-      <c r="AW78" s="92"/>
-      <c r="AX78" s="92"/>
-      <c r="AY78" s="92"/>
-      <c r="AZ78" s="92"/>
-      <c r="BA78" s="92"/>
-      <c r="BB78" s="92"/>
-      <c r="BC78" s="92"/>
-      <c r="BD78" s="92"/>
-      <c r="BE78" s="92"/>
-      <c r="BF78" s="92"/>
-      <c r="BG78" s="92"/>
-      <c r="BH78" s="92"/>
-      <c r="BI78" s="92"/>
-      <c r="BJ78" s="92"/>
-      <c r="BK78" s="92"/>
-      <c r="BL78" s="92"/>
-      <c r="BM78" s="92"/>
-      <c r="BN78" s="92"/>
-      <c r="BO78" s="92"/>
-      <c r="BP78" s="92"/>
-      <c r="BQ78" s="92"/>
-      <c r="BR78" s="92"/>
-      <c r="BS78" s="92"/>
-      <c r="BT78" s="92"/>
-      <c r="BU78" s="92"/>
-      <c r="BV78" s="92"/>
-      <c r="BW78" s="92"/>
-      <c r="BX78" s="92"/>
-      <c r="BY78" s="92"/>
-      <c r="BZ78" s="93"/>
-      <c r="CA78" s="91" t="s">
+      <c r="AP80" s="109"/>
+      <c r="AQ80" s="109"/>
+      <c r="AR80" s="109"/>
+      <c r="AS80" s="109"/>
+      <c r="AT80" s="109"/>
+      <c r="AU80" s="109"/>
+      <c r="AV80" s="109"/>
+      <c r="AW80" s="109"/>
+      <c r="AX80" s="109"/>
+      <c r="AY80" s="109"/>
+      <c r="AZ80" s="109"/>
+      <c r="BA80" s="109"/>
+      <c r="BB80" s="109"/>
+      <c r="BC80" s="109"/>
+      <c r="BD80" s="109"/>
+      <c r="BE80" s="109"/>
+      <c r="BF80" s="109"/>
+      <c r="BG80" s="109"/>
+      <c r="BH80" s="109"/>
+      <c r="BI80" s="109"/>
+      <c r="BJ80" s="109"/>
+      <c r="BK80" s="109"/>
+      <c r="BL80" s="109"/>
+      <c r="BM80" s="109"/>
+      <c r="BN80" s="109"/>
+      <c r="BO80" s="109"/>
+      <c r="BP80" s="109"/>
+      <c r="BQ80" s="109"/>
+      <c r="BR80" s="109"/>
+      <c r="BS80" s="109"/>
+      <c r="BT80" s="109"/>
+      <c r="BU80" s="109"/>
+      <c r="BV80" s="109"/>
+      <c r="BW80" s="109"/>
+      <c r="BX80" s="109"/>
+      <c r="BY80" s="109"/>
+      <c r="BZ80" s="110"/>
+      <c r="CA80" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="CB78" s="92"/>
-      <c r="CC78" s="92"/>
-      <c r="CD78" s="92"/>
-      <c r="CE78" s="92"/>
-      <c r="CF78" s="92"/>
-      <c r="CG78" s="92"/>
-      <c r="CH78" s="92"/>
-      <c r="CI78" s="92"/>
-      <c r="CJ78" s="92"/>
-      <c r="CK78" s="92"/>
-      <c r="CL78" s="92"/>
-      <c r="CM78" s="92"/>
-      <c r="CN78" s="92"/>
-      <c r="CO78" s="92"/>
-      <c r="CP78" s="92"/>
-      <c r="CQ78" s="92"/>
-      <c r="CR78" s="92"/>
-      <c r="CS78" s="92"/>
-      <c r="CT78" s="92"/>
-      <c r="CU78" s="93"/>
-      <c r="CV78" s="91" t="s">
+      <c r="CB80" s="109"/>
+      <c r="CC80" s="109"/>
+      <c r="CD80" s="109"/>
+      <c r="CE80" s="109"/>
+      <c r="CF80" s="109"/>
+      <c r="CG80" s="109"/>
+      <c r="CH80" s="109"/>
+      <c r="CI80" s="109"/>
+      <c r="CJ80" s="109"/>
+      <c r="CK80" s="109"/>
+      <c r="CL80" s="109"/>
+      <c r="CM80" s="109"/>
+      <c r="CN80" s="109"/>
+      <c r="CO80" s="109"/>
+      <c r="CP80" s="109"/>
+      <c r="CQ80" s="109"/>
+      <c r="CR80" s="109"/>
+      <c r="CS80" s="109"/>
+      <c r="CT80" s="109"/>
+      <c r="CU80" s="110"/>
+      <c r="CV80" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="CW78" s="92"/>
-      <c r="CX78" s="92"/>
-      <c r="CY78" s="92"/>
-      <c r="CZ78" s="92"/>
-      <c r="DA78" s="92"/>
-      <c r="DB78" s="92"/>
-      <c r="DC78" s="92"/>
-      <c r="DD78" s="92"/>
-      <c r="DE78" s="92"/>
-      <c r="DF78" s="92"/>
-      <c r="DG78" s="92"/>
-      <c r="DH78" s="92"/>
-      <c r="DI78" s="92"/>
-      <c r="DJ78" s="92"/>
-      <c r="DK78" s="92"/>
-      <c r="DL78" s="92"/>
-      <c r="DM78" s="92"/>
-      <c r="DN78" s="92"/>
-      <c r="DO78" s="92"/>
-      <c r="DP78" s="92"/>
-      <c r="DQ78" s="92"/>
-      <c r="DR78" s="92"/>
-      <c r="DS78" s="92"/>
-      <c r="DT78" s="92"/>
-      <c r="DU78" s="92"/>
-      <c r="DV78" s="92"/>
-      <c r="DW78" s="92"/>
-      <c r="DX78" s="92"/>
-      <c r="DY78" s="92"/>
-      <c r="DZ78" s="92"/>
-      <c r="EA78" s="92"/>
-      <c r="EB78" s="92"/>
-      <c r="EC78" s="92"/>
-      <c r="ED78" s="93"/>
-      <c r="EE78" s="91" t="s">
+      <c r="CW80" s="109"/>
+      <c r="CX80" s="109"/>
+      <c r="CY80" s="109"/>
+      <c r="CZ80" s="109"/>
+      <c r="DA80" s="109"/>
+      <c r="DB80" s="109"/>
+      <c r="DC80" s="109"/>
+      <c r="DD80" s="109"/>
+      <c r="DE80" s="109"/>
+      <c r="DF80" s="109"/>
+      <c r="DG80" s="109"/>
+      <c r="DH80" s="109"/>
+      <c r="DI80" s="109"/>
+      <c r="DJ80" s="109"/>
+      <c r="DK80" s="109"/>
+      <c r="DL80" s="109"/>
+      <c r="DM80" s="109"/>
+      <c r="DN80" s="109"/>
+      <c r="DO80" s="109"/>
+      <c r="DP80" s="109"/>
+      <c r="DQ80" s="109"/>
+      <c r="DR80" s="109"/>
+      <c r="DS80" s="109"/>
+      <c r="DT80" s="109"/>
+      <c r="DU80" s="109"/>
+      <c r="DV80" s="109"/>
+      <c r="DW80" s="109"/>
+      <c r="DX80" s="109"/>
+      <c r="DY80" s="109"/>
+      <c r="DZ80" s="109"/>
+      <c r="EA80" s="109"/>
+      <c r="EB80" s="109"/>
+      <c r="EC80" s="109"/>
+      <c r="ED80" s="110"/>
+      <c r="EE80" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="EF78" s="92"/>
-      <c r="EG78" s="92"/>
-      <c r="EH78" s="92"/>
-      <c r="EI78" s="92"/>
-      <c r="EJ78" s="92"/>
-      <c r="EK78" s="92"/>
-      <c r="EL78" s="92"/>
-      <c r="EM78" s="92"/>
-      <c r="EN78" s="92"/>
-      <c r="EO78" s="92"/>
-      <c r="EP78" s="92"/>
-      <c r="EQ78" s="92"/>
-      <c r="ER78" s="92"/>
-      <c r="ES78" s="92"/>
-      <c r="ET78" s="92"/>
-      <c r="EU78" s="92"/>
-      <c r="EV78" s="92"/>
-      <c r="EW78" s="92"/>
-      <c r="EX78" s="92"/>
-      <c r="EY78" s="92"/>
-      <c r="EZ78" s="92"/>
-      <c r="FA78" s="92"/>
-      <c r="FB78" s="92"/>
-      <c r="FC78" s="92"/>
-      <c r="FD78" s="92"/>
-      <c r="FE78" s="92"/>
-      <c r="FF78" s="92"/>
-      <c r="FG78" s="92"/>
-      <c r="FH78" s="92"/>
-      <c r="FI78" s="92"/>
-      <c r="FJ78" s="92"/>
-      <c r="FK78" s="92"/>
-      <c r="FL78" s="93"/>
-      <c r="FM78" s="91" t="s">
+      <c r="EF80" s="109"/>
+      <c r="EG80" s="109"/>
+      <c r="EH80" s="109"/>
+      <c r="EI80" s="109"/>
+      <c r="EJ80" s="109"/>
+      <c r="EK80" s="109"/>
+      <c r="EL80" s="109"/>
+      <c r="EM80" s="109"/>
+      <c r="EN80" s="109"/>
+      <c r="EO80" s="109"/>
+      <c r="EP80" s="109"/>
+      <c r="EQ80" s="109"/>
+      <c r="ER80" s="109"/>
+      <c r="ES80" s="109"/>
+      <c r="ET80" s="109"/>
+      <c r="EU80" s="109"/>
+      <c r="EV80" s="109"/>
+      <c r="EW80" s="109"/>
+      <c r="EX80" s="109"/>
+      <c r="EY80" s="109"/>
+      <c r="EZ80" s="109"/>
+      <c r="FA80" s="109"/>
+      <c r="FB80" s="109"/>
+      <c r="FC80" s="109"/>
+      <c r="FD80" s="109"/>
+      <c r="FE80" s="109"/>
+      <c r="FF80" s="109"/>
+      <c r="FG80" s="109"/>
+      <c r="FH80" s="109"/>
+      <c r="FI80" s="109"/>
+      <c r="FJ80" s="109"/>
+      <c r="FK80" s="109"/>
+      <c r="FL80" s="110"/>
+      <c r="FM80" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="FN78" s="92"/>
-      <c r="FO78" s="92"/>
-      <c r="FP78" s="92"/>
-      <c r="FQ78" s="92"/>
-      <c r="FR78" s="92"/>
-      <c r="FS78" s="92"/>
-      <c r="FT78" s="92"/>
-      <c r="FU78" s="92"/>
-      <c r="FV78" s="92"/>
-      <c r="FW78" s="92"/>
-      <c r="FX78" s="92"/>
-      <c r="FY78" s="92"/>
-      <c r="FZ78" s="92"/>
-      <c r="GA78" s="92"/>
-      <c r="GB78" s="92"/>
-      <c r="GC78" s="94"/>
+      <c r="FN80" s="109"/>
+      <c r="FO80" s="109"/>
+      <c r="FP80" s="109"/>
+      <c r="FQ80" s="109"/>
+      <c r="FR80" s="109"/>
+      <c r="FS80" s="109"/>
+      <c r="FT80" s="109"/>
+      <c r="FU80" s="109"/>
+      <c r="FV80" s="109"/>
+      <c r="FW80" s="109"/>
+      <c r="FX80" s="109"/>
+      <c r="FY80" s="109"/>
+      <c r="FZ80" s="109"/>
+      <c r="GA80" s="109"/>
+      <c r="GB80" s="109"/>
+      <c r="GC80" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -17616,13 +17990,13 @@
     <mergeCell ref="CA4:CU4"/>
     <mergeCell ref="CV4:ED4"/>
     <mergeCell ref="EE4:FL4"/>
-    <mergeCell ref="EE78:FL78"/>
-    <mergeCell ref="FM78:GC78"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="F78:AN78"/>
-    <mergeCell ref="AO78:BZ78"/>
-    <mergeCell ref="CA78:CU78"/>
-    <mergeCell ref="CV78:ED78"/>
+    <mergeCell ref="EE80:FL80"/>
+    <mergeCell ref="FM80:GC80"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="F80:AN80"/>
+    <mergeCell ref="AO80:BZ80"/>
+    <mergeCell ref="CA80:CU80"/>
+    <mergeCell ref="CV80:ED80"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -17634,176 +18008,176 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="128.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="128.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="131" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+    <row r="1" spans="1:5" s="92" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="93" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="138" t="s">
+      <c r="C3" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="133" t="s">
+      <c r="D3" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="134" t="s">
+      <c r="E3" s="95" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="139" t="s">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A4" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="141">
+      <c r="C4" s="102">
         <v>42666</v>
       </c>
-      <c r="D4" s="135" t="s">
+      <c r="D4" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="144" t="s">
+      <c r="E4" s="105" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
+    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A5" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="97" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="142">
+      <c r="C5" s="103">
         <v>42704</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="145" t="s">
+      <c r="E5" s="106" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="139" t="s">
+    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A6" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="142">
+      <c r="C6" s="103">
         <v>42704</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="145" t="s">
+      <c r="E6" s="106" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="139" t="s">
+    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A7" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="146" t="s">
+      <c r="B7" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="142">
+      <c r="C7" s="103">
         <v>42725</v>
       </c>
-      <c r="D7" s="135" t="s">
+      <c r="D7" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="106" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="139" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="142">
+      <c r="C8" s="103">
         <v>42760</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="144" t="s">
+      <c r="E8" s="105" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="139" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="142">
+      <c r="C9" s="103">
         <v>42795</v>
       </c>
-      <c r="D9" s="135" t="s">
+      <c r="D9" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="144" t="s">
+      <c r="E9" s="105" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="139" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="143" t="s">
+      <c r="B10" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="142">
+      <c r="C10" s="103">
         <v>42810</v>
       </c>
-      <c r="D10" s="135" t="s">
+      <c r="D10" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="144" t="s">
+      <c r="E10" s="105" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="139" t="s">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="142">
+      <c r="C11" s="103">
         <v>42810</v>
       </c>
-      <c r="D11" s="135" t="s">
+      <c r="D11" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="144" t="s">
+      <c r="E11" s="105" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
requirements / planning / minutes
</commit_message>
<xml_diff>
--- a/doc/planning/Projektplanung_Spektrometer.xlsx
+++ b/doc/planning/Projektplanung_Spektrometer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="39940" windowHeight="24080"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="abc">[1]Stammdaten!$B$2:$B$9</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$GC$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$GC$81</definedName>
     <definedName name="Teammitglieder">#REF!</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -1767,6 +1767,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1795,96 +1885,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2352,13 +2352,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:GC80"/>
+  <dimension ref="A1:GC82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="EZ39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="8" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="FX51" sqref="FX51:GB51"/>
+      <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2374,13 +2374,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:185" s="12" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="135"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="117"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -2563,11 +2563,11 @@
       <c r="GC1" s="6"/>
     </row>
     <row r="2" spans="1:185" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="142"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144"/>
+      <c r="A2" s="127"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="129"/>
       <c r="F2" s="50"/>
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
@@ -2949,851 +2949,851 @@
       <c r="GC3" s="18"/>
     </row>
     <row r="4" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="137"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="118" t="s">
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
-      <c r="M4" s="119"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="119"/>
-      <c r="P4" s="119"/>
-      <c r="Q4" s="119"/>
-      <c r="R4" s="119"/>
-      <c r="S4" s="119"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="119"/>
-      <c r="V4" s="119"/>
-      <c r="W4" s="119"/>
-      <c r="X4" s="119"/>
-      <c r="Y4" s="119"/>
-      <c r="Z4" s="119"/>
-      <c r="AA4" s="119"/>
-      <c r="AB4" s="119"/>
-      <c r="AC4" s="119"/>
-      <c r="AD4" s="119"/>
-      <c r="AE4" s="119"/>
-      <c r="AF4" s="119"/>
-      <c r="AG4" s="119"/>
-      <c r="AH4" s="119"/>
-      <c r="AI4" s="119"/>
-      <c r="AJ4" s="119"/>
-      <c r="AK4" s="119"/>
-      <c r="AL4" s="119"/>
-      <c r="AM4" s="119"/>
-      <c r="AN4" s="119"/>
-      <c r="AO4" s="119" t="s">
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="136"/>
+      <c r="P4" s="136"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="136"/>
+      <c r="S4" s="136"/>
+      <c r="T4" s="136"/>
+      <c r="U4" s="136"/>
+      <c r="V4" s="136"/>
+      <c r="W4" s="136"/>
+      <c r="X4" s="136"/>
+      <c r="Y4" s="136"/>
+      <c r="Z4" s="136"/>
+      <c r="AA4" s="136"/>
+      <c r="AB4" s="136"/>
+      <c r="AC4" s="136"/>
+      <c r="AD4" s="136"/>
+      <c r="AE4" s="136"/>
+      <c r="AF4" s="136"/>
+      <c r="AG4" s="136"/>
+      <c r="AH4" s="136"/>
+      <c r="AI4" s="136"/>
+      <c r="AJ4" s="136"/>
+      <c r="AK4" s="136"/>
+      <c r="AL4" s="136"/>
+      <c r="AM4" s="136"/>
+      <c r="AN4" s="136"/>
+      <c r="AO4" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="AP4" s="119"/>
-      <c r="AQ4" s="119"/>
-      <c r="AR4" s="119"/>
-      <c r="AS4" s="119"/>
-      <c r="AT4" s="119"/>
-      <c r="AU4" s="119"/>
-      <c r="AV4" s="119"/>
-      <c r="AW4" s="119"/>
-      <c r="AX4" s="119"/>
-      <c r="AY4" s="119"/>
-      <c r="AZ4" s="119"/>
-      <c r="BA4" s="119"/>
-      <c r="BB4" s="119"/>
-      <c r="BC4" s="119"/>
-      <c r="BD4" s="119"/>
-      <c r="BE4" s="119"/>
-      <c r="BF4" s="119"/>
-      <c r="BG4" s="119"/>
-      <c r="BH4" s="119"/>
-      <c r="BI4" s="119"/>
-      <c r="BJ4" s="119"/>
-      <c r="BK4" s="119"/>
-      <c r="BL4" s="119"/>
-      <c r="BM4" s="119"/>
-      <c r="BN4" s="119"/>
-      <c r="BO4" s="119"/>
-      <c r="BP4" s="119"/>
-      <c r="BQ4" s="119"/>
-      <c r="BR4" s="119"/>
-      <c r="BS4" s="119"/>
-      <c r="BT4" s="119"/>
-      <c r="BU4" s="119"/>
-      <c r="BV4" s="119"/>
-      <c r="BW4" s="119"/>
-      <c r="BX4" s="119"/>
-      <c r="BY4" s="119"/>
-      <c r="BZ4" s="119"/>
-      <c r="CA4" s="119" t="s">
+      <c r="AP4" s="136"/>
+      <c r="AQ4" s="136"/>
+      <c r="AR4" s="136"/>
+      <c r="AS4" s="136"/>
+      <c r="AT4" s="136"/>
+      <c r="AU4" s="136"/>
+      <c r="AV4" s="136"/>
+      <c r="AW4" s="136"/>
+      <c r="AX4" s="136"/>
+      <c r="AY4" s="136"/>
+      <c r="AZ4" s="136"/>
+      <c r="BA4" s="136"/>
+      <c r="BB4" s="136"/>
+      <c r="BC4" s="136"/>
+      <c r="BD4" s="136"/>
+      <c r="BE4" s="136"/>
+      <c r="BF4" s="136"/>
+      <c r="BG4" s="136"/>
+      <c r="BH4" s="136"/>
+      <c r="BI4" s="136"/>
+      <c r="BJ4" s="136"/>
+      <c r="BK4" s="136"/>
+      <c r="BL4" s="136"/>
+      <c r="BM4" s="136"/>
+      <c r="BN4" s="136"/>
+      <c r="BO4" s="136"/>
+      <c r="BP4" s="136"/>
+      <c r="BQ4" s="136"/>
+      <c r="BR4" s="136"/>
+      <c r="BS4" s="136"/>
+      <c r="BT4" s="136"/>
+      <c r="BU4" s="136"/>
+      <c r="BV4" s="136"/>
+      <c r="BW4" s="136"/>
+      <c r="BX4" s="136"/>
+      <c r="BY4" s="136"/>
+      <c r="BZ4" s="136"/>
+      <c r="CA4" s="136" t="s">
         <v>93</v>
       </c>
-      <c r="CB4" s="119"/>
-      <c r="CC4" s="119"/>
-      <c r="CD4" s="119"/>
-      <c r="CE4" s="119"/>
-      <c r="CF4" s="119"/>
-      <c r="CG4" s="119"/>
-      <c r="CH4" s="119"/>
-      <c r="CI4" s="119"/>
-      <c r="CJ4" s="119"/>
-      <c r="CK4" s="119"/>
-      <c r="CL4" s="119"/>
-      <c r="CM4" s="119"/>
-      <c r="CN4" s="119"/>
-      <c r="CO4" s="119"/>
-      <c r="CP4" s="119"/>
-      <c r="CQ4" s="119"/>
-      <c r="CR4" s="119"/>
-      <c r="CS4" s="119"/>
-      <c r="CT4" s="119"/>
-      <c r="CU4" s="119"/>
-      <c r="CV4" s="119" t="s">
+      <c r="CB4" s="136"/>
+      <c r="CC4" s="136"/>
+      <c r="CD4" s="136"/>
+      <c r="CE4" s="136"/>
+      <c r="CF4" s="136"/>
+      <c r="CG4" s="136"/>
+      <c r="CH4" s="136"/>
+      <c r="CI4" s="136"/>
+      <c r="CJ4" s="136"/>
+      <c r="CK4" s="136"/>
+      <c r="CL4" s="136"/>
+      <c r="CM4" s="136"/>
+      <c r="CN4" s="136"/>
+      <c r="CO4" s="136"/>
+      <c r="CP4" s="136"/>
+      <c r="CQ4" s="136"/>
+      <c r="CR4" s="136"/>
+      <c r="CS4" s="136"/>
+      <c r="CT4" s="136"/>
+      <c r="CU4" s="136"/>
+      <c r="CV4" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="CW4" s="119"/>
-      <c r="CX4" s="119"/>
-      <c r="CY4" s="119"/>
-      <c r="CZ4" s="119"/>
-      <c r="DA4" s="119"/>
-      <c r="DB4" s="119"/>
-      <c r="DC4" s="119"/>
-      <c r="DD4" s="119"/>
-      <c r="DE4" s="119"/>
-      <c r="DF4" s="119"/>
-      <c r="DG4" s="119"/>
-      <c r="DH4" s="119"/>
-      <c r="DI4" s="119"/>
-      <c r="DJ4" s="119"/>
-      <c r="DK4" s="119"/>
-      <c r="DL4" s="119"/>
-      <c r="DM4" s="119"/>
-      <c r="DN4" s="119"/>
-      <c r="DO4" s="119"/>
-      <c r="DP4" s="119"/>
-      <c r="DQ4" s="119"/>
-      <c r="DR4" s="119"/>
-      <c r="DS4" s="119"/>
-      <c r="DT4" s="119"/>
-      <c r="DU4" s="119"/>
-      <c r="DV4" s="119"/>
-      <c r="DW4" s="119"/>
-      <c r="DX4" s="119"/>
-      <c r="DY4" s="119"/>
-      <c r="DZ4" s="119"/>
-      <c r="EA4" s="119"/>
-      <c r="EB4" s="119"/>
-      <c r="EC4" s="119"/>
-      <c r="ED4" s="119"/>
-      <c r="EE4" s="119" t="s">
+      <c r="CW4" s="136"/>
+      <c r="CX4" s="136"/>
+      <c r="CY4" s="136"/>
+      <c r="CZ4" s="136"/>
+      <c r="DA4" s="136"/>
+      <c r="DB4" s="136"/>
+      <c r="DC4" s="136"/>
+      <c r="DD4" s="136"/>
+      <c r="DE4" s="136"/>
+      <c r="DF4" s="136"/>
+      <c r="DG4" s="136"/>
+      <c r="DH4" s="136"/>
+      <c r="DI4" s="136"/>
+      <c r="DJ4" s="136"/>
+      <c r="DK4" s="136"/>
+      <c r="DL4" s="136"/>
+      <c r="DM4" s="136"/>
+      <c r="DN4" s="136"/>
+      <c r="DO4" s="136"/>
+      <c r="DP4" s="136"/>
+      <c r="DQ4" s="136"/>
+      <c r="DR4" s="136"/>
+      <c r="DS4" s="136"/>
+      <c r="DT4" s="136"/>
+      <c r="DU4" s="136"/>
+      <c r="DV4" s="136"/>
+      <c r="DW4" s="136"/>
+      <c r="DX4" s="136"/>
+      <c r="DY4" s="136"/>
+      <c r="DZ4" s="136"/>
+      <c r="EA4" s="136"/>
+      <c r="EB4" s="136"/>
+      <c r="EC4" s="136"/>
+      <c r="ED4" s="136"/>
+      <c r="EE4" s="136" t="s">
         <v>95</v>
       </c>
-      <c r="EF4" s="119"/>
-      <c r="EG4" s="119"/>
-      <c r="EH4" s="119"/>
-      <c r="EI4" s="119"/>
-      <c r="EJ4" s="119"/>
-      <c r="EK4" s="119"/>
-      <c r="EL4" s="119"/>
-      <c r="EM4" s="119"/>
-      <c r="EN4" s="119"/>
-      <c r="EO4" s="119"/>
-      <c r="EP4" s="119"/>
-      <c r="EQ4" s="119"/>
-      <c r="ER4" s="119"/>
-      <c r="ES4" s="119"/>
-      <c r="ET4" s="119"/>
-      <c r="EU4" s="119"/>
-      <c r="EV4" s="119"/>
-      <c r="EW4" s="119"/>
-      <c r="EX4" s="119"/>
-      <c r="EY4" s="119"/>
-      <c r="EZ4" s="119"/>
-      <c r="FA4" s="119"/>
-      <c r="FB4" s="119"/>
-      <c r="FC4" s="119"/>
-      <c r="FD4" s="119"/>
-      <c r="FE4" s="119"/>
-      <c r="FF4" s="119"/>
-      <c r="FG4" s="119"/>
-      <c r="FH4" s="119"/>
-      <c r="FI4" s="119"/>
-      <c r="FJ4" s="119"/>
-      <c r="FK4" s="119"/>
-      <c r="FL4" s="119"/>
-      <c r="FM4" s="119" t="s">
+      <c r="EF4" s="136"/>
+      <c r="EG4" s="136"/>
+      <c r="EH4" s="136"/>
+      <c r="EI4" s="136"/>
+      <c r="EJ4" s="136"/>
+      <c r="EK4" s="136"/>
+      <c r="EL4" s="136"/>
+      <c r="EM4" s="136"/>
+      <c r="EN4" s="136"/>
+      <c r="EO4" s="136"/>
+      <c r="EP4" s="136"/>
+      <c r="EQ4" s="136"/>
+      <c r="ER4" s="136"/>
+      <c r="ES4" s="136"/>
+      <c r="ET4" s="136"/>
+      <c r="EU4" s="136"/>
+      <c r="EV4" s="136"/>
+      <c r="EW4" s="136"/>
+      <c r="EX4" s="136"/>
+      <c r="EY4" s="136"/>
+      <c r="EZ4" s="136"/>
+      <c r="FA4" s="136"/>
+      <c r="FB4" s="136"/>
+      <c r="FC4" s="136"/>
+      <c r="FD4" s="136"/>
+      <c r="FE4" s="136"/>
+      <c r="FF4" s="136"/>
+      <c r="FG4" s="136"/>
+      <c r="FH4" s="136"/>
+      <c r="FI4" s="136"/>
+      <c r="FJ4" s="136"/>
+      <c r="FK4" s="136"/>
+      <c r="FL4" s="136"/>
+      <c r="FM4" s="136" t="s">
         <v>92</v>
       </c>
-      <c r="FN4" s="119"/>
-      <c r="FO4" s="119"/>
-      <c r="FP4" s="119"/>
-      <c r="FQ4" s="119"/>
-      <c r="FR4" s="119"/>
-      <c r="FS4" s="119"/>
-      <c r="FT4" s="119"/>
-      <c r="FU4" s="119"/>
-      <c r="FV4" s="119"/>
-      <c r="FW4" s="119"/>
-      <c r="FX4" s="119"/>
-      <c r="FY4" s="119"/>
-      <c r="FZ4" s="119"/>
-      <c r="GA4" s="119"/>
-      <c r="GB4" s="119"/>
-      <c r="GC4" s="120"/>
+      <c r="FN4" s="136"/>
+      <c r="FO4" s="136"/>
+      <c r="FP4" s="136"/>
+      <c r="FQ4" s="136"/>
+      <c r="FR4" s="136"/>
+      <c r="FS4" s="136"/>
+      <c r="FT4" s="136"/>
+      <c r="FU4" s="136"/>
+      <c r="FV4" s="136"/>
+      <c r="FW4" s="136"/>
+      <c r="FX4" s="136"/>
+      <c r="FY4" s="136"/>
+      <c r="FZ4" s="136"/>
+      <c r="GA4" s="136"/>
+      <c r="GB4" s="136"/>
+      <c r="GC4" s="137"/>
     </row>
     <row r="5" spans="1:185" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="123">
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="133">
         <v>2016</v>
       </c>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
-      <c r="Y5" s="124"/>
-      <c r="Z5" s="124"/>
-      <c r="AA5" s="124"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="124"/>
-      <c r="AE5" s="124"/>
-      <c r="AF5" s="124"/>
-      <c r="AG5" s="124"/>
-      <c r="AH5" s="124"/>
-      <c r="AI5" s="124"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="124"/>
-      <c r="AL5" s="124"/>
-      <c r="AM5" s="124"/>
-      <c r="AN5" s="124"/>
-      <c r="AO5" s="124"/>
-      <c r="AP5" s="124"/>
-      <c r="AQ5" s="124"/>
-      <c r="AR5" s="124"/>
-      <c r="AS5" s="124"/>
-      <c r="AT5" s="124"/>
-      <c r="AU5" s="124"/>
-      <c r="AV5" s="124"/>
-      <c r="AW5" s="124"/>
-      <c r="AX5" s="124"/>
-      <c r="AY5" s="124"/>
-      <c r="AZ5" s="124"/>
-      <c r="BA5" s="124"/>
-      <c r="BB5" s="124"/>
-      <c r="BC5" s="124"/>
-      <c r="BD5" s="124"/>
-      <c r="BE5" s="124"/>
-      <c r="BF5" s="124"/>
-      <c r="BG5" s="124"/>
-      <c r="BH5" s="124"/>
-      <c r="BI5" s="124"/>
-      <c r="BJ5" s="124"/>
-      <c r="BK5" s="124"/>
-      <c r="BL5" s="124"/>
-      <c r="BM5" s="124"/>
-      <c r="BN5" s="124"/>
-      <c r="BO5" s="124"/>
-      <c r="BP5" s="124"/>
-      <c r="BQ5" s="124"/>
-      <c r="BR5" s="124"/>
-      <c r="BS5" s="124"/>
-      <c r="BT5" s="124"/>
-      <c r="BU5" s="124"/>
-      <c r="BV5" s="124"/>
-      <c r="BW5" s="124"/>
-      <c r="BX5" s="124"/>
-      <c r="BY5" s="124"/>
-      <c r="BZ5" s="124"/>
-      <c r="CA5" s="124"/>
-      <c r="CB5" s="124"/>
-      <c r="CC5" s="124"/>
-      <c r="CD5" s="124"/>
-      <c r="CE5" s="124"/>
-      <c r="CF5" s="124"/>
-      <c r="CG5" s="124"/>
-      <c r="CH5" s="124"/>
-      <c r="CI5" s="124"/>
-      <c r="CJ5" s="124"/>
-      <c r="CK5" s="124"/>
-      <c r="CL5" s="124"/>
-      <c r="CM5" s="124"/>
-      <c r="CN5" s="124"/>
-      <c r="CO5" s="124"/>
-      <c r="CP5" s="124"/>
-      <c r="CQ5" s="124"/>
-      <c r="CR5" s="124"/>
-      <c r="CS5" s="124"/>
-      <c r="CT5" s="124"/>
-      <c r="CU5" s="124"/>
-      <c r="CV5" s="124"/>
-      <c r="CW5" s="124"/>
-      <c r="CX5" s="124"/>
-      <c r="CY5" s="124"/>
-      <c r="CZ5" s="124"/>
-      <c r="DA5" s="124"/>
-      <c r="DB5" s="124"/>
-      <c r="DC5" s="124"/>
-      <c r="DD5" s="124"/>
-      <c r="DE5" s="124"/>
-      <c r="DF5" s="124">
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="111"/>
+      <c r="X5" s="111"/>
+      <c r="Y5" s="111"/>
+      <c r="Z5" s="111"/>
+      <c r="AA5" s="111"/>
+      <c r="AB5" s="111"/>
+      <c r="AC5" s="111"/>
+      <c r="AD5" s="111"/>
+      <c r="AE5" s="111"/>
+      <c r="AF5" s="111"/>
+      <c r="AG5" s="111"/>
+      <c r="AH5" s="111"/>
+      <c r="AI5" s="111"/>
+      <c r="AJ5" s="111"/>
+      <c r="AK5" s="111"/>
+      <c r="AL5" s="111"/>
+      <c r="AM5" s="111"/>
+      <c r="AN5" s="111"/>
+      <c r="AO5" s="111"/>
+      <c r="AP5" s="111"/>
+      <c r="AQ5" s="111"/>
+      <c r="AR5" s="111"/>
+      <c r="AS5" s="111"/>
+      <c r="AT5" s="111"/>
+      <c r="AU5" s="111"/>
+      <c r="AV5" s="111"/>
+      <c r="AW5" s="111"/>
+      <c r="AX5" s="111"/>
+      <c r="AY5" s="111"/>
+      <c r="AZ5" s="111"/>
+      <c r="BA5" s="111"/>
+      <c r="BB5" s="111"/>
+      <c r="BC5" s="111"/>
+      <c r="BD5" s="111"/>
+      <c r="BE5" s="111"/>
+      <c r="BF5" s="111"/>
+      <c r="BG5" s="111"/>
+      <c r="BH5" s="111"/>
+      <c r="BI5" s="111"/>
+      <c r="BJ5" s="111"/>
+      <c r="BK5" s="111"/>
+      <c r="BL5" s="111"/>
+      <c r="BM5" s="111"/>
+      <c r="BN5" s="111"/>
+      <c r="BO5" s="111"/>
+      <c r="BP5" s="111"/>
+      <c r="BQ5" s="111"/>
+      <c r="BR5" s="111"/>
+      <c r="BS5" s="111"/>
+      <c r="BT5" s="111"/>
+      <c r="BU5" s="111"/>
+      <c r="BV5" s="111"/>
+      <c r="BW5" s="111"/>
+      <c r="BX5" s="111"/>
+      <c r="BY5" s="111"/>
+      <c r="BZ5" s="111"/>
+      <c r="CA5" s="111"/>
+      <c r="CB5" s="111"/>
+      <c r="CC5" s="111"/>
+      <c r="CD5" s="111"/>
+      <c r="CE5" s="111"/>
+      <c r="CF5" s="111"/>
+      <c r="CG5" s="111"/>
+      <c r="CH5" s="111"/>
+      <c r="CI5" s="111"/>
+      <c r="CJ5" s="111"/>
+      <c r="CK5" s="111"/>
+      <c r="CL5" s="111"/>
+      <c r="CM5" s="111"/>
+      <c r="CN5" s="111"/>
+      <c r="CO5" s="111"/>
+      <c r="CP5" s="111"/>
+      <c r="CQ5" s="111"/>
+      <c r="CR5" s="111"/>
+      <c r="CS5" s="111"/>
+      <c r="CT5" s="111"/>
+      <c r="CU5" s="111"/>
+      <c r="CV5" s="111"/>
+      <c r="CW5" s="111"/>
+      <c r="CX5" s="111"/>
+      <c r="CY5" s="111"/>
+      <c r="CZ5" s="111"/>
+      <c r="DA5" s="111"/>
+      <c r="DB5" s="111"/>
+      <c r="DC5" s="111"/>
+      <c r="DD5" s="111"/>
+      <c r="DE5" s="111"/>
+      <c r="DF5" s="111">
         <v>2017</v>
       </c>
-      <c r="DG5" s="124"/>
-      <c r="DH5" s="124"/>
-      <c r="DI5" s="124"/>
-      <c r="DJ5" s="124"/>
-      <c r="DK5" s="124"/>
-      <c r="DL5" s="124"/>
-      <c r="DM5" s="124"/>
-      <c r="DN5" s="124"/>
-      <c r="DO5" s="124"/>
-      <c r="DP5" s="124"/>
-      <c r="DQ5" s="124"/>
-      <c r="DR5" s="124"/>
-      <c r="DS5" s="124"/>
-      <c r="DT5" s="124"/>
-      <c r="DU5" s="124"/>
-      <c r="DV5" s="124"/>
-      <c r="DW5" s="124"/>
-      <c r="DX5" s="124"/>
-      <c r="DY5" s="124"/>
-      <c r="DZ5" s="124"/>
-      <c r="EA5" s="124"/>
-      <c r="EB5" s="124"/>
-      <c r="EC5" s="124"/>
-      <c r="ED5" s="124"/>
-      <c r="EE5" s="124"/>
-      <c r="EF5" s="124"/>
-      <c r="EG5" s="124"/>
-      <c r="EH5" s="124"/>
-      <c r="EI5" s="124"/>
-      <c r="EJ5" s="124"/>
-      <c r="EK5" s="124"/>
-      <c r="EL5" s="124"/>
-      <c r="EM5" s="124"/>
-      <c r="EN5" s="124"/>
-      <c r="EO5" s="124"/>
-      <c r="EP5" s="124"/>
-      <c r="EQ5" s="124"/>
-      <c r="ER5" s="124"/>
-      <c r="ES5" s="124"/>
-      <c r="ET5" s="124"/>
-      <c r="EU5" s="124"/>
-      <c r="EV5" s="124"/>
-      <c r="EW5" s="124"/>
-      <c r="EX5" s="124"/>
-      <c r="EY5" s="124"/>
-      <c r="EZ5" s="124"/>
-      <c r="FA5" s="124"/>
-      <c r="FB5" s="124"/>
-      <c r="FC5" s="124"/>
-      <c r="FD5" s="124"/>
-      <c r="FE5" s="124"/>
-      <c r="FF5" s="124"/>
-      <c r="FG5" s="124"/>
-      <c r="FH5" s="124"/>
-      <c r="FI5" s="124"/>
-      <c r="FJ5" s="124"/>
-      <c r="FK5" s="124"/>
-      <c r="FL5" s="124"/>
-      <c r="FM5" s="124"/>
-      <c r="FN5" s="124"/>
-      <c r="FO5" s="124"/>
-      <c r="FP5" s="124"/>
-      <c r="FQ5" s="124"/>
-      <c r="FR5" s="124"/>
-      <c r="FS5" s="124"/>
-      <c r="FT5" s="124"/>
-      <c r="FU5" s="124"/>
-      <c r="FV5" s="124"/>
-      <c r="FW5" s="124"/>
-      <c r="FX5" s="124"/>
-      <c r="FY5" s="124"/>
-      <c r="FZ5" s="124"/>
-      <c r="GA5" s="124"/>
-      <c r="GB5" s="124"/>
-      <c r="GC5" s="146"/>
+      <c r="DG5" s="111"/>
+      <c r="DH5" s="111"/>
+      <c r="DI5" s="111"/>
+      <c r="DJ5" s="111"/>
+      <c r="DK5" s="111"/>
+      <c r="DL5" s="111"/>
+      <c r="DM5" s="111"/>
+      <c r="DN5" s="111"/>
+      <c r="DO5" s="111"/>
+      <c r="DP5" s="111"/>
+      <c r="DQ5" s="111"/>
+      <c r="DR5" s="111"/>
+      <c r="DS5" s="111"/>
+      <c r="DT5" s="111"/>
+      <c r="DU5" s="111"/>
+      <c r="DV5" s="111"/>
+      <c r="DW5" s="111"/>
+      <c r="DX5" s="111"/>
+      <c r="DY5" s="111"/>
+      <c r="DZ5" s="111"/>
+      <c r="EA5" s="111"/>
+      <c r="EB5" s="111"/>
+      <c r="EC5" s="111"/>
+      <c r="ED5" s="111"/>
+      <c r="EE5" s="111"/>
+      <c r="EF5" s="111"/>
+      <c r="EG5" s="111"/>
+      <c r="EH5" s="111"/>
+      <c r="EI5" s="111"/>
+      <c r="EJ5" s="111"/>
+      <c r="EK5" s="111"/>
+      <c r="EL5" s="111"/>
+      <c r="EM5" s="111"/>
+      <c r="EN5" s="111"/>
+      <c r="EO5" s="111"/>
+      <c r="EP5" s="111"/>
+      <c r="EQ5" s="111"/>
+      <c r="ER5" s="111"/>
+      <c r="ES5" s="111"/>
+      <c r="ET5" s="111"/>
+      <c r="EU5" s="111"/>
+      <c r="EV5" s="111"/>
+      <c r="EW5" s="111"/>
+      <c r="EX5" s="111"/>
+      <c r="EY5" s="111"/>
+      <c r="EZ5" s="111"/>
+      <c r="FA5" s="111"/>
+      <c r="FB5" s="111"/>
+      <c r="FC5" s="111"/>
+      <c r="FD5" s="111"/>
+      <c r="FE5" s="111"/>
+      <c r="FF5" s="111"/>
+      <c r="FG5" s="111"/>
+      <c r="FH5" s="111"/>
+      <c r="FI5" s="111"/>
+      <c r="FJ5" s="111"/>
+      <c r="FK5" s="111"/>
+      <c r="FL5" s="111"/>
+      <c r="FM5" s="111"/>
+      <c r="FN5" s="111"/>
+      <c r="FO5" s="111"/>
+      <c r="FP5" s="111"/>
+      <c r="FQ5" s="111"/>
+      <c r="FR5" s="111"/>
+      <c r="FS5" s="111"/>
+      <c r="FT5" s="111"/>
+      <c r="FU5" s="111"/>
+      <c r="FV5" s="111"/>
+      <c r="FW5" s="111"/>
+      <c r="FX5" s="111"/>
+      <c r="FY5" s="111"/>
+      <c r="FZ5" s="111"/>
+      <c r="GA5" s="111"/>
+      <c r="GB5" s="111"/>
+      <c r="GC5" s="112"/>
     </row>
     <row r="6" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="140"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="121" t="s">
+      <c r="B6" s="125"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="122"/>
-      <c r="L6" s="122"/>
-      <c r="M6" s="122"/>
-      <c r="N6" s="122"/>
-      <c r="O6" s="122"/>
-      <c r="P6" s="122"/>
-      <c r="Q6" s="122"/>
-      <c r="R6" s="122" t="s">
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="122"/>
-      <c r="T6" s="122"/>
-      <c r="U6" s="122"/>
-      <c r="V6" s="122"/>
-      <c r="W6" s="122"/>
-      <c r="X6" s="122"/>
-      <c r="Y6" s="122"/>
-      <c r="Z6" s="122"/>
-      <c r="AA6" s="122"/>
-      <c r="AB6" s="122"/>
-      <c r="AC6" s="122"/>
-      <c r="AD6" s="122"/>
-      <c r="AE6" s="122"/>
-      <c r="AF6" s="122"/>
-      <c r="AG6" s="122"/>
-      <c r="AH6" s="122"/>
-      <c r="AI6" s="122"/>
-      <c r="AJ6" s="122"/>
-      <c r="AK6" s="122"/>
-      <c r="AL6" s="122"/>
-      <c r="AM6" s="122"/>
-      <c r="AN6" s="122"/>
-      <c r="AO6" s="122"/>
-      <c r="AP6" s="122"/>
-      <c r="AQ6" s="122"/>
-      <c r="AR6" s="122"/>
-      <c r="AS6" s="122"/>
-      <c r="AT6" s="122"/>
-      <c r="AU6" s="122"/>
-      <c r="AV6" s="122"/>
-      <c r="AW6" s="122" t="s">
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="109"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="109"/>
+      <c r="AB6" s="109"/>
+      <c r="AC6" s="109"/>
+      <c r="AD6" s="109"/>
+      <c r="AE6" s="109"/>
+      <c r="AF6" s="109"/>
+      <c r="AG6" s="109"/>
+      <c r="AH6" s="109"/>
+      <c r="AI6" s="109"/>
+      <c r="AJ6" s="109"/>
+      <c r="AK6" s="109"/>
+      <c r="AL6" s="109"/>
+      <c r="AM6" s="109"/>
+      <c r="AN6" s="109"/>
+      <c r="AO6" s="109"/>
+      <c r="AP6" s="109"/>
+      <c r="AQ6" s="109"/>
+      <c r="AR6" s="109"/>
+      <c r="AS6" s="109"/>
+      <c r="AT6" s="109"/>
+      <c r="AU6" s="109"/>
+      <c r="AV6" s="109"/>
+      <c r="AW6" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="AX6" s="122"/>
-      <c r="AY6" s="122"/>
-      <c r="AZ6" s="122"/>
-      <c r="BA6" s="122"/>
-      <c r="BB6" s="122"/>
-      <c r="BC6" s="122"/>
-      <c r="BD6" s="122"/>
-      <c r="BE6" s="122"/>
-      <c r="BF6" s="122"/>
-      <c r="BG6" s="122"/>
-      <c r="BH6" s="122"/>
-      <c r="BI6" s="122"/>
-      <c r="BJ6" s="122"/>
-      <c r="BK6" s="122"/>
-      <c r="BL6" s="122"/>
-      <c r="BM6" s="122"/>
-      <c r="BN6" s="122"/>
-      <c r="BO6" s="122"/>
-      <c r="BP6" s="122"/>
-      <c r="BQ6" s="122"/>
-      <c r="BR6" s="122"/>
-      <c r="BS6" s="122"/>
-      <c r="BT6" s="122"/>
-      <c r="BU6" s="122"/>
-      <c r="BV6" s="122"/>
-      <c r="BW6" s="122"/>
-      <c r="BX6" s="122"/>
-      <c r="BY6" s="122"/>
-      <c r="BZ6" s="122"/>
-      <c r="CA6" s="122" t="s">
+      <c r="AX6" s="109"/>
+      <c r="AY6" s="109"/>
+      <c r="AZ6" s="109"/>
+      <c r="BA6" s="109"/>
+      <c r="BB6" s="109"/>
+      <c r="BC6" s="109"/>
+      <c r="BD6" s="109"/>
+      <c r="BE6" s="109"/>
+      <c r="BF6" s="109"/>
+      <c r="BG6" s="109"/>
+      <c r="BH6" s="109"/>
+      <c r="BI6" s="109"/>
+      <c r="BJ6" s="109"/>
+      <c r="BK6" s="109"/>
+      <c r="BL6" s="109"/>
+      <c r="BM6" s="109"/>
+      <c r="BN6" s="109"/>
+      <c r="BO6" s="109"/>
+      <c r="BP6" s="109"/>
+      <c r="BQ6" s="109"/>
+      <c r="BR6" s="109"/>
+      <c r="BS6" s="109"/>
+      <c r="BT6" s="109"/>
+      <c r="BU6" s="109"/>
+      <c r="BV6" s="109"/>
+      <c r="BW6" s="109"/>
+      <c r="BX6" s="109"/>
+      <c r="BY6" s="109"/>
+      <c r="BZ6" s="109"/>
+      <c r="CA6" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="CB6" s="122"/>
-      <c r="CC6" s="122"/>
-      <c r="CD6" s="122"/>
-      <c r="CE6" s="122"/>
-      <c r="CF6" s="122"/>
-      <c r="CG6" s="122"/>
-      <c r="CH6" s="122"/>
-      <c r="CI6" s="122"/>
-      <c r="CJ6" s="122"/>
-      <c r="CK6" s="122"/>
-      <c r="CL6" s="122"/>
-      <c r="CM6" s="122"/>
-      <c r="CN6" s="122"/>
-      <c r="CO6" s="122"/>
-      <c r="CP6" s="122"/>
-      <c r="CQ6" s="122"/>
-      <c r="CR6" s="122"/>
-      <c r="CS6" s="122"/>
-      <c r="CT6" s="122"/>
-      <c r="CU6" s="122"/>
-      <c r="CV6" s="122"/>
-      <c r="CW6" s="122"/>
-      <c r="CX6" s="122"/>
-      <c r="CY6" s="122"/>
-      <c r="CZ6" s="122"/>
-      <c r="DA6" s="122"/>
-      <c r="DB6" s="122"/>
-      <c r="DC6" s="122"/>
-      <c r="DD6" s="122"/>
-      <c r="DE6" s="122"/>
-      <c r="DF6" s="122" t="s">
+      <c r="CB6" s="109"/>
+      <c r="CC6" s="109"/>
+      <c r="CD6" s="109"/>
+      <c r="CE6" s="109"/>
+      <c r="CF6" s="109"/>
+      <c r="CG6" s="109"/>
+      <c r="CH6" s="109"/>
+      <c r="CI6" s="109"/>
+      <c r="CJ6" s="109"/>
+      <c r="CK6" s="109"/>
+      <c r="CL6" s="109"/>
+      <c r="CM6" s="109"/>
+      <c r="CN6" s="109"/>
+      <c r="CO6" s="109"/>
+      <c r="CP6" s="109"/>
+      <c r="CQ6" s="109"/>
+      <c r="CR6" s="109"/>
+      <c r="CS6" s="109"/>
+      <c r="CT6" s="109"/>
+      <c r="CU6" s="109"/>
+      <c r="CV6" s="109"/>
+      <c r="CW6" s="109"/>
+      <c r="CX6" s="109"/>
+      <c r="CY6" s="109"/>
+      <c r="CZ6" s="109"/>
+      <c r="DA6" s="109"/>
+      <c r="DB6" s="109"/>
+      <c r="DC6" s="109"/>
+      <c r="DD6" s="109"/>
+      <c r="DE6" s="109"/>
+      <c r="DF6" s="109" t="s">
         <v>39</v>
       </c>
-      <c r="DG6" s="122"/>
-      <c r="DH6" s="122"/>
-      <c r="DI6" s="122"/>
-      <c r="DJ6" s="122"/>
-      <c r="DK6" s="122"/>
-      <c r="DL6" s="122"/>
-      <c r="DM6" s="122"/>
-      <c r="DN6" s="122"/>
-      <c r="DO6" s="122"/>
-      <c r="DP6" s="122"/>
-      <c r="DQ6" s="122"/>
-      <c r="DR6" s="122"/>
-      <c r="DS6" s="122"/>
-      <c r="DT6" s="122"/>
-      <c r="DU6" s="122"/>
-      <c r="DV6" s="122"/>
-      <c r="DW6" s="122"/>
-      <c r="DX6" s="122"/>
-      <c r="DY6" s="122"/>
-      <c r="DZ6" s="122"/>
-      <c r="EA6" s="122"/>
-      <c r="EB6" s="122"/>
-      <c r="EC6" s="122"/>
-      <c r="ED6" s="122"/>
-      <c r="EE6" s="122"/>
-      <c r="EF6" s="122"/>
-      <c r="EG6" s="122"/>
-      <c r="EH6" s="122"/>
-      <c r="EI6" s="122"/>
-      <c r="EJ6" s="122"/>
-      <c r="EK6" s="122" t="s">
+      <c r="DG6" s="109"/>
+      <c r="DH6" s="109"/>
+      <c r="DI6" s="109"/>
+      <c r="DJ6" s="109"/>
+      <c r="DK6" s="109"/>
+      <c r="DL6" s="109"/>
+      <c r="DM6" s="109"/>
+      <c r="DN6" s="109"/>
+      <c r="DO6" s="109"/>
+      <c r="DP6" s="109"/>
+      <c r="DQ6" s="109"/>
+      <c r="DR6" s="109"/>
+      <c r="DS6" s="109"/>
+      <c r="DT6" s="109"/>
+      <c r="DU6" s="109"/>
+      <c r="DV6" s="109"/>
+      <c r="DW6" s="109"/>
+      <c r="DX6" s="109"/>
+      <c r="DY6" s="109"/>
+      <c r="DZ6" s="109"/>
+      <c r="EA6" s="109"/>
+      <c r="EB6" s="109"/>
+      <c r="EC6" s="109"/>
+      <c r="ED6" s="109"/>
+      <c r="EE6" s="109"/>
+      <c r="EF6" s="109"/>
+      <c r="EG6" s="109"/>
+      <c r="EH6" s="109"/>
+      <c r="EI6" s="109"/>
+      <c r="EJ6" s="109"/>
+      <c r="EK6" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="EL6" s="122"/>
-      <c r="EM6" s="122"/>
-      <c r="EN6" s="122"/>
-      <c r="EO6" s="122"/>
-      <c r="EP6" s="122"/>
-      <c r="EQ6" s="122"/>
-      <c r="ER6" s="122"/>
-      <c r="ES6" s="122"/>
-      <c r="ET6" s="122"/>
-      <c r="EU6" s="122"/>
-      <c r="EV6" s="122"/>
-      <c r="EW6" s="122"/>
-      <c r="EX6" s="122"/>
-      <c r="EY6" s="122"/>
-      <c r="EZ6" s="122"/>
-      <c r="FA6" s="122"/>
-      <c r="FB6" s="122"/>
-      <c r="FC6" s="122"/>
-      <c r="FD6" s="122"/>
-      <c r="FE6" s="122"/>
-      <c r="FF6" s="122"/>
-      <c r="FG6" s="122"/>
-      <c r="FH6" s="122"/>
-      <c r="FI6" s="122"/>
-      <c r="FJ6" s="122"/>
-      <c r="FK6" s="122"/>
-      <c r="FL6" s="122"/>
-      <c r="FM6" s="122" t="s">
+      <c r="EL6" s="109"/>
+      <c r="EM6" s="109"/>
+      <c r="EN6" s="109"/>
+      <c r="EO6" s="109"/>
+      <c r="EP6" s="109"/>
+      <c r="EQ6" s="109"/>
+      <c r="ER6" s="109"/>
+      <c r="ES6" s="109"/>
+      <c r="ET6" s="109"/>
+      <c r="EU6" s="109"/>
+      <c r="EV6" s="109"/>
+      <c r="EW6" s="109"/>
+      <c r="EX6" s="109"/>
+      <c r="EY6" s="109"/>
+      <c r="EZ6" s="109"/>
+      <c r="FA6" s="109"/>
+      <c r="FB6" s="109"/>
+      <c r="FC6" s="109"/>
+      <c r="FD6" s="109"/>
+      <c r="FE6" s="109"/>
+      <c r="FF6" s="109"/>
+      <c r="FG6" s="109"/>
+      <c r="FH6" s="109"/>
+      <c r="FI6" s="109"/>
+      <c r="FJ6" s="109"/>
+      <c r="FK6" s="109"/>
+      <c r="FL6" s="109"/>
+      <c r="FM6" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="FN6" s="122"/>
-      <c r="FO6" s="122"/>
-      <c r="FP6" s="122"/>
-      <c r="FQ6" s="122"/>
-      <c r="FR6" s="122"/>
-      <c r="FS6" s="122"/>
-      <c r="FT6" s="122"/>
-      <c r="FU6" s="122"/>
-      <c r="FV6" s="122"/>
-      <c r="FW6" s="122"/>
-      <c r="FX6" s="122"/>
-      <c r="FY6" s="122"/>
-      <c r="FZ6" s="122"/>
-      <c r="GA6" s="122"/>
-      <c r="GB6" s="122"/>
-      <c r="GC6" s="145"/>
+      <c r="FN6" s="109"/>
+      <c r="FO6" s="109"/>
+      <c r="FP6" s="109"/>
+      <c r="FQ6" s="109"/>
+      <c r="FR6" s="109"/>
+      <c r="FS6" s="109"/>
+      <c r="FT6" s="109"/>
+      <c r="FU6" s="109"/>
+      <c r="FV6" s="109"/>
+      <c r="FW6" s="109"/>
+      <c r="FX6" s="109"/>
+      <c r="FY6" s="109"/>
+      <c r="FZ6" s="109"/>
+      <c r="GA6" s="109"/>
+      <c r="GB6" s="109"/>
+      <c r="GC6" s="110"/>
     </row>
     <row r="7" spans="1:185" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="130" t="s">
+      <c r="A7" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="131"/>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="123" t="s">
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="133" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="129"/>
-      <c r="M7" s="128" t="s">
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="124"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-      <c r="Q7" s="124"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="129"/>
-      <c r="T7" s="128" t="s">
+      <c r="N7" s="111"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="111"/>
+      <c r="S7" s="114"/>
+      <c r="T7" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="124"/>
-      <c r="V7" s="124"/>
-      <c r="W7" s="124"/>
-      <c r="X7" s="124"/>
-      <c r="Y7" s="124"/>
-      <c r="Z7" s="129"/>
-      <c r="AA7" s="128" t="s">
+      <c r="U7" s="111"/>
+      <c r="V7" s="111"/>
+      <c r="W7" s="111"/>
+      <c r="X7" s="111"/>
+      <c r="Y7" s="111"/>
+      <c r="Z7" s="114"/>
+      <c r="AA7" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="AB7" s="124"/>
-      <c r="AC7" s="124"/>
-      <c r="AD7" s="124"/>
-      <c r="AE7" s="124"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="129"/>
-      <c r="AH7" s="128" t="s">
+      <c r="AB7" s="111"/>
+      <c r="AC7" s="111"/>
+      <c r="AD7" s="111"/>
+      <c r="AE7" s="111"/>
+      <c r="AF7" s="111"/>
+      <c r="AG7" s="114"/>
+      <c r="AH7" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="AI7" s="124"/>
-      <c r="AJ7" s="124"/>
-      <c r="AK7" s="124"/>
-      <c r="AL7" s="124"/>
-      <c r="AM7" s="124"/>
-      <c r="AN7" s="129"/>
-      <c r="AO7" s="128" t="s">
+      <c r="AI7" s="111"/>
+      <c r="AJ7" s="111"/>
+      <c r="AK7" s="111"/>
+      <c r="AL7" s="111"/>
+      <c r="AM7" s="111"/>
+      <c r="AN7" s="114"/>
+      <c r="AO7" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="AP7" s="124"/>
-      <c r="AQ7" s="124"/>
-      <c r="AR7" s="124"/>
-      <c r="AS7" s="124"/>
-      <c r="AT7" s="124"/>
-      <c r="AU7" s="129"/>
-      <c r="AV7" s="128" t="s">
+      <c r="AP7" s="111"/>
+      <c r="AQ7" s="111"/>
+      <c r="AR7" s="111"/>
+      <c r="AS7" s="111"/>
+      <c r="AT7" s="111"/>
+      <c r="AU7" s="114"/>
+      <c r="AV7" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="AW7" s="124"/>
-      <c r="AX7" s="124"/>
-      <c r="AY7" s="124"/>
-      <c r="AZ7" s="124"/>
-      <c r="BA7" s="124"/>
-      <c r="BB7" s="129"/>
-      <c r="BC7" s="128" t="s">
+      <c r="AW7" s="111"/>
+      <c r="AX7" s="111"/>
+      <c r="AY7" s="111"/>
+      <c r="AZ7" s="111"/>
+      <c r="BA7" s="111"/>
+      <c r="BB7" s="114"/>
+      <c r="BC7" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="BD7" s="124"/>
-      <c r="BE7" s="124"/>
-      <c r="BF7" s="124"/>
-      <c r="BG7" s="124"/>
-      <c r="BH7" s="124"/>
-      <c r="BI7" s="129"/>
-      <c r="BJ7" s="128" t="s">
+      <c r="BD7" s="111"/>
+      <c r="BE7" s="111"/>
+      <c r="BF7" s="111"/>
+      <c r="BG7" s="111"/>
+      <c r="BH7" s="111"/>
+      <c r="BI7" s="114"/>
+      <c r="BJ7" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="BK7" s="124"/>
-      <c r="BL7" s="124"/>
-      <c r="BM7" s="124"/>
-      <c r="BN7" s="124"/>
-      <c r="BO7" s="124"/>
-      <c r="BP7" s="129"/>
-      <c r="BQ7" s="128" t="s">
+      <c r="BK7" s="111"/>
+      <c r="BL7" s="111"/>
+      <c r="BM7" s="111"/>
+      <c r="BN7" s="111"/>
+      <c r="BO7" s="111"/>
+      <c r="BP7" s="114"/>
+      <c r="BQ7" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="BR7" s="124"/>
-      <c r="BS7" s="124"/>
-      <c r="BT7" s="124"/>
-      <c r="BU7" s="124"/>
-      <c r="BV7" s="124"/>
-      <c r="BW7" s="129"/>
-      <c r="BX7" s="128" t="s">
+      <c r="BR7" s="111"/>
+      <c r="BS7" s="111"/>
+      <c r="BT7" s="111"/>
+      <c r="BU7" s="111"/>
+      <c r="BV7" s="111"/>
+      <c r="BW7" s="114"/>
+      <c r="BX7" s="113" t="s">
         <v>15</v>
       </c>
-      <c r="BY7" s="124"/>
-      <c r="BZ7" s="124"/>
-      <c r="CA7" s="124"/>
-      <c r="CB7" s="124"/>
-      <c r="CC7" s="124"/>
-      <c r="CD7" s="129"/>
-      <c r="CE7" s="128" t="s">
+      <c r="BY7" s="111"/>
+      <c r="BZ7" s="111"/>
+      <c r="CA7" s="111"/>
+      <c r="CB7" s="111"/>
+      <c r="CC7" s="111"/>
+      <c r="CD7" s="114"/>
+      <c r="CE7" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="CF7" s="124"/>
-      <c r="CG7" s="124"/>
-      <c r="CH7" s="124"/>
-      <c r="CI7" s="124"/>
-      <c r="CJ7" s="124"/>
-      <c r="CK7" s="129"/>
-      <c r="CL7" s="128" t="s">
+      <c r="CF7" s="111"/>
+      <c r="CG7" s="111"/>
+      <c r="CH7" s="111"/>
+      <c r="CI7" s="111"/>
+      <c r="CJ7" s="111"/>
+      <c r="CK7" s="114"/>
+      <c r="CL7" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="CM7" s="124"/>
-      <c r="CN7" s="124"/>
-      <c r="CO7" s="124"/>
-      <c r="CP7" s="124"/>
-      <c r="CQ7" s="124"/>
-      <c r="CR7" s="129"/>
-      <c r="CS7" s="128" t="s">
+      <c r="CM7" s="111"/>
+      <c r="CN7" s="111"/>
+      <c r="CO7" s="111"/>
+      <c r="CP7" s="111"/>
+      <c r="CQ7" s="111"/>
+      <c r="CR7" s="114"/>
+      <c r="CS7" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="CT7" s="124"/>
-      <c r="CU7" s="124"/>
-      <c r="CV7" s="124"/>
-      <c r="CW7" s="124"/>
-      <c r="CX7" s="124"/>
-      <c r="CY7" s="129"/>
-      <c r="CZ7" s="128" t="s">
+      <c r="CT7" s="111"/>
+      <c r="CU7" s="111"/>
+      <c r="CV7" s="111"/>
+      <c r="CW7" s="111"/>
+      <c r="CX7" s="111"/>
+      <c r="CY7" s="114"/>
+      <c r="CZ7" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="DA7" s="124"/>
-      <c r="DB7" s="124"/>
-      <c r="DC7" s="124"/>
-      <c r="DD7" s="124"/>
-      <c r="DE7" s="124"/>
-      <c r="DF7" s="124"/>
-      <c r="DG7" s="128" t="s">
+      <c r="DA7" s="111"/>
+      <c r="DB7" s="111"/>
+      <c r="DC7" s="111"/>
+      <c r="DD7" s="111"/>
+      <c r="DE7" s="111"/>
+      <c r="DF7" s="111"/>
+      <c r="DG7" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="DH7" s="124"/>
-      <c r="DI7" s="124"/>
-      <c r="DJ7" s="124"/>
-      <c r="DK7" s="124"/>
-      <c r="DL7" s="124"/>
-      <c r="DM7" s="129"/>
-      <c r="DN7" s="124" t="s">
+      <c r="DH7" s="111"/>
+      <c r="DI7" s="111"/>
+      <c r="DJ7" s="111"/>
+      <c r="DK7" s="111"/>
+      <c r="DL7" s="111"/>
+      <c r="DM7" s="114"/>
+      <c r="DN7" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="DO7" s="124"/>
-      <c r="DP7" s="124"/>
-      <c r="DQ7" s="124"/>
-      <c r="DR7" s="124"/>
-      <c r="DS7" s="124"/>
-      <c r="DT7" s="124"/>
-      <c r="DU7" s="128" t="s">
+      <c r="DO7" s="111"/>
+      <c r="DP7" s="111"/>
+      <c r="DQ7" s="111"/>
+      <c r="DR7" s="111"/>
+      <c r="DS7" s="111"/>
+      <c r="DT7" s="111"/>
+      <c r="DU7" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="DV7" s="124"/>
-      <c r="DW7" s="124"/>
-      <c r="DX7" s="124"/>
-      <c r="DY7" s="124"/>
-      <c r="DZ7" s="124"/>
-      <c r="EA7" s="129"/>
-      <c r="EB7" s="124" t="s">
+      <c r="DV7" s="111"/>
+      <c r="DW7" s="111"/>
+      <c r="DX7" s="111"/>
+      <c r="DY7" s="111"/>
+      <c r="DZ7" s="111"/>
+      <c r="EA7" s="114"/>
+      <c r="EB7" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="EC7" s="124"/>
-      <c r="ED7" s="124"/>
-      <c r="EE7" s="124"/>
-      <c r="EF7" s="124"/>
-      <c r="EG7" s="124"/>
-      <c r="EH7" s="124"/>
-      <c r="EI7" s="128" t="s">
+      <c r="EC7" s="111"/>
+      <c r="ED7" s="111"/>
+      <c r="EE7" s="111"/>
+      <c r="EF7" s="111"/>
+      <c r="EG7" s="111"/>
+      <c r="EH7" s="111"/>
+      <c r="EI7" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="EJ7" s="124"/>
-      <c r="EK7" s="124"/>
-      <c r="EL7" s="124"/>
-      <c r="EM7" s="124"/>
-      <c r="EN7" s="124"/>
-      <c r="EO7" s="129"/>
-      <c r="EP7" s="124" t="s">
+      <c r="EJ7" s="111"/>
+      <c r="EK7" s="111"/>
+      <c r="EL7" s="111"/>
+      <c r="EM7" s="111"/>
+      <c r="EN7" s="111"/>
+      <c r="EO7" s="114"/>
+      <c r="EP7" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="EQ7" s="124"/>
-      <c r="ER7" s="124"/>
-      <c r="ES7" s="124"/>
-      <c r="ET7" s="124"/>
-      <c r="EU7" s="124"/>
-      <c r="EV7" s="124"/>
-      <c r="EW7" s="128" t="s">
+      <c r="EQ7" s="111"/>
+      <c r="ER7" s="111"/>
+      <c r="ES7" s="111"/>
+      <c r="ET7" s="111"/>
+      <c r="EU7" s="111"/>
+      <c r="EV7" s="111"/>
+      <c r="EW7" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="EX7" s="124"/>
-      <c r="EY7" s="124"/>
-      <c r="EZ7" s="124"/>
-      <c r="FA7" s="124"/>
-      <c r="FB7" s="124"/>
-      <c r="FC7" s="129"/>
-      <c r="FD7" s="124" t="s">
+      <c r="EX7" s="111"/>
+      <c r="EY7" s="111"/>
+      <c r="EZ7" s="111"/>
+      <c r="FA7" s="111"/>
+      <c r="FB7" s="111"/>
+      <c r="FC7" s="114"/>
+      <c r="FD7" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="FE7" s="124"/>
-      <c r="FF7" s="124"/>
-      <c r="FG7" s="124"/>
-      <c r="FH7" s="124"/>
-      <c r="FI7" s="124"/>
-      <c r="FJ7" s="124"/>
-      <c r="FK7" s="128" t="s">
+      <c r="FE7" s="111"/>
+      <c r="FF7" s="111"/>
+      <c r="FG7" s="111"/>
+      <c r="FH7" s="111"/>
+      <c r="FI7" s="111"/>
+      <c r="FJ7" s="111"/>
+      <c r="FK7" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="FL7" s="124"/>
-      <c r="FM7" s="124"/>
-      <c r="FN7" s="124"/>
-      <c r="FO7" s="124"/>
-      <c r="FP7" s="124"/>
-      <c r="FQ7" s="129"/>
-      <c r="FR7" s="124" t="s">
+      <c r="FL7" s="111"/>
+      <c r="FM7" s="111"/>
+      <c r="FN7" s="111"/>
+      <c r="FO7" s="111"/>
+      <c r="FP7" s="111"/>
+      <c r="FQ7" s="114"/>
+      <c r="FR7" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="FS7" s="124"/>
-      <c r="FT7" s="124"/>
-      <c r="FU7" s="124"/>
-      <c r="FV7" s="124"/>
-      <c r="FW7" s="124"/>
-      <c r="FX7" s="124"/>
-      <c r="FY7" s="128" t="s">
+      <c r="FS7" s="111"/>
+      <c r="FT7" s="111"/>
+      <c r="FU7" s="111"/>
+      <c r="FV7" s="111"/>
+      <c r="FW7" s="111"/>
+      <c r="FX7" s="111"/>
+      <c r="FY7" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="FZ7" s="124"/>
-      <c r="GA7" s="124"/>
-      <c r="GB7" s="124"/>
-      <c r="GC7" s="146"/>
+      <c r="FZ7" s="111"/>
+      <c r="GA7" s="111"/>
+      <c r="GB7" s="111"/>
+      <c r="GC7" s="112"/>
     </row>
     <row r="8" spans="1:185" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="125" t="s">
+      <c r="A8" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="126"/>
-      <c r="E8" s="127"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
       <c r="F8" s="25">
         <v>19</v>
       </c>
@@ -15491,15 +15491,12 @@
       <c r="GB67" s="11"/>
       <c r="GC67" s="24"/>
     </row>
-    <row r="68" spans="1:185" x14ac:dyDescent="0.2">
-      <c r="A68" s="33"/>
-      <c r="B68" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C68" s="47">
-        <v>42720</v>
-      </c>
-      <c r="D68" s="7"/>
+    <row r="68" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="32"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="42"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
@@ -15594,7 +15591,7 @@
       <c r="CS68" s="23"/>
       <c r="CT68" s="11"/>
       <c r="CU68" s="11"/>
-      <c r="CV68" s="90"/>
+      <c r="CV68" s="67"/>
       <c r="CW68" s="11"/>
       <c r="CX68" s="11"/>
       <c r="CY68" s="22"/>
@@ -15684,10 +15681,10 @@
     <row r="69" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A69" s="33"/>
       <c r="B69" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C69" s="47">
-        <v>42776</v>
+        <v>42720</v>
       </c>
       <c r="D69" s="7"/>
       <c r="F69" s="11"/>
@@ -15778,13 +15775,13 @@
       <c r="CM69" s="11"/>
       <c r="CN69" s="11"/>
       <c r="CO69" s="11"/>
-      <c r="CP69" s="11"/>
+      <c r="CP69" s="51"/>
       <c r="CQ69" s="11"/>
       <c r="CR69" s="11"/>
       <c r="CS69" s="23"/>
       <c r="CT69" s="11"/>
       <c r="CU69" s="11"/>
-      <c r="CV69" s="90"/>
+      <c r="CV69" s="67"/>
       <c r="CW69" s="11"/>
       <c r="CX69" s="11"/>
       <c r="CY69" s="22"/>
@@ -15871,11 +15868,12 @@
       <c r="GB69" s="11"/>
       <c r="GC69" s="24"/>
     </row>
-    <row r="70" spans="1:185" x14ac:dyDescent="0.2">
-      <c r="A70" s="33"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
+    <row r="70" spans="1:185" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="32"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="42"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
@@ -16060,9 +16058,11 @@
     <row r="71" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A71" s="33"/>
       <c r="B71" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="C71" s="47">
+        <v>42776</v>
+      </c>
       <c r="D71" s="7"/>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
@@ -16162,20 +16162,20 @@
       <c r="CW71" s="11"/>
       <c r="CX71" s="11"/>
       <c r="CY71" s="22"/>
-      <c r="CZ71" s="51"/>
-      <c r="DA71" s="51"/>
-      <c r="DB71" s="51"/>
-      <c r="DC71" s="51"/>
-      <c r="DD71" s="51"/>
-      <c r="DE71" s="51"/>
-      <c r="DF71" s="51"/>
-      <c r="DG71" s="63"/>
-      <c r="DH71" s="51"/>
-      <c r="DI71" s="51"/>
-      <c r="DJ71" s="51"/>
-      <c r="DK71" s="51"/>
-      <c r="DL71" s="51"/>
-      <c r="DM71" s="64"/>
+      <c r="CZ71" s="11"/>
+      <c r="DA71" s="11"/>
+      <c r="DB71" s="11"/>
+      <c r="DC71" s="11"/>
+      <c r="DD71" s="11"/>
+      <c r="DE71" s="11"/>
+      <c r="DF71" s="11"/>
+      <c r="DG71" s="23"/>
+      <c r="DH71" s="11"/>
+      <c r="DI71" s="11"/>
+      <c r="DJ71" s="11"/>
+      <c r="DK71" s="11"/>
+      <c r="DL71" s="11"/>
+      <c r="DM71" s="22"/>
       <c r="DN71" s="11"/>
       <c r="DO71" s="11"/>
       <c r="DP71" s="11"/>
@@ -16208,7 +16208,7 @@
       <c r="EQ71" s="11"/>
       <c r="ER71" s="11"/>
       <c r="ES71" s="11"/>
-      <c r="ET71" s="11"/>
+      <c r="ET71" s="51"/>
       <c r="EU71" s="11"/>
       <c r="EV71" s="11"/>
       <c r="EW71" s="23"/>
@@ -16245,7 +16245,7 @@
       <c r="GB71" s="11"/>
       <c r="GC71" s="24"/>
     </row>
-    <row r="72" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A72" s="33"/>
       <c r="B72" s="9"/>
       <c r="C72" s="7"/>
@@ -16434,7 +16434,7 @@
     <row r="73" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A73" s="33"/>
       <c r="B73" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -16529,13 +16529,13 @@
       <c r="CP73" s="11"/>
       <c r="CQ73" s="11"/>
       <c r="CR73" s="11"/>
-      <c r="CS73" s="63"/>
-      <c r="CT73" s="51"/>
-      <c r="CU73" s="51"/>
-      <c r="CV73" s="90"/>
-      <c r="CW73" s="51"/>
-      <c r="CX73" s="51"/>
-      <c r="CY73" s="64"/>
+      <c r="CS73" s="23"/>
+      <c r="CT73" s="11"/>
+      <c r="CU73" s="11"/>
+      <c r="CV73" s="67"/>
+      <c r="CW73" s="11"/>
+      <c r="CX73" s="11"/>
+      <c r="CY73" s="22"/>
       <c r="CZ73" s="51"/>
       <c r="DA73" s="51"/>
       <c r="DB73" s="51"/>
@@ -16550,36 +16550,36 @@
       <c r="DK73" s="51"/>
       <c r="DL73" s="51"/>
       <c r="DM73" s="64"/>
-      <c r="DN73" s="51"/>
-      <c r="DO73" s="51"/>
-      <c r="DP73" s="51"/>
-      <c r="DQ73" s="51"/>
-      <c r="DR73" s="51"/>
-      <c r="DS73" s="51"/>
-      <c r="DT73" s="51"/>
-      <c r="DU73" s="63"/>
-      <c r="DV73" s="51"/>
-      <c r="DW73" s="51"/>
-      <c r="DX73" s="51"/>
-      <c r="DY73" s="51"/>
-      <c r="DZ73" s="51"/>
-      <c r="EA73" s="64"/>
-      <c r="EB73" s="51"/>
-      <c r="EC73" s="51"/>
-      <c r="ED73" s="147"/>
-      <c r="EE73" s="51"/>
-      <c r="EF73" s="51"/>
-      <c r="EG73" s="51"/>
-      <c r="EH73" s="51"/>
-      <c r="EI73" s="63"/>
-      <c r="EJ73" s="51"/>
-      <c r="EK73" s="51"/>
-      <c r="EL73" s="51"/>
-      <c r="EM73" s="51"/>
-      <c r="EN73" s="51"/>
-      <c r="EO73" s="64"/>
-      <c r="EP73" s="51"/>
-      <c r="EQ73" s="51"/>
+      <c r="DN73" s="11"/>
+      <c r="DO73" s="11"/>
+      <c r="DP73" s="11"/>
+      <c r="DQ73" s="11"/>
+      <c r="DR73" s="11"/>
+      <c r="DS73" s="11"/>
+      <c r="DT73" s="11"/>
+      <c r="DU73" s="23"/>
+      <c r="DV73" s="11"/>
+      <c r="DW73" s="11"/>
+      <c r="DX73" s="11"/>
+      <c r="DY73" s="11"/>
+      <c r="DZ73" s="11"/>
+      <c r="EA73" s="22"/>
+      <c r="EB73" s="11"/>
+      <c r="EC73" s="11"/>
+      <c r="ED73" s="73"/>
+      <c r="EE73" s="11"/>
+      <c r="EF73" s="11"/>
+      <c r="EG73" s="11"/>
+      <c r="EH73" s="11"/>
+      <c r="EI73" s="23"/>
+      <c r="EJ73" s="11"/>
+      <c r="EK73" s="11"/>
+      <c r="EL73" s="11"/>
+      <c r="EM73" s="11"/>
+      <c r="EN73" s="11"/>
+      <c r="EO73" s="22"/>
+      <c r="EP73" s="11"/>
+      <c r="EQ73" s="11"/>
       <c r="ER73" s="11"/>
       <c r="ES73" s="11"/>
       <c r="ET73" s="11"/>
@@ -16808,7 +16808,7 @@
     <row r="75" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A75" s="33"/>
       <c r="B75" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -16903,13 +16903,13 @@
       <c r="CP75" s="11"/>
       <c r="CQ75" s="11"/>
       <c r="CR75" s="11"/>
-      <c r="CS75" s="23"/>
-      <c r="CT75" s="11"/>
-      <c r="CU75" s="11"/>
-      <c r="CV75" s="67"/>
-      <c r="CW75" s="11"/>
-      <c r="CX75" s="11"/>
-      <c r="CY75" s="22"/>
+      <c r="CS75" s="63"/>
+      <c r="CT75" s="51"/>
+      <c r="CU75" s="51"/>
+      <c r="CV75" s="90"/>
+      <c r="CW75" s="51"/>
+      <c r="CX75" s="51"/>
+      <c r="CY75" s="64"/>
       <c r="CZ75" s="51"/>
       <c r="DA75" s="51"/>
       <c r="DB75" s="51"/>
@@ -16924,36 +16924,36 @@
       <c r="DK75" s="51"/>
       <c r="DL75" s="51"/>
       <c r="DM75" s="64"/>
-      <c r="DN75" s="11"/>
-      <c r="DO75" s="11"/>
-      <c r="DP75" s="11"/>
-      <c r="DQ75" s="11"/>
-      <c r="DR75" s="11"/>
-      <c r="DS75" s="11"/>
-      <c r="DT75" s="11"/>
-      <c r="DU75" s="23"/>
-      <c r="DV75" s="11"/>
-      <c r="DW75" s="11"/>
-      <c r="DX75" s="11"/>
-      <c r="DY75" s="11"/>
-      <c r="DZ75" s="11"/>
-      <c r="EA75" s="22"/>
-      <c r="EB75" s="11"/>
-      <c r="EC75" s="11"/>
-      <c r="ED75" s="73"/>
-      <c r="EE75" s="11"/>
-      <c r="EF75" s="11"/>
-      <c r="EG75" s="11"/>
-      <c r="EH75" s="11"/>
-      <c r="EI75" s="23"/>
-      <c r="EJ75" s="11"/>
-      <c r="EK75" s="11"/>
-      <c r="EL75" s="11"/>
-      <c r="EM75" s="11"/>
-      <c r="EN75" s="11"/>
-      <c r="EO75" s="22"/>
-      <c r="EP75" s="11"/>
-      <c r="EQ75" s="11"/>
+      <c r="DN75" s="51"/>
+      <c r="DO75" s="51"/>
+      <c r="DP75" s="51"/>
+      <c r="DQ75" s="51"/>
+      <c r="DR75" s="51"/>
+      <c r="DS75" s="51"/>
+      <c r="DT75" s="51"/>
+      <c r="DU75" s="63"/>
+      <c r="DV75" s="51"/>
+      <c r="DW75" s="51"/>
+      <c r="DX75" s="51"/>
+      <c r="DY75" s="51"/>
+      <c r="DZ75" s="51"/>
+      <c r="EA75" s="64"/>
+      <c r="EB75" s="51"/>
+      <c r="EC75" s="51"/>
+      <c r="ED75" s="108"/>
+      <c r="EE75" s="51"/>
+      <c r="EF75" s="51"/>
+      <c r="EG75" s="51"/>
+      <c r="EH75" s="51"/>
+      <c r="EI75" s="63"/>
+      <c r="EJ75" s="51"/>
+      <c r="EK75" s="51"/>
+      <c r="EL75" s="51"/>
+      <c r="EM75" s="51"/>
+      <c r="EN75" s="51"/>
+      <c r="EO75" s="64"/>
+      <c r="EP75" s="51"/>
+      <c r="EQ75" s="51"/>
       <c r="ER75" s="11"/>
       <c r="ES75" s="11"/>
       <c r="ET75" s="11"/>
@@ -17182,7 +17182,7 @@
     <row r="77" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A77" s="33"/>
       <c r="B77" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -17284,20 +17284,20 @@
       <c r="CW77" s="11"/>
       <c r="CX77" s="11"/>
       <c r="CY77" s="22"/>
-      <c r="CZ77" s="11"/>
-      <c r="DA77" s="11"/>
-      <c r="DB77" s="11"/>
-      <c r="DC77" s="11"/>
-      <c r="DD77" s="11"/>
-      <c r="DE77" s="11"/>
-      <c r="DF77" s="11"/>
-      <c r="DG77" s="23"/>
-      <c r="DH77" s="11"/>
-      <c r="DI77" s="11"/>
-      <c r="DJ77" s="11"/>
-      <c r="DK77" s="11"/>
-      <c r="DL77" s="11"/>
-      <c r="DM77" s="22"/>
+      <c r="CZ77" s="51"/>
+      <c r="DA77" s="51"/>
+      <c r="DB77" s="51"/>
+      <c r="DC77" s="51"/>
+      <c r="DD77" s="51"/>
+      <c r="DE77" s="51"/>
+      <c r="DF77" s="51"/>
+      <c r="DG77" s="63"/>
+      <c r="DH77" s="51"/>
+      <c r="DI77" s="51"/>
+      <c r="DJ77" s="51"/>
+      <c r="DK77" s="51"/>
+      <c r="DL77" s="51"/>
+      <c r="DM77" s="64"/>
       <c r="DN77" s="11"/>
       <c r="DO77" s="11"/>
       <c r="DP77" s="11"/>
@@ -17367,7 +17367,7 @@
       <c r="GB77" s="11"/>
       <c r="GC77" s="24"/>
     </row>
-    <row r="78" spans="1:185" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:185" ht="2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="33"/>
       <c r="B78" s="9"/>
       <c r="C78" s="7"/>
@@ -17555,7 +17555,9 @@
     </row>
     <row r="79" spans="1:185" x14ac:dyDescent="0.2">
       <c r="A79" s="33"/>
-      <c r="B79" s="9"/>
+      <c r="B79" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="F79" s="11"/>
@@ -17739,209 +17741,622 @@
       <c r="GB79" s="11"/>
       <c r="GC79" s="24"/>
     </row>
-    <row r="80" spans="1:185" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="112" t="s">
+    <row r="80" spans="1:185" x14ac:dyDescent="0.2">
+      <c r="A80" s="33"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="11"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="23"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="22"/>
+      <c r="T80" s="11"/>
+      <c r="U80" s="11"/>
+      <c r="V80" s="11"/>
+      <c r="W80" s="11"/>
+      <c r="X80" s="11"/>
+      <c r="Y80" s="11"/>
+      <c r="Z80" s="11"/>
+      <c r="AA80" s="23"/>
+      <c r="AB80" s="11"/>
+      <c r="AC80" s="11"/>
+      <c r="AD80" s="11"/>
+      <c r="AE80" s="11"/>
+      <c r="AF80" s="11"/>
+      <c r="AG80" s="22"/>
+      <c r="AH80" s="11"/>
+      <c r="AI80" s="11"/>
+      <c r="AJ80" s="11"/>
+      <c r="AK80" s="11"/>
+      <c r="AL80" s="11"/>
+      <c r="AM80" s="11"/>
+      <c r="AN80" s="11"/>
+      <c r="AO80" s="76"/>
+      <c r="AP80" s="11"/>
+      <c r="AQ80" s="11"/>
+      <c r="AR80" s="11"/>
+      <c r="AS80" s="11"/>
+      <c r="AT80" s="11"/>
+      <c r="AU80" s="22"/>
+      <c r="AV80" s="11"/>
+      <c r="AW80" s="11"/>
+      <c r="AX80" s="11"/>
+      <c r="AY80" s="11"/>
+      <c r="AZ80" s="11"/>
+      <c r="BA80" s="11"/>
+      <c r="BB80" s="11"/>
+      <c r="BC80" s="23"/>
+      <c r="BD80" s="11"/>
+      <c r="BE80" s="11"/>
+      <c r="BF80" s="11"/>
+      <c r="BG80" s="11"/>
+      <c r="BH80" s="11"/>
+      <c r="BI80" s="22"/>
+      <c r="BJ80" s="11"/>
+      <c r="BK80" s="11"/>
+      <c r="BL80" s="11"/>
+      <c r="BM80" s="11"/>
+      <c r="BN80" s="11"/>
+      <c r="BO80" s="11"/>
+      <c r="BP80" s="11"/>
+      <c r="BQ80" s="23"/>
+      <c r="BR80" s="11"/>
+      <c r="BS80" s="11"/>
+      <c r="BT80" s="11"/>
+      <c r="BU80" s="11"/>
+      <c r="BV80" s="11"/>
+      <c r="BW80" s="22"/>
+      <c r="BX80" s="11"/>
+      <c r="BY80" s="11"/>
+      <c r="BZ80" s="73"/>
+      <c r="CA80" s="11"/>
+      <c r="CB80" s="11"/>
+      <c r="CC80" s="11"/>
+      <c r="CD80" s="11"/>
+      <c r="CE80" s="23"/>
+      <c r="CF80" s="11"/>
+      <c r="CG80" s="11"/>
+      <c r="CH80" s="11"/>
+      <c r="CI80" s="11"/>
+      <c r="CJ80" s="11"/>
+      <c r="CK80" s="22"/>
+      <c r="CL80" s="11"/>
+      <c r="CM80" s="11"/>
+      <c r="CN80" s="11"/>
+      <c r="CO80" s="11"/>
+      <c r="CP80" s="11"/>
+      <c r="CQ80" s="11"/>
+      <c r="CR80" s="11"/>
+      <c r="CS80" s="23"/>
+      <c r="CT80" s="11"/>
+      <c r="CU80" s="11"/>
+      <c r="CV80" s="67"/>
+      <c r="CW80" s="11"/>
+      <c r="CX80" s="11"/>
+      <c r="CY80" s="22"/>
+      <c r="CZ80" s="11"/>
+      <c r="DA80" s="11"/>
+      <c r="DB80" s="11"/>
+      <c r="DC80" s="11"/>
+      <c r="DD80" s="11"/>
+      <c r="DE80" s="11"/>
+      <c r="DF80" s="11"/>
+      <c r="DG80" s="23"/>
+      <c r="DH80" s="11"/>
+      <c r="DI80" s="11"/>
+      <c r="DJ80" s="11"/>
+      <c r="DK80" s="11"/>
+      <c r="DL80" s="11"/>
+      <c r="DM80" s="22"/>
+      <c r="DN80" s="11"/>
+      <c r="DO80" s="11"/>
+      <c r="DP80" s="11"/>
+      <c r="DQ80" s="11"/>
+      <c r="DR80" s="11"/>
+      <c r="DS80" s="11"/>
+      <c r="DT80" s="11"/>
+      <c r="DU80" s="23"/>
+      <c r="DV80" s="11"/>
+      <c r="DW80" s="11"/>
+      <c r="DX80" s="11"/>
+      <c r="DY80" s="11"/>
+      <c r="DZ80" s="11"/>
+      <c r="EA80" s="22"/>
+      <c r="EB80" s="11"/>
+      <c r="EC80" s="11"/>
+      <c r="ED80" s="73"/>
+      <c r="EE80" s="11"/>
+      <c r="EF80" s="11"/>
+      <c r="EG80" s="11"/>
+      <c r="EH80" s="11"/>
+      <c r="EI80" s="23"/>
+      <c r="EJ80" s="11"/>
+      <c r="EK80" s="11"/>
+      <c r="EL80" s="11"/>
+      <c r="EM80" s="11"/>
+      <c r="EN80" s="11"/>
+      <c r="EO80" s="22"/>
+      <c r="EP80" s="11"/>
+      <c r="EQ80" s="11"/>
+      <c r="ER80" s="11"/>
+      <c r="ES80" s="11"/>
+      <c r="ET80" s="11"/>
+      <c r="EU80" s="11"/>
+      <c r="EV80" s="11"/>
+      <c r="EW80" s="23"/>
+      <c r="EX80" s="11"/>
+      <c r="EY80" s="11"/>
+      <c r="EZ80" s="11"/>
+      <c r="FA80" s="11"/>
+      <c r="FB80" s="11"/>
+      <c r="FC80" s="22"/>
+      <c r="FD80" s="11"/>
+      <c r="FE80" s="11"/>
+      <c r="FF80" s="11"/>
+      <c r="FG80" s="11"/>
+      <c r="FH80" s="11"/>
+      <c r="FI80" s="11"/>
+      <c r="FJ80" s="11"/>
+      <c r="FK80" s="23"/>
+      <c r="FL80" s="11"/>
+      <c r="FM80" s="67"/>
+      <c r="FN80" s="11"/>
+      <c r="FO80" s="11"/>
+      <c r="FP80" s="11"/>
+      <c r="FQ80" s="22"/>
+      <c r="FR80" s="11"/>
+      <c r="FS80" s="11"/>
+      <c r="FT80" s="11"/>
+      <c r="FU80" s="11"/>
+      <c r="FV80" s="11"/>
+      <c r="FW80" s="11"/>
+      <c r="FX80" s="11"/>
+      <c r="FY80" s="23"/>
+      <c r="FZ80" s="11"/>
+      <c r="GA80" s="11"/>
+      <c r="GB80" s="11"/>
+      <c r="GC80" s="24"/>
+    </row>
+    <row r="81" spans="1:185" x14ac:dyDescent="0.2">
+      <c r="A81" s="33"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="11"/>
+      <c r="K81" s="11"/>
+      <c r="L81" s="11"/>
+      <c r="M81" s="23"/>
+      <c r="N81" s="11"/>
+      <c r="O81" s="11"/>
+      <c r="P81" s="11"/>
+      <c r="Q81" s="11"/>
+      <c r="R81" s="11"/>
+      <c r="S81" s="22"/>
+      <c r="T81" s="11"/>
+      <c r="U81" s="11"/>
+      <c r="V81" s="11"/>
+      <c r="W81" s="11"/>
+      <c r="X81" s="11"/>
+      <c r="Y81" s="11"/>
+      <c r="Z81" s="11"/>
+      <c r="AA81" s="23"/>
+      <c r="AB81" s="11"/>
+      <c r="AC81" s="11"/>
+      <c r="AD81" s="11"/>
+      <c r="AE81" s="11"/>
+      <c r="AF81" s="11"/>
+      <c r="AG81" s="22"/>
+      <c r="AH81" s="11"/>
+      <c r="AI81" s="11"/>
+      <c r="AJ81" s="11"/>
+      <c r="AK81" s="11"/>
+      <c r="AL81" s="11"/>
+      <c r="AM81" s="11"/>
+      <c r="AN81" s="11"/>
+      <c r="AO81" s="76"/>
+      <c r="AP81" s="11"/>
+      <c r="AQ81" s="11"/>
+      <c r="AR81" s="11"/>
+      <c r="AS81" s="11"/>
+      <c r="AT81" s="11"/>
+      <c r="AU81" s="22"/>
+      <c r="AV81" s="11"/>
+      <c r="AW81" s="11"/>
+      <c r="AX81" s="11"/>
+      <c r="AY81" s="11"/>
+      <c r="AZ81" s="11"/>
+      <c r="BA81" s="11"/>
+      <c r="BB81" s="11"/>
+      <c r="BC81" s="23"/>
+      <c r="BD81" s="11"/>
+      <c r="BE81" s="11"/>
+      <c r="BF81" s="11"/>
+      <c r="BG81" s="11"/>
+      <c r="BH81" s="11"/>
+      <c r="BI81" s="22"/>
+      <c r="BJ81" s="11"/>
+      <c r="BK81" s="11"/>
+      <c r="BL81" s="11"/>
+      <c r="BM81" s="11"/>
+      <c r="BN81" s="11"/>
+      <c r="BO81" s="11"/>
+      <c r="BP81" s="11"/>
+      <c r="BQ81" s="23"/>
+      <c r="BR81" s="11"/>
+      <c r="BS81" s="11"/>
+      <c r="BT81" s="11"/>
+      <c r="BU81" s="11"/>
+      <c r="BV81" s="11"/>
+      <c r="BW81" s="22"/>
+      <c r="BX81" s="11"/>
+      <c r="BY81" s="11"/>
+      <c r="BZ81" s="73"/>
+      <c r="CA81" s="11"/>
+      <c r="CB81" s="11"/>
+      <c r="CC81" s="11"/>
+      <c r="CD81" s="11"/>
+      <c r="CE81" s="23"/>
+      <c r="CF81" s="11"/>
+      <c r="CG81" s="11"/>
+      <c r="CH81" s="11"/>
+      <c r="CI81" s="11"/>
+      <c r="CJ81" s="11"/>
+      <c r="CK81" s="22"/>
+      <c r="CL81" s="11"/>
+      <c r="CM81" s="11"/>
+      <c r="CN81" s="11"/>
+      <c r="CO81" s="11"/>
+      <c r="CP81" s="11"/>
+      <c r="CQ81" s="11"/>
+      <c r="CR81" s="11"/>
+      <c r="CS81" s="23"/>
+      <c r="CT81" s="11"/>
+      <c r="CU81" s="11"/>
+      <c r="CV81" s="67"/>
+      <c r="CW81" s="11"/>
+      <c r="CX81" s="11"/>
+      <c r="CY81" s="22"/>
+      <c r="CZ81" s="11"/>
+      <c r="DA81" s="11"/>
+      <c r="DB81" s="11"/>
+      <c r="DC81" s="11"/>
+      <c r="DD81" s="11"/>
+      <c r="DE81" s="11"/>
+      <c r="DF81" s="11"/>
+      <c r="DG81" s="23"/>
+      <c r="DH81" s="11"/>
+      <c r="DI81" s="11"/>
+      <c r="DJ81" s="11"/>
+      <c r="DK81" s="11"/>
+      <c r="DL81" s="11"/>
+      <c r="DM81" s="22"/>
+      <c r="DN81" s="11"/>
+      <c r="DO81" s="11"/>
+      <c r="DP81" s="11"/>
+      <c r="DQ81" s="11"/>
+      <c r="DR81" s="11"/>
+      <c r="DS81" s="11"/>
+      <c r="DT81" s="11"/>
+      <c r="DU81" s="23"/>
+      <c r="DV81" s="11"/>
+      <c r="DW81" s="11"/>
+      <c r="DX81" s="11"/>
+      <c r="DY81" s="11"/>
+      <c r="DZ81" s="11"/>
+      <c r="EA81" s="22"/>
+      <c r="EB81" s="11"/>
+      <c r="EC81" s="11"/>
+      <c r="ED81" s="73"/>
+      <c r="EE81" s="11"/>
+      <c r="EF81" s="11"/>
+      <c r="EG81" s="11"/>
+      <c r="EH81" s="11"/>
+      <c r="EI81" s="23"/>
+      <c r="EJ81" s="11"/>
+      <c r="EK81" s="11"/>
+      <c r="EL81" s="11"/>
+      <c r="EM81" s="11"/>
+      <c r="EN81" s="11"/>
+      <c r="EO81" s="22"/>
+      <c r="EP81" s="11"/>
+      <c r="EQ81" s="11"/>
+      <c r="ER81" s="11"/>
+      <c r="ES81" s="11"/>
+      <c r="ET81" s="11"/>
+      <c r="EU81" s="11"/>
+      <c r="EV81" s="11"/>
+      <c r="EW81" s="23"/>
+      <c r="EX81" s="11"/>
+      <c r="EY81" s="11"/>
+      <c r="EZ81" s="11"/>
+      <c r="FA81" s="11"/>
+      <c r="FB81" s="11"/>
+      <c r="FC81" s="22"/>
+      <c r="FD81" s="11"/>
+      <c r="FE81" s="11"/>
+      <c r="FF81" s="11"/>
+      <c r="FG81" s="11"/>
+      <c r="FH81" s="11"/>
+      <c r="FI81" s="11"/>
+      <c r="FJ81" s="11"/>
+      <c r="FK81" s="23"/>
+      <c r="FL81" s="11"/>
+      <c r="FM81" s="67"/>
+      <c r="FN81" s="11"/>
+      <c r="FO81" s="11"/>
+      <c r="FP81" s="11"/>
+      <c r="FQ81" s="22"/>
+      <c r="FR81" s="11"/>
+      <c r="FS81" s="11"/>
+      <c r="FT81" s="11"/>
+      <c r="FU81" s="11"/>
+      <c r="FV81" s="11"/>
+      <c r="FW81" s="11"/>
+      <c r="FX81" s="11"/>
+      <c r="FY81" s="23"/>
+      <c r="FZ81" s="11"/>
+      <c r="GA81" s="11"/>
+      <c r="GB81" s="11"/>
+      <c r="GC81" s="24"/>
+    </row>
+    <row r="82" spans="1:185" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="113"/>
-      <c r="C80" s="113"/>
-      <c r="D80" s="113"/>
-      <c r="E80" s="114"/>
-      <c r="F80" s="115" t="s">
+      <c r="B82" s="143"/>
+      <c r="C82" s="143"/>
+      <c r="D82" s="143"/>
+      <c r="E82" s="144"/>
+      <c r="F82" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G80" s="109"/>
-      <c r="H80" s="109"/>
-      <c r="I80" s="109"/>
-      <c r="J80" s="109"/>
-      <c r="K80" s="109"/>
-      <c r="L80" s="109"/>
-      <c r="M80" s="109"/>
-      <c r="N80" s="109"/>
-      <c r="O80" s="109"/>
-      <c r="P80" s="109"/>
-      <c r="Q80" s="109"/>
-      <c r="R80" s="109"/>
-      <c r="S80" s="109"/>
-      <c r="T80" s="109"/>
-      <c r="U80" s="109"/>
-      <c r="V80" s="109"/>
-      <c r="W80" s="109"/>
-      <c r="X80" s="109"/>
-      <c r="Y80" s="109"/>
-      <c r="Z80" s="109"/>
-      <c r="AA80" s="109"/>
-      <c r="AB80" s="109"/>
-      <c r="AC80" s="109"/>
-      <c r="AD80" s="109"/>
-      <c r="AE80" s="109"/>
-      <c r="AF80" s="109"/>
-      <c r="AG80" s="109"/>
-      <c r="AH80" s="109"/>
-      <c r="AI80" s="109"/>
-      <c r="AJ80" s="109"/>
-      <c r="AK80" s="109"/>
-      <c r="AL80" s="109"/>
-      <c r="AM80" s="109"/>
-      <c r="AN80" s="116"/>
-      <c r="AO80" s="117" t="s">
+      <c r="G82" s="139"/>
+      <c r="H82" s="139"/>
+      <c r="I82" s="139"/>
+      <c r="J82" s="139"/>
+      <c r="K82" s="139"/>
+      <c r="L82" s="139"/>
+      <c r="M82" s="139"/>
+      <c r="N82" s="139"/>
+      <c r="O82" s="139"/>
+      <c r="P82" s="139"/>
+      <c r="Q82" s="139"/>
+      <c r="R82" s="139"/>
+      <c r="S82" s="139"/>
+      <c r="T82" s="139"/>
+      <c r="U82" s="139"/>
+      <c r="V82" s="139"/>
+      <c r="W82" s="139"/>
+      <c r="X82" s="139"/>
+      <c r="Y82" s="139"/>
+      <c r="Z82" s="139"/>
+      <c r="AA82" s="139"/>
+      <c r="AB82" s="139"/>
+      <c r="AC82" s="139"/>
+      <c r="AD82" s="139"/>
+      <c r="AE82" s="139"/>
+      <c r="AF82" s="139"/>
+      <c r="AG82" s="139"/>
+      <c r="AH82" s="139"/>
+      <c r="AI82" s="139"/>
+      <c r="AJ82" s="139"/>
+      <c r="AK82" s="139"/>
+      <c r="AL82" s="139"/>
+      <c r="AM82" s="139"/>
+      <c r="AN82" s="146"/>
+      <c r="AO82" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="AP80" s="109"/>
-      <c r="AQ80" s="109"/>
-      <c r="AR80" s="109"/>
-      <c r="AS80" s="109"/>
-      <c r="AT80" s="109"/>
-      <c r="AU80" s="109"/>
-      <c r="AV80" s="109"/>
-      <c r="AW80" s="109"/>
-      <c r="AX80" s="109"/>
-      <c r="AY80" s="109"/>
-      <c r="AZ80" s="109"/>
-      <c r="BA80" s="109"/>
-      <c r="BB80" s="109"/>
-      <c r="BC80" s="109"/>
-      <c r="BD80" s="109"/>
-      <c r="BE80" s="109"/>
-      <c r="BF80" s="109"/>
-      <c r="BG80" s="109"/>
-      <c r="BH80" s="109"/>
-      <c r="BI80" s="109"/>
-      <c r="BJ80" s="109"/>
-      <c r="BK80" s="109"/>
-      <c r="BL80" s="109"/>
-      <c r="BM80" s="109"/>
-      <c r="BN80" s="109"/>
-      <c r="BO80" s="109"/>
-      <c r="BP80" s="109"/>
-      <c r="BQ80" s="109"/>
-      <c r="BR80" s="109"/>
-      <c r="BS80" s="109"/>
-      <c r="BT80" s="109"/>
-      <c r="BU80" s="109"/>
-      <c r="BV80" s="109"/>
-      <c r="BW80" s="109"/>
-      <c r="BX80" s="109"/>
-      <c r="BY80" s="109"/>
-      <c r="BZ80" s="110"/>
-      <c r="CA80" s="108" t="s">
+      <c r="AP82" s="139"/>
+      <c r="AQ82" s="139"/>
+      <c r="AR82" s="139"/>
+      <c r="AS82" s="139"/>
+      <c r="AT82" s="139"/>
+      <c r="AU82" s="139"/>
+      <c r="AV82" s="139"/>
+      <c r="AW82" s="139"/>
+      <c r="AX82" s="139"/>
+      <c r="AY82" s="139"/>
+      <c r="AZ82" s="139"/>
+      <c r="BA82" s="139"/>
+      <c r="BB82" s="139"/>
+      <c r="BC82" s="139"/>
+      <c r="BD82" s="139"/>
+      <c r="BE82" s="139"/>
+      <c r="BF82" s="139"/>
+      <c r="BG82" s="139"/>
+      <c r="BH82" s="139"/>
+      <c r="BI82" s="139"/>
+      <c r="BJ82" s="139"/>
+      <c r="BK82" s="139"/>
+      <c r="BL82" s="139"/>
+      <c r="BM82" s="139"/>
+      <c r="BN82" s="139"/>
+      <c r="BO82" s="139"/>
+      <c r="BP82" s="139"/>
+      <c r="BQ82" s="139"/>
+      <c r="BR82" s="139"/>
+      <c r="BS82" s="139"/>
+      <c r="BT82" s="139"/>
+      <c r="BU82" s="139"/>
+      <c r="BV82" s="139"/>
+      <c r="BW82" s="139"/>
+      <c r="BX82" s="139"/>
+      <c r="BY82" s="139"/>
+      <c r="BZ82" s="140"/>
+      <c r="CA82" s="138" t="s">
         <v>93</v>
       </c>
-      <c r="CB80" s="109"/>
-      <c r="CC80" s="109"/>
-      <c r="CD80" s="109"/>
-      <c r="CE80" s="109"/>
-      <c r="CF80" s="109"/>
-      <c r="CG80" s="109"/>
-      <c r="CH80" s="109"/>
-      <c r="CI80" s="109"/>
-      <c r="CJ80" s="109"/>
-      <c r="CK80" s="109"/>
-      <c r="CL80" s="109"/>
-      <c r="CM80" s="109"/>
-      <c r="CN80" s="109"/>
-      <c r="CO80" s="109"/>
-      <c r="CP80" s="109"/>
-      <c r="CQ80" s="109"/>
-      <c r="CR80" s="109"/>
-      <c r="CS80" s="109"/>
-      <c r="CT80" s="109"/>
-      <c r="CU80" s="110"/>
-      <c r="CV80" s="108" t="s">
+      <c r="CB82" s="139"/>
+      <c r="CC82" s="139"/>
+      <c r="CD82" s="139"/>
+      <c r="CE82" s="139"/>
+      <c r="CF82" s="139"/>
+      <c r="CG82" s="139"/>
+      <c r="CH82" s="139"/>
+      <c r="CI82" s="139"/>
+      <c r="CJ82" s="139"/>
+      <c r="CK82" s="139"/>
+      <c r="CL82" s="139"/>
+      <c r="CM82" s="139"/>
+      <c r="CN82" s="139"/>
+      <c r="CO82" s="139"/>
+      <c r="CP82" s="139"/>
+      <c r="CQ82" s="139"/>
+      <c r="CR82" s="139"/>
+      <c r="CS82" s="139"/>
+      <c r="CT82" s="139"/>
+      <c r="CU82" s="140"/>
+      <c r="CV82" s="138" t="s">
         <v>94</v>
       </c>
-      <c r="CW80" s="109"/>
-      <c r="CX80" s="109"/>
-      <c r="CY80" s="109"/>
-      <c r="CZ80" s="109"/>
-      <c r="DA80" s="109"/>
-      <c r="DB80" s="109"/>
-      <c r="DC80" s="109"/>
-      <c r="DD80" s="109"/>
-      <c r="DE80" s="109"/>
-      <c r="DF80" s="109"/>
-      <c r="DG80" s="109"/>
-      <c r="DH80" s="109"/>
-      <c r="DI80" s="109"/>
-      <c r="DJ80" s="109"/>
-      <c r="DK80" s="109"/>
-      <c r="DL80" s="109"/>
-      <c r="DM80" s="109"/>
-      <c r="DN80" s="109"/>
-      <c r="DO80" s="109"/>
-      <c r="DP80" s="109"/>
-      <c r="DQ80" s="109"/>
-      <c r="DR80" s="109"/>
-      <c r="DS80" s="109"/>
-      <c r="DT80" s="109"/>
-      <c r="DU80" s="109"/>
-      <c r="DV80" s="109"/>
-      <c r="DW80" s="109"/>
-      <c r="DX80" s="109"/>
-      <c r="DY80" s="109"/>
-      <c r="DZ80" s="109"/>
-      <c r="EA80" s="109"/>
-      <c r="EB80" s="109"/>
-      <c r="EC80" s="109"/>
-      <c r="ED80" s="110"/>
-      <c r="EE80" s="108" t="s">
+      <c r="CW82" s="139"/>
+      <c r="CX82" s="139"/>
+      <c r="CY82" s="139"/>
+      <c r="CZ82" s="139"/>
+      <c r="DA82" s="139"/>
+      <c r="DB82" s="139"/>
+      <c r="DC82" s="139"/>
+      <c r="DD82" s="139"/>
+      <c r="DE82" s="139"/>
+      <c r="DF82" s="139"/>
+      <c r="DG82" s="139"/>
+      <c r="DH82" s="139"/>
+      <c r="DI82" s="139"/>
+      <c r="DJ82" s="139"/>
+      <c r="DK82" s="139"/>
+      <c r="DL82" s="139"/>
+      <c r="DM82" s="139"/>
+      <c r="DN82" s="139"/>
+      <c r="DO82" s="139"/>
+      <c r="DP82" s="139"/>
+      <c r="DQ82" s="139"/>
+      <c r="DR82" s="139"/>
+      <c r="DS82" s="139"/>
+      <c r="DT82" s="139"/>
+      <c r="DU82" s="139"/>
+      <c r="DV82" s="139"/>
+      <c r="DW82" s="139"/>
+      <c r="DX82" s="139"/>
+      <c r="DY82" s="139"/>
+      <c r="DZ82" s="139"/>
+      <c r="EA82" s="139"/>
+      <c r="EB82" s="139"/>
+      <c r="EC82" s="139"/>
+      <c r="ED82" s="140"/>
+      <c r="EE82" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="EF80" s="109"/>
-      <c r="EG80" s="109"/>
-      <c r="EH80" s="109"/>
-      <c r="EI80" s="109"/>
-      <c r="EJ80" s="109"/>
-      <c r="EK80" s="109"/>
-      <c r="EL80" s="109"/>
-      <c r="EM80" s="109"/>
-      <c r="EN80" s="109"/>
-      <c r="EO80" s="109"/>
-      <c r="EP80" s="109"/>
-      <c r="EQ80" s="109"/>
-      <c r="ER80" s="109"/>
-      <c r="ES80" s="109"/>
-      <c r="ET80" s="109"/>
-      <c r="EU80" s="109"/>
-      <c r="EV80" s="109"/>
-      <c r="EW80" s="109"/>
-      <c r="EX80" s="109"/>
-      <c r="EY80" s="109"/>
-      <c r="EZ80" s="109"/>
-      <c r="FA80" s="109"/>
-      <c r="FB80" s="109"/>
-      <c r="FC80" s="109"/>
-      <c r="FD80" s="109"/>
-      <c r="FE80" s="109"/>
-      <c r="FF80" s="109"/>
-      <c r="FG80" s="109"/>
-      <c r="FH80" s="109"/>
-      <c r="FI80" s="109"/>
-      <c r="FJ80" s="109"/>
-      <c r="FK80" s="109"/>
-      <c r="FL80" s="110"/>
-      <c r="FM80" s="108" t="s">
+      <c r="EF82" s="139"/>
+      <c r="EG82" s="139"/>
+      <c r="EH82" s="139"/>
+      <c r="EI82" s="139"/>
+      <c r="EJ82" s="139"/>
+      <c r="EK82" s="139"/>
+      <c r="EL82" s="139"/>
+      <c r="EM82" s="139"/>
+      <c r="EN82" s="139"/>
+      <c r="EO82" s="139"/>
+      <c r="EP82" s="139"/>
+      <c r="EQ82" s="139"/>
+      <c r="ER82" s="139"/>
+      <c r="ES82" s="139"/>
+      <c r="ET82" s="139"/>
+      <c r="EU82" s="139"/>
+      <c r="EV82" s="139"/>
+      <c r="EW82" s="139"/>
+      <c r="EX82" s="139"/>
+      <c r="EY82" s="139"/>
+      <c r="EZ82" s="139"/>
+      <c r="FA82" s="139"/>
+      <c r="FB82" s="139"/>
+      <c r="FC82" s="139"/>
+      <c r="FD82" s="139"/>
+      <c r="FE82" s="139"/>
+      <c r="FF82" s="139"/>
+      <c r="FG82" s="139"/>
+      <c r="FH82" s="139"/>
+      <c r="FI82" s="139"/>
+      <c r="FJ82" s="139"/>
+      <c r="FK82" s="139"/>
+      <c r="FL82" s="140"/>
+      <c r="FM82" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="FN80" s="109"/>
-      <c r="FO80" s="109"/>
-      <c r="FP80" s="109"/>
-      <c r="FQ80" s="109"/>
-      <c r="FR80" s="109"/>
-      <c r="FS80" s="109"/>
-      <c r="FT80" s="109"/>
-      <c r="FU80" s="109"/>
-      <c r="FV80" s="109"/>
-      <c r="FW80" s="109"/>
-      <c r="FX80" s="109"/>
-      <c r="FY80" s="109"/>
-      <c r="FZ80" s="109"/>
-      <c r="GA80" s="109"/>
-      <c r="GB80" s="109"/>
-      <c r="GC80" s="111"/>
+      <c r="FN82" s="139"/>
+      <c r="FO82" s="139"/>
+      <c r="FP82" s="139"/>
+      <c r="FQ82" s="139"/>
+      <c r="FR82" s="139"/>
+      <c r="FS82" s="139"/>
+      <c r="FT82" s="139"/>
+      <c r="FU82" s="139"/>
+      <c r="FV82" s="139"/>
+      <c r="FW82" s="139"/>
+      <c r="FX82" s="139"/>
+      <c r="FY82" s="139"/>
+      <c r="FZ82" s="139"/>
+      <c r="GA82" s="139"/>
+      <c r="GB82" s="139"/>
+      <c r="GC82" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="EE82:FL82"/>
+    <mergeCell ref="FM82:GC82"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="F82:AN82"/>
+    <mergeCell ref="AO82:BZ82"/>
+    <mergeCell ref="CA82:CU82"/>
+    <mergeCell ref="CV82:ED82"/>
+    <mergeCell ref="F4:AN4"/>
+    <mergeCell ref="AO4:BZ4"/>
+    <mergeCell ref="FM4:GC4"/>
+    <mergeCell ref="CA4:CU4"/>
+    <mergeCell ref="CV4:ED4"/>
+    <mergeCell ref="EE4:FL4"/>
+    <mergeCell ref="F6:Q6"/>
+    <mergeCell ref="R6:AV6"/>
+    <mergeCell ref="AW6:BZ6"/>
+    <mergeCell ref="CA6:DE6"/>
+    <mergeCell ref="F5:DE5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="BQ7:BW7"/>
+    <mergeCell ref="BX7:CD7"/>
+    <mergeCell ref="CE7:CK7"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="M7:S7"/>
+    <mergeCell ref="T7:Z7"/>
+    <mergeCell ref="AA7:AG7"/>
+    <mergeCell ref="CL7:CR7"/>
+    <mergeCell ref="CS7:CY7"/>
+    <mergeCell ref="CZ7:DF7"/>
+    <mergeCell ref="DG7:DM7"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="AH7:AN7"/>
+    <mergeCell ref="AO7:AU7"/>
+    <mergeCell ref="AV7:BB7"/>
+    <mergeCell ref="BC7:BI7"/>
+    <mergeCell ref="BJ7:BP7"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="EK6:FL6"/>
     <mergeCell ref="FM6:GC6"/>
     <mergeCell ref="DF5:GC5"/>
@@ -17956,47 +18371,6 @@
     <mergeCell ref="FY7:GC7"/>
     <mergeCell ref="DN7:DT7"/>
     <mergeCell ref="DF6:EJ6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="CL7:CR7"/>
-    <mergeCell ref="CS7:CY7"/>
-    <mergeCell ref="CZ7:DF7"/>
-    <mergeCell ref="DG7:DM7"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="AH7:AN7"/>
-    <mergeCell ref="AO7:AU7"/>
-    <mergeCell ref="AV7:BB7"/>
-    <mergeCell ref="BC7:BI7"/>
-    <mergeCell ref="BJ7:BP7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="BQ7:BW7"/>
-    <mergeCell ref="BX7:CD7"/>
-    <mergeCell ref="CE7:CK7"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="M7:S7"/>
-    <mergeCell ref="T7:Z7"/>
-    <mergeCell ref="AA7:AG7"/>
-    <mergeCell ref="F6:Q6"/>
-    <mergeCell ref="R6:AV6"/>
-    <mergeCell ref="AW6:BZ6"/>
-    <mergeCell ref="CA6:DE6"/>
-    <mergeCell ref="F5:DE5"/>
-    <mergeCell ref="F4:AN4"/>
-    <mergeCell ref="AO4:BZ4"/>
-    <mergeCell ref="FM4:GC4"/>
-    <mergeCell ref="CA4:CU4"/>
-    <mergeCell ref="CV4:ED4"/>
-    <mergeCell ref="EE4:FL4"/>
-    <mergeCell ref="EE80:FL80"/>
-    <mergeCell ref="FM80:GC80"/>
-    <mergeCell ref="A80:E80"/>
-    <mergeCell ref="F80:AN80"/>
-    <mergeCell ref="AO80:BZ80"/>
-    <mergeCell ref="CA80:CU80"/>
-    <mergeCell ref="CV80:ED80"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added time compare do documentation
</commit_message>
<xml_diff>
--- a/doc/planning/Projektplanung_Spektrometer.xlsx
+++ b/doc/planning/Projektplanung_Spektrometer.xlsx
@@ -2044,91 +2044,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2161,31 +2101,91 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2389,7 +2389,7 @@
                 <a:ea typeface="Open Sans" charset="0"/>
                 <a:cs typeface="Open Sans" charset="0"/>
               </a:rPr>
-              <a:t>Ist</a:t>
+              <a:t>Vergleich</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" b="1" baseline="0">
@@ -2397,7 +2397,7 @@
                 <a:ea typeface="Open Sans" charset="0"/>
                 <a:cs typeface="Open Sans" charset="0"/>
               </a:rPr>
-              <a:t> / Soll Vergleich</a:t>
+              <a:t> der Soll- und Ist Zeiten</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE" b="1">
               <a:latin typeface="Open Sans" charset="0"/>
@@ -2728,11 +2728,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="407822752"/>
-        <c:axId val="407825072"/>
+        <c:axId val="1808184608"/>
+        <c:axId val="1766718256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="407822752"/>
+        <c:axId val="1808184608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2775,7 +2775,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407825072"/>
+        <c:crossAx val="1766718256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2783,7 +2783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="407825072"/>
+        <c:axId val="1766718256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2834,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="407822752"/>
+        <c:crossAx val="1808184608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3786,13 +3786,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:185" s="12" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="159" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="133"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="161"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -3975,11 +3975,11 @@
       <c r="GC1" s="6"/>
     </row>
     <row r="2" spans="1:185" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="143"/>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="145"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="170"/>
       <c r="F2" s="102"/>
       <c r="G2" s="102"/>
       <c r="H2" s="102"/>
@@ -4361,851 +4361,851 @@
       <c r="GC3" s="18"/>
     </row>
     <row r="4" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="134" t="s">
+      <c r="A4" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="151" t="s">
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
-      <c r="L4" s="152"/>
-      <c r="M4" s="152"/>
-      <c r="N4" s="152"/>
-      <c r="O4" s="152"/>
-      <c r="P4" s="152"/>
-      <c r="Q4" s="152"/>
-      <c r="R4" s="152"/>
-      <c r="S4" s="152"/>
-      <c r="T4" s="152"/>
-      <c r="U4" s="152"/>
-      <c r="V4" s="152"/>
-      <c r="W4" s="152"/>
-      <c r="X4" s="152"/>
-      <c r="Y4" s="152"/>
-      <c r="Z4" s="152"/>
-      <c r="AA4" s="152"/>
-      <c r="AB4" s="152"/>
-      <c r="AC4" s="152"/>
-      <c r="AD4" s="152"/>
-      <c r="AE4" s="152"/>
-      <c r="AF4" s="152"/>
-      <c r="AG4" s="152"/>
-      <c r="AH4" s="152"/>
-      <c r="AI4" s="152"/>
-      <c r="AJ4" s="152"/>
-      <c r="AK4" s="152"/>
-      <c r="AL4" s="152"/>
-      <c r="AM4" s="152"/>
-      <c r="AN4" s="152"/>
-      <c r="AO4" s="152" t="s">
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="145"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="145"/>
+      <c r="P4" s="145"/>
+      <c r="Q4" s="145"/>
+      <c r="R4" s="145"/>
+      <c r="S4" s="145"/>
+      <c r="T4" s="145"/>
+      <c r="U4" s="145"/>
+      <c r="V4" s="145"/>
+      <c r="W4" s="145"/>
+      <c r="X4" s="145"/>
+      <c r="Y4" s="145"/>
+      <c r="Z4" s="145"/>
+      <c r="AA4" s="145"/>
+      <c r="AB4" s="145"/>
+      <c r="AC4" s="145"/>
+      <c r="AD4" s="145"/>
+      <c r="AE4" s="145"/>
+      <c r="AF4" s="145"/>
+      <c r="AG4" s="145"/>
+      <c r="AH4" s="145"/>
+      <c r="AI4" s="145"/>
+      <c r="AJ4" s="145"/>
+      <c r="AK4" s="145"/>
+      <c r="AL4" s="145"/>
+      <c r="AM4" s="145"/>
+      <c r="AN4" s="145"/>
+      <c r="AO4" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="AP4" s="152"/>
-      <c r="AQ4" s="152"/>
-      <c r="AR4" s="152"/>
-      <c r="AS4" s="152"/>
-      <c r="AT4" s="152"/>
-      <c r="AU4" s="152"/>
-      <c r="AV4" s="152"/>
-      <c r="AW4" s="152"/>
-      <c r="AX4" s="152"/>
-      <c r="AY4" s="152"/>
-      <c r="AZ4" s="152"/>
-      <c r="BA4" s="152"/>
-      <c r="BB4" s="152"/>
-      <c r="BC4" s="152"/>
-      <c r="BD4" s="152"/>
-      <c r="BE4" s="152"/>
-      <c r="BF4" s="152"/>
-      <c r="BG4" s="152"/>
-      <c r="BH4" s="152"/>
-      <c r="BI4" s="152"/>
-      <c r="BJ4" s="152"/>
-      <c r="BK4" s="152"/>
-      <c r="BL4" s="152"/>
-      <c r="BM4" s="152"/>
-      <c r="BN4" s="152"/>
-      <c r="BO4" s="152"/>
-      <c r="BP4" s="152"/>
-      <c r="BQ4" s="152"/>
-      <c r="BR4" s="152"/>
-      <c r="BS4" s="152"/>
-      <c r="BT4" s="152"/>
-      <c r="BU4" s="152"/>
-      <c r="BV4" s="152"/>
-      <c r="BW4" s="152"/>
-      <c r="BX4" s="152"/>
-      <c r="BY4" s="152"/>
-      <c r="BZ4" s="152"/>
-      <c r="CA4" s="152" t="s">
+      <c r="AP4" s="145"/>
+      <c r="AQ4" s="145"/>
+      <c r="AR4" s="145"/>
+      <c r="AS4" s="145"/>
+      <c r="AT4" s="145"/>
+      <c r="AU4" s="145"/>
+      <c r="AV4" s="145"/>
+      <c r="AW4" s="145"/>
+      <c r="AX4" s="145"/>
+      <c r="AY4" s="145"/>
+      <c r="AZ4" s="145"/>
+      <c r="BA4" s="145"/>
+      <c r="BB4" s="145"/>
+      <c r="BC4" s="145"/>
+      <c r="BD4" s="145"/>
+      <c r="BE4" s="145"/>
+      <c r="BF4" s="145"/>
+      <c r="BG4" s="145"/>
+      <c r="BH4" s="145"/>
+      <c r="BI4" s="145"/>
+      <c r="BJ4" s="145"/>
+      <c r="BK4" s="145"/>
+      <c r="BL4" s="145"/>
+      <c r="BM4" s="145"/>
+      <c r="BN4" s="145"/>
+      <c r="BO4" s="145"/>
+      <c r="BP4" s="145"/>
+      <c r="BQ4" s="145"/>
+      <c r="BR4" s="145"/>
+      <c r="BS4" s="145"/>
+      <c r="BT4" s="145"/>
+      <c r="BU4" s="145"/>
+      <c r="BV4" s="145"/>
+      <c r="BW4" s="145"/>
+      <c r="BX4" s="145"/>
+      <c r="BY4" s="145"/>
+      <c r="BZ4" s="145"/>
+      <c r="CA4" s="145" t="s">
         <v>92</v>
       </c>
-      <c r="CB4" s="152"/>
-      <c r="CC4" s="152"/>
-      <c r="CD4" s="152"/>
-      <c r="CE4" s="152"/>
-      <c r="CF4" s="152"/>
-      <c r="CG4" s="152"/>
-      <c r="CH4" s="152"/>
-      <c r="CI4" s="152"/>
-      <c r="CJ4" s="152"/>
-      <c r="CK4" s="152"/>
-      <c r="CL4" s="152"/>
-      <c r="CM4" s="152"/>
-      <c r="CN4" s="152"/>
-      <c r="CO4" s="152"/>
-      <c r="CP4" s="152"/>
-      <c r="CQ4" s="152"/>
-      <c r="CR4" s="152"/>
-      <c r="CS4" s="152"/>
-      <c r="CT4" s="152"/>
-      <c r="CU4" s="152"/>
-      <c r="CV4" s="152" t="s">
+      <c r="CB4" s="145"/>
+      <c r="CC4" s="145"/>
+      <c r="CD4" s="145"/>
+      <c r="CE4" s="145"/>
+      <c r="CF4" s="145"/>
+      <c r="CG4" s="145"/>
+      <c r="CH4" s="145"/>
+      <c r="CI4" s="145"/>
+      <c r="CJ4" s="145"/>
+      <c r="CK4" s="145"/>
+      <c r="CL4" s="145"/>
+      <c r="CM4" s="145"/>
+      <c r="CN4" s="145"/>
+      <c r="CO4" s="145"/>
+      <c r="CP4" s="145"/>
+      <c r="CQ4" s="145"/>
+      <c r="CR4" s="145"/>
+      <c r="CS4" s="145"/>
+      <c r="CT4" s="145"/>
+      <c r="CU4" s="145"/>
+      <c r="CV4" s="145" t="s">
         <v>93</v>
       </c>
-      <c r="CW4" s="152"/>
-      <c r="CX4" s="152"/>
-      <c r="CY4" s="152"/>
-      <c r="CZ4" s="152"/>
-      <c r="DA4" s="152"/>
-      <c r="DB4" s="152"/>
-      <c r="DC4" s="152"/>
-      <c r="DD4" s="152"/>
-      <c r="DE4" s="152"/>
-      <c r="DF4" s="152"/>
-      <c r="DG4" s="152"/>
-      <c r="DH4" s="152"/>
-      <c r="DI4" s="152"/>
-      <c r="DJ4" s="152"/>
-      <c r="DK4" s="152"/>
-      <c r="DL4" s="152"/>
-      <c r="DM4" s="152"/>
-      <c r="DN4" s="152"/>
-      <c r="DO4" s="152"/>
-      <c r="DP4" s="152"/>
-      <c r="DQ4" s="152"/>
-      <c r="DR4" s="152"/>
-      <c r="DS4" s="152"/>
-      <c r="DT4" s="152"/>
-      <c r="DU4" s="152"/>
-      <c r="DV4" s="152"/>
-      <c r="DW4" s="152"/>
-      <c r="DX4" s="152"/>
-      <c r="DY4" s="152"/>
-      <c r="DZ4" s="152"/>
-      <c r="EA4" s="152"/>
-      <c r="EB4" s="152"/>
-      <c r="EC4" s="152"/>
-      <c r="ED4" s="152"/>
-      <c r="EE4" s="152" t="s">
+      <c r="CW4" s="145"/>
+      <c r="CX4" s="145"/>
+      <c r="CY4" s="145"/>
+      <c r="CZ4" s="145"/>
+      <c r="DA4" s="145"/>
+      <c r="DB4" s="145"/>
+      <c r="DC4" s="145"/>
+      <c r="DD4" s="145"/>
+      <c r="DE4" s="145"/>
+      <c r="DF4" s="145"/>
+      <c r="DG4" s="145"/>
+      <c r="DH4" s="145"/>
+      <c r="DI4" s="145"/>
+      <c r="DJ4" s="145"/>
+      <c r="DK4" s="145"/>
+      <c r="DL4" s="145"/>
+      <c r="DM4" s="145"/>
+      <c r="DN4" s="145"/>
+      <c r="DO4" s="145"/>
+      <c r="DP4" s="145"/>
+      <c r="DQ4" s="145"/>
+      <c r="DR4" s="145"/>
+      <c r="DS4" s="145"/>
+      <c r="DT4" s="145"/>
+      <c r="DU4" s="145"/>
+      <c r="DV4" s="145"/>
+      <c r="DW4" s="145"/>
+      <c r="DX4" s="145"/>
+      <c r="DY4" s="145"/>
+      <c r="DZ4" s="145"/>
+      <c r="EA4" s="145"/>
+      <c r="EB4" s="145"/>
+      <c r="EC4" s="145"/>
+      <c r="ED4" s="145"/>
+      <c r="EE4" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="EF4" s="152"/>
-      <c r="EG4" s="152"/>
-      <c r="EH4" s="152"/>
-      <c r="EI4" s="152"/>
-      <c r="EJ4" s="152"/>
-      <c r="EK4" s="152"/>
-      <c r="EL4" s="152"/>
-      <c r="EM4" s="152"/>
-      <c r="EN4" s="152"/>
-      <c r="EO4" s="152"/>
-      <c r="EP4" s="152"/>
-      <c r="EQ4" s="152"/>
-      <c r="ER4" s="152"/>
-      <c r="ES4" s="152"/>
-      <c r="ET4" s="152"/>
-      <c r="EU4" s="152"/>
-      <c r="EV4" s="152"/>
-      <c r="EW4" s="152"/>
-      <c r="EX4" s="152"/>
-      <c r="EY4" s="152"/>
-      <c r="EZ4" s="152"/>
-      <c r="FA4" s="152"/>
-      <c r="FB4" s="152"/>
-      <c r="FC4" s="152"/>
-      <c r="FD4" s="152"/>
-      <c r="FE4" s="152"/>
-      <c r="FF4" s="152"/>
-      <c r="FG4" s="152"/>
-      <c r="FH4" s="152"/>
-      <c r="FI4" s="152"/>
-      <c r="FJ4" s="152"/>
-      <c r="FK4" s="152"/>
-      <c r="FL4" s="152"/>
-      <c r="FM4" s="152" t="s">
+      <c r="EF4" s="145"/>
+      <c r="EG4" s="145"/>
+      <c r="EH4" s="145"/>
+      <c r="EI4" s="145"/>
+      <c r="EJ4" s="145"/>
+      <c r="EK4" s="145"/>
+      <c r="EL4" s="145"/>
+      <c r="EM4" s="145"/>
+      <c r="EN4" s="145"/>
+      <c r="EO4" s="145"/>
+      <c r="EP4" s="145"/>
+      <c r="EQ4" s="145"/>
+      <c r="ER4" s="145"/>
+      <c r="ES4" s="145"/>
+      <c r="ET4" s="145"/>
+      <c r="EU4" s="145"/>
+      <c r="EV4" s="145"/>
+      <c r="EW4" s="145"/>
+      <c r="EX4" s="145"/>
+      <c r="EY4" s="145"/>
+      <c r="EZ4" s="145"/>
+      <c r="FA4" s="145"/>
+      <c r="FB4" s="145"/>
+      <c r="FC4" s="145"/>
+      <c r="FD4" s="145"/>
+      <c r="FE4" s="145"/>
+      <c r="FF4" s="145"/>
+      <c r="FG4" s="145"/>
+      <c r="FH4" s="145"/>
+      <c r="FI4" s="145"/>
+      <c r="FJ4" s="145"/>
+      <c r="FK4" s="145"/>
+      <c r="FL4" s="145"/>
+      <c r="FM4" s="145" t="s">
         <v>91</v>
       </c>
-      <c r="FN4" s="152"/>
-      <c r="FO4" s="152"/>
-      <c r="FP4" s="152"/>
-      <c r="FQ4" s="152"/>
-      <c r="FR4" s="152"/>
-      <c r="FS4" s="152"/>
-      <c r="FT4" s="152"/>
-      <c r="FU4" s="152"/>
-      <c r="FV4" s="152"/>
-      <c r="FW4" s="152"/>
-      <c r="FX4" s="152"/>
-      <c r="FY4" s="152"/>
-      <c r="FZ4" s="152"/>
-      <c r="GA4" s="152"/>
-      <c r="GB4" s="152"/>
-      <c r="GC4" s="153"/>
+      <c r="FN4" s="145"/>
+      <c r="FO4" s="145"/>
+      <c r="FP4" s="145"/>
+      <c r="FQ4" s="145"/>
+      <c r="FR4" s="145"/>
+      <c r="FS4" s="145"/>
+      <c r="FT4" s="145"/>
+      <c r="FU4" s="145"/>
+      <c r="FV4" s="145"/>
+      <c r="FW4" s="145"/>
+      <c r="FX4" s="145"/>
+      <c r="FY4" s="145"/>
+      <c r="FZ4" s="145"/>
+      <c r="GA4" s="145"/>
+      <c r="GB4" s="145"/>
+      <c r="GC4" s="146"/>
     </row>
     <row r="5" spans="1:185" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="139"/>
+      <c r="B5" s="157"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="158"/>
       <c r="F5" s="149">
         <v>2016</v>
       </c>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="127"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
-      <c r="Q5" s="127"/>
-      <c r="R5" s="127"/>
-      <c r="S5" s="127"/>
-      <c r="T5" s="127"/>
-      <c r="U5" s="127"/>
-      <c r="V5" s="127"/>
-      <c r="W5" s="127"/>
-      <c r="X5" s="127"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
-      <c r="AA5" s="127"/>
-      <c r="AB5" s="127"/>
-      <c r="AC5" s="127"/>
-      <c r="AD5" s="127"/>
-      <c r="AE5" s="127"/>
-      <c r="AF5" s="127"/>
-      <c r="AG5" s="127"/>
-      <c r="AH5" s="127"/>
-      <c r="AI5" s="127"/>
-      <c r="AJ5" s="127"/>
-      <c r="AK5" s="127"/>
-      <c r="AL5" s="127"/>
-      <c r="AM5" s="127"/>
-      <c r="AN5" s="127"/>
-      <c r="AO5" s="127"/>
-      <c r="AP5" s="127"/>
-      <c r="AQ5" s="127"/>
-      <c r="AR5" s="127"/>
-      <c r="AS5" s="127"/>
-      <c r="AT5" s="127"/>
-      <c r="AU5" s="127"/>
-      <c r="AV5" s="127"/>
-      <c r="AW5" s="127"/>
-      <c r="AX5" s="127"/>
-      <c r="AY5" s="127"/>
-      <c r="AZ5" s="127"/>
-      <c r="BA5" s="127"/>
-      <c r="BB5" s="127"/>
-      <c r="BC5" s="127"/>
-      <c r="BD5" s="127"/>
-      <c r="BE5" s="127"/>
-      <c r="BF5" s="127"/>
-      <c r="BG5" s="127"/>
-      <c r="BH5" s="127"/>
-      <c r="BI5" s="127"/>
-      <c r="BJ5" s="127"/>
-      <c r="BK5" s="127"/>
-      <c r="BL5" s="127"/>
-      <c r="BM5" s="127"/>
-      <c r="BN5" s="127"/>
-      <c r="BO5" s="127"/>
-      <c r="BP5" s="127"/>
-      <c r="BQ5" s="127"/>
-      <c r="BR5" s="127"/>
-      <c r="BS5" s="127"/>
-      <c r="BT5" s="127"/>
-      <c r="BU5" s="127"/>
-      <c r="BV5" s="127"/>
-      <c r="BW5" s="127"/>
-      <c r="BX5" s="127"/>
-      <c r="BY5" s="127"/>
-      <c r="BZ5" s="127"/>
-      <c r="CA5" s="127"/>
-      <c r="CB5" s="127"/>
-      <c r="CC5" s="127"/>
-      <c r="CD5" s="127"/>
-      <c r="CE5" s="127"/>
-      <c r="CF5" s="127"/>
-      <c r="CG5" s="127"/>
-      <c r="CH5" s="127"/>
-      <c r="CI5" s="127"/>
-      <c r="CJ5" s="127"/>
-      <c r="CK5" s="127"/>
-      <c r="CL5" s="127"/>
-      <c r="CM5" s="127"/>
-      <c r="CN5" s="127"/>
-      <c r="CO5" s="127"/>
-      <c r="CP5" s="127"/>
-      <c r="CQ5" s="127"/>
-      <c r="CR5" s="127"/>
-      <c r="CS5" s="127"/>
-      <c r="CT5" s="127"/>
-      <c r="CU5" s="127"/>
-      <c r="CV5" s="127"/>
-      <c r="CW5" s="127"/>
-      <c r="CX5" s="127"/>
-      <c r="CY5" s="127"/>
-      <c r="CZ5" s="127"/>
-      <c r="DA5" s="127"/>
-      <c r="DB5" s="127"/>
-      <c r="DC5" s="127"/>
-      <c r="DD5" s="127"/>
-      <c r="DE5" s="127"/>
-      <c r="DF5" s="127">
+      <c r="G5" s="150"/>
+      <c r="H5" s="150"/>
+      <c r="I5" s="150"/>
+      <c r="J5" s="150"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="150"/>
+      <c r="O5" s="150"/>
+      <c r="P5" s="150"/>
+      <c r="Q5" s="150"/>
+      <c r="R5" s="150"/>
+      <c r="S5" s="150"/>
+      <c r="T5" s="150"/>
+      <c r="U5" s="150"/>
+      <c r="V5" s="150"/>
+      <c r="W5" s="150"/>
+      <c r="X5" s="150"/>
+      <c r="Y5" s="150"/>
+      <c r="Z5" s="150"/>
+      <c r="AA5" s="150"/>
+      <c r="AB5" s="150"/>
+      <c r="AC5" s="150"/>
+      <c r="AD5" s="150"/>
+      <c r="AE5" s="150"/>
+      <c r="AF5" s="150"/>
+      <c r="AG5" s="150"/>
+      <c r="AH5" s="150"/>
+      <c r="AI5" s="150"/>
+      <c r="AJ5" s="150"/>
+      <c r="AK5" s="150"/>
+      <c r="AL5" s="150"/>
+      <c r="AM5" s="150"/>
+      <c r="AN5" s="150"/>
+      <c r="AO5" s="150"/>
+      <c r="AP5" s="150"/>
+      <c r="AQ5" s="150"/>
+      <c r="AR5" s="150"/>
+      <c r="AS5" s="150"/>
+      <c r="AT5" s="150"/>
+      <c r="AU5" s="150"/>
+      <c r="AV5" s="150"/>
+      <c r="AW5" s="150"/>
+      <c r="AX5" s="150"/>
+      <c r="AY5" s="150"/>
+      <c r="AZ5" s="150"/>
+      <c r="BA5" s="150"/>
+      <c r="BB5" s="150"/>
+      <c r="BC5" s="150"/>
+      <c r="BD5" s="150"/>
+      <c r="BE5" s="150"/>
+      <c r="BF5" s="150"/>
+      <c r="BG5" s="150"/>
+      <c r="BH5" s="150"/>
+      <c r="BI5" s="150"/>
+      <c r="BJ5" s="150"/>
+      <c r="BK5" s="150"/>
+      <c r="BL5" s="150"/>
+      <c r="BM5" s="150"/>
+      <c r="BN5" s="150"/>
+      <c r="BO5" s="150"/>
+      <c r="BP5" s="150"/>
+      <c r="BQ5" s="150"/>
+      <c r="BR5" s="150"/>
+      <c r="BS5" s="150"/>
+      <c r="BT5" s="150"/>
+      <c r="BU5" s="150"/>
+      <c r="BV5" s="150"/>
+      <c r="BW5" s="150"/>
+      <c r="BX5" s="150"/>
+      <c r="BY5" s="150"/>
+      <c r="BZ5" s="150"/>
+      <c r="CA5" s="150"/>
+      <c r="CB5" s="150"/>
+      <c r="CC5" s="150"/>
+      <c r="CD5" s="150"/>
+      <c r="CE5" s="150"/>
+      <c r="CF5" s="150"/>
+      <c r="CG5" s="150"/>
+      <c r="CH5" s="150"/>
+      <c r="CI5" s="150"/>
+      <c r="CJ5" s="150"/>
+      <c r="CK5" s="150"/>
+      <c r="CL5" s="150"/>
+      <c r="CM5" s="150"/>
+      <c r="CN5" s="150"/>
+      <c r="CO5" s="150"/>
+      <c r="CP5" s="150"/>
+      <c r="CQ5" s="150"/>
+      <c r="CR5" s="150"/>
+      <c r="CS5" s="150"/>
+      <c r="CT5" s="150"/>
+      <c r="CU5" s="150"/>
+      <c r="CV5" s="150"/>
+      <c r="CW5" s="150"/>
+      <c r="CX5" s="150"/>
+      <c r="CY5" s="150"/>
+      <c r="CZ5" s="150"/>
+      <c r="DA5" s="150"/>
+      <c r="DB5" s="150"/>
+      <c r="DC5" s="150"/>
+      <c r="DD5" s="150"/>
+      <c r="DE5" s="150"/>
+      <c r="DF5" s="150">
         <v>2017</v>
       </c>
-      <c r="DG5" s="127"/>
-      <c r="DH5" s="127"/>
-      <c r="DI5" s="127"/>
-      <c r="DJ5" s="127"/>
-      <c r="DK5" s="127"/>
-      <c r="DL5" s="127"/>
-      <c r="DM5" s="127"/>
-      <c r="DN5" s="127"/>
-      <c r="DO5" s="127"/>
-      <c r="DP5" s="127"/>
-      <c r="DQ5" s="127"/>
-      <c r="DR5" s="127"/>
-      <c r="DS5" s="127"/>
-      <c r="DT5" s="127"/>
-      <c r="DU5" s="127"/>
-      <c r="DV5" s="127"/>
-      <c r="DW5" s="127"/>
-      <c r="DX5" s="127"/>
-      <c r="DY5" s="127"/>
-      <c r="DZ5" s="127"/>
-      <c r="EA5" s="127"/>
-      <c r="EB5" s="127"/>
-      <c r="EC5" s="127"/>
-      <c r="ED5" s="127"/>
-      <c r="EE5" s="127"/>
-      <c r="EF5" s="127"/>
-      <c r="EG5" s="127"/>
-      <c r="EH5" s="127"/>
-      <c r="EI5" s="127"/>
-      <c r="EJ5" s="127"/>
-      <c r="EK5" s="127"/>
-      <c r="EL5" s="127"/>
-      <c r="EM5" s="127"/>
-      <c r="EN5" s="127"/>
-      <c r="EO5" s="127"/>
-      <c r="EP5" s="127"/>
-      <c r="EQ5" s="127"/>
-      <c r="ER5" s="127"/>
-      <c r="ES5" s="127"/>
-      <c r="ET5" s="127"/>
-      <c r="EU5" s="127"/>
-      <c r="EV5" s="127"/>
-      <c r="EW5" s="127"/>
-      <c r="EX5" s="127"/>
-      <c r="EY5" s="127"/>
-      <c r="EZ5" s="127"/>
-      <c r="FA5" s="127"/>
-      <c r="FB5" s="127"/>
-      <c r="FC5" s="127"/>
-      <c r="FD5" s="127"/>
-      <c r="FE5" s="127"/>
-      <c r="FF5" s="127"/>
-      <c r="FG5" s="127"/>
-      <c r="FH5" s="127"/>
-      <c r="FI5" s="127"/>
-      <c r="FJ5" s="127"/>
-      <c r="FK5" s="127"/>
-      <c r="FL5" s="127"/>
-      <c r="FM5" s="127"/>
-      <c r="FN5" s="127"/>
-      <c r="FO5" s="127"/>
-      <c r="FP5" s="127"/>
-      <c r="FQ5" s="127"/>
-      <c r="FR5" s="127"/>
-      <c r="FS5" s="127"/>
-      <c r="FT5" s="127"/>
-      <c r="FU5" s="127"/>
-      <c r="FV5" s="127"/>
-      <c r="FW5" s="127"/>
-      <c r="FX5" s="127"/>
-      <c r="FY5" s="127"/>
-      <c r="FZ5" s="127"/>
-      <c r="GA5" s="127"/>
-      <c r="GB5" s="127"/>
-      <c r="GC5" s="128"/>
+      <c r="DG5" s="150"/>
+      <c r="DH5" s="150"/>
+      <c r="DI5" s="150"/>
+      <c r="DJ5" s="150"/>
+      <c r="DK5" s="150"/>
+      <c r="DL5" s="150"/>
+      <c r="DM5" s="150"/>
+      <c r="DN5" s="150"/>
+      <c r="DO5" s="150"/>
+      <c r="DP5" s="150"/>
+      <c r="DQ5" s="150"/>
+      <c r="DR5" s="150"/>
+      <c r="DS5" s="150"/>
+      <c r="DT5" s="150"/>
+      <c r="DU5" s="150"/>
+      <c r="DV5" s="150"/>
+      <c r="DW5" s="150"/>
+      <c r="DX5" s="150"/>
+      <c r="DY5" s="150"/>
+      <c r="DZ5" s="150"/>
+      <c r="EA5" s="150"/>
+      <c r="EB5" s="150"/>
+      <c r="EC5" s="150"/>
+      <c r="ED5" s="150"/>
+      <c r="EE5" s="150"/>
+      <c r="EF5" s="150"/>
+      <c r="EG5" s="150"/>
+      <c r="EH5" s="150"/>
+      <c r="EI5" s="150"/>
+      <c r="EJ5" s="150"/>
+      <c r="EK5" s="150"/>
+      <c r="EL5" s="150"/>
+      <c r="EM5" s="150"/>
+      <c r="EN5" s="150"/>
+      <c r="EO5" s="150"/>
+      <c r="EP5" s="150"/>
+      <c r="EQ5" s="150"/>
+      <c r="ER5" s="150"/>
+      <c r="ES5" s="150"/>
+      <c r="ET5" s="150"/>
+      <c r="EU5" s="150"/>
+      <c r="EV5" s="150"/>
+      <c r="EW5" s="150"/>
+      <c r="EX5" s="150"/>
+      <c r="EY5" s="150"/>
+      <c r="EZ5" s="150"/>
+      <c r="FA5" s="150"/>
+      <c r="FB5" s="150"/>
+      <c r="FC5" s="150"/>
+      <c r="FD5" s="150"/>
+      <c r="FE5" s="150"/>
+      <c r="FF5" s="150"/>
+      <c r="FG5" s="150"/>
+      <c r="FH5" s="150"/>
+      <c r="FI5" s="150"/>
+      <c r="FJ5" s="150"/>
+      <c r="FK5" s="150"/>
+      <c r="FL5" s="150"/>
+      <c r="FM5" s="150"/>
+      <c r="FN5" s="150"/>
+      <c r="FO5" s="150"/>
+      <c r="FP5" s="150"/>
+      <c r="FQ5" s="150"/>
+      <c r="FR5" s="150"/>
+      <c r="FS5" s="150"/>
+      <c r="FT5" s="150"/>
+      <c r="FU5" s="150"/>
+      <c r="FV5" s="150"/>
+      <c r="FW5" s="150"/>
+      <c r="FX5" s="150"/>
+      <c r="FY5" s="150"/>
+      <c r="FZ5" s="150"/>
+      <c r="GA5" s="150"/>
+      <c r="GB5" s="150"/>
+      <c r="GC5" s="172"/>
     </row>
     <row r="6" spans="1:185" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="140" t="s">
+      <c r="A6" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="141"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="150" t="s">
+      <c r="B6" s="166"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="166"/>
+      <c r="E6" s="167"/>
+      <c r="F6" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="125"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="125"/>
-      <c r="K6" s="125"/>
-      <c r="L6" s="125"/>
-      <c r="M6" s="125"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="125"/>
-      <c r="P6" s="125"/>
-      <c r="Q6" s="125"/>
-      <c r="R6" s="125" t="s">
+      <c r="G6" s="148"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="148"/>
+      <c r="Q6" s="148"/>
+      <c r="R6" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="S6" s="125"/>
-      <c r="T6" s="125"/>
-      <c r="U6" s="125"/>
-      <c r="V6" s="125"/>
-      <c r="W6" s="125"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="125"/>
-      <c r="Z6" s="125"/>
-      <c r="AA6" s="125"/>
-      <c r="AB6" s="125"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="125"/>
-      <c r="AE6" s="125"/>
-      <c r="AF6" s="125"/>
-      <c r="AG6" s="125"/>
-      <c r="AH6" s="125"/>
-      <c r="AI6" s="125"/>
-      <c r="AJ6" s="125"/>
-      <c r="AK6" s="125"/>
-      <c r="AL6" s="125"/>
-      <c r="AM6" s="125"/>
-      <c r="AN6" s="125"/>
-      <c r="AO6" s="125"/>
-      <c r="AP6" s="125"/>
-      <c r="AQ6" s="125"/>
-      <c r="AR6" s="125"/>
-      <c r="AS6" s="125"/>
-      <c r="AT6" s="125"/>
-      <c r="AU6" s="125"/>
-      <c r="AV6" s="125"/>
-      <c r="AW6" s="125" t="s">
+      <c r="S6" s="148"/>
+      <c r="T6" s="148"/>
+      <c r="U6" s="148"/>
+      <c r="V6" s="148"/>
+      <c r="W6" s="148"/>
+      <c r="X6" s="148"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="148"/>
+      <c r="AA6" s="148"/>
+      <c r="AB6" s="148"/>
+      <c r="AC6" s="148"/>
+      <c r="AD6" s="148"/>
+      <c r="AE6" s="148"/>
+      <c r="AF6" s="148"/>
+      <c r="AG6" s="148"/>
+      <c r="AH6" s="148"/>
+      <c r="AI6" s="148"/>
+      <c r="AJ6" s="148"/>
+      <c r="AK6" s="148"/>
+      <c r="AL6" s="148"/>
+      <c r="AM6" s="148"/>
+      <c r="AN6" s="148"/>
+      <c r="AO6" s="148"/>
+      <c r="AP6" s="148"/>
+      <c r="AQ6" s="148"/>
+      <c r="AR6" s="148"/>
+      <c r="AS6" s="148"/>
+      <c r="AT6" s="148"/>
+      <c r="AU6" s="148"/>
+      <c r="AV6" s="148"/>
+      <c r="AW6" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="AX6" s="125"/>
-      <c r="AY6" s="125"/>
-      <c r="AZ6" s="125"/>
-      <c r="BA6" s="125"/>
-      <c r="BB6" s="125"/>
-      <c r="BC6" s="125"/>
-      <c r="BD6" s="125"/>
-      <c r="BE6" s="125"/>
-      <c r="BF6" s="125"/>
-      <c r="BG6" s="125"/>
-      <c r="BH6" s="125"/>
-      <c r="BI6" s="125"/>
-      <c r="BJ6" s="125"/>
-      <c r="BK6" s="125"/>
-      <c r="BL6" s="125"/>
-      <c r="BM6" s="125"/>
-      <c r="BN6" s="125"/>
-      <c r="BO6" s="125"/>
-      <c r="BP6" s="125"/>
-      <c r="BQ6" s="125"/>
-      <c r="BR6" s="125"/>
-      <c r="BS6" s="125"/>
-      <c r="BT6" s="125"/>
-      <c r="BU6" s="125"/>
-      <c r="BV6" s="125"/>
-      <c r="BW6" s="125"/>
-      <c r="BX6" s="125"/>
-      <c r="BY6" s="125"/>
-      <c r="BZ6" s="125"/>
-      <c r="CA6" s="125" t="s">
+      <c r="AX6" s="148"/>
+      <c r="AY6" s="148"/>
+      <c r="AZ6" s="148"/>
+      <c r="BA6" s="148"/>
+      <c r="BB6" s="148"/>
+      <c r="BC6" s="148"/>
+      <c r="BD6" s="148"/>
+      <c r="BE6" s="148"/>
+      <c r="BF6" s="148"/>
+      <c r="BG6" s="148"/>
+      <c r="BH6" s="148"/>
+      <c r="BI6" s="148"/>
+      <c r="BJ6" s="148"/>
+      <c r="BK6" s="148"/>
+      <c r="BL6" s="148"/>
+      <c r="BM6" s="148"/>
+      <c r="BN6" s="148"/>
+      <c r="BO6" s="148"/>
+      <c r="BP6" s="148"/>
+      <c r="BQ6" s="148"/>
+      <c r="BR6" s="148"/>
+      <c r="BS6" s="148"/>
+      <c r="BT6" s="148"/>
+      <c r="BU6" s="148"/>
+      <c r="BV6" s="148"/>
+      <c r="BW6" s="148"/>
+      <c r="BX6" s="148"/>
+      <c r="BY6" s="148"/>
+      <c r="BZ6" s="148"/>
+      <c r="CA6" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="CB6" s="125"/>
-      <c r="CC6" s="125"/>
-      <c r="CD6" s="125"/>
-      <c r="CE6" s="125"/>
-      <c r="CF6" s="125"/>
-      <c r="CG6" s="125"/>
-      <c r="CH6" s="125"/>
-      <c r="CI6" s="125"/>
-      <c r="CJ6" s="125"/>
-      <c r="CK6" s="125"/>
-      <c r="CL6" s="125"/>
-      <c r="CM6" s="125"/>
-      <c r="CN6" s="125"/>
-      <c r="CO6" s="125"/>
-      <c r="CP6" s="125"/>
-      <c r="CQ6" s="125"/>
-      <c r="CR6" s="125"/>
-      <c r="CS6" s="125"/>
-      <c r="CT6" s="125"/>
-      <c r="CU6" s="125"/>
-      <c r="CV6" s="125"/>
-      <c r="CW6" s="125"/>
-      <c r="CX6" s="125"/>
-      <c r="CY6" s="125"/>
-      <c r="CZ6" s="125"/>
-      <c r="DA6" s="125"/>
-      <c r="DB6" s="125"/>
-      <c r="DC6" s="125"/>
-      <c r="DD6" s="125"/>
-      <c r="DE6" s="125"/>
-      <c r="DF6" s="125" t="s">
+      <c r="CB6" s="148"/>
+      <c r="CC6" s="148"/>
+      <c r="CD6" s="148"/>
+      <c r="CE6" s="148"/>
+      <c r="CF6" s="148"/>
+      <c r="CG6" s="148"/>
+      <c r="CH6" s="148"/>
+      <c r="CI6" s="148"/>
+      <c r="CJ6" s="148"/>
+      <c r="CK6" s="148"/>
+      <c r="CL6" s="148"/>
+      <c r="CM6" s="148"/>
+      <c r="CN6" s="148"/>
+      <c r="CO6" s="148"/>
+      <c r="CP6" s="148"/>
+      <c r="CQ6" s="148"/>
+      <c r="CR6" s="148"/>
+      <c r="CS6" s="148"/>
+      <c r="CT6" s="148"/>
+      <c r="CU6" s="148"/>
+      <c r="CV6" s="148"/>
+      <c r="CW6" s="148"/>
+      <c r="CX6" s="148"/>
+      <c r="CY6" s="148"/>
+      <c r="CZ6" s="148"/>
+      <c r="DA6" s="148"/>
+      <c r="DB6" s="148"/>
+      <c r="DC6" s="148"/>
+      <c r="DD6" s="148"/>
+      <c r="DE6" s="148"/>
+      <c r="DF6" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="DG6" s="125"/>
-      <c r="DH6" s="125"/>
-      <c r="DI6" s="125"/>
-      <c r="DJ6" s="125"/>
-      <c r="DK6" s="125"/>
-      <c r="DL6" s="125"/>
-      <c r="DM6" s="125"/>
-      <c r="DN6" s="125"/>
-      <c r="DO6" s="125"/>
-      <c r="DP6" s="125"/>
-      <c r="DQ6" s="125"/>
-      <c r="DR6" s="125"/>
-      <c r="DS6" s="125"/>
-      <c r="DT6" s="125"/>
-      <c r="DU6" s="125"/>
-      <c r="DV6" s="125"/>
-      <c r="DW6" s="125"/>
-      <c r="DX6" s="125"/>
-      <c r="DY6" s="125"/>
-      <c r="DZ6" s="125"/>
-      <c r="EA6" s="125"/>
-      <c r="EB6" s="125"/>
-      <c r="EC6" s="125"/>
-      <c r="ED6" s="125"/>
-      <c r="EE6" s="125"/>
-      <c r="EF6" s="125"/>
-      <c r="EG6" s="125"/>
-      <c r="EH6" s="125"/>
-      <c r="EI6" s="125"/>
-      <c r="EJ6" s="125"/>
-      <c r="EK6" s="125" t="s">
+      <c r="DG6" s="148"/>
+      <c r="DH6" s="148"/>
+      <c r="DI6" s="148"/>
+      <c r="DJ6" s="148"/>
+      <c r="DK6" s="148"/>
+      <c r="DL6" s="148"/>
+      <c r="DM6" s="148"/>
+      <c r="DN6" s="148"/>
+      <c r="DO6" s="148"/>
+      <c r="DP6" s="148"/>
+      <c r="DQ6" s="148"/>
+      <c r="DR6" s="148"/>
+      <c r="DS6" s="148"/>
+      <c r="DT6" s="148"/>
+      <c r="DU6" s="148"/>
+      <c r="DV6" s="148"/>
+      <c r="DW6" s="148"/>
+      <c r="DX6" s="148"/>
+      <c r="DY6" s="148"/>
+      <c r="DZ6" s="148"/>
+      <c r="EA6" s="148"/>
+      <c r="EB6" s="148"/>
+      <c r="EC6" s="148"/>
+      <c r="ED6" s="148"/>
+      <c r="EE6" s="148"/>
+      <c r="EF6" s="148"/>
+      <c r="EG6" s="148"/>
+      <c r="EH6" s="148"/>
+      <c r="EI6" s="148"/>
+      <c r="EJ6" s="148"/>
+      <c r="EK6" s="148" t="s">
         <v>50</v>
       </c>
-      <c r="EL6" s="125"/>
-      <c r="EM6" s="125"/>
-      <c r="EN6" s="125"/>
-      <c r="EO6" s="125"/>
-      <c r="EP6" s="125"/>
-      <c r="EQ6" s="125"/>
-      <c r="ER6" s="125"/>
-      <c r="ES6" s="125"/>
-      <c r="ET6" s="125"/>
-      <c r="EU6" s="125"/>
-      <c r="EV6" s="125"/>
-      <c r="EW6" s="125"/>
-      <c r="EX6" s="125"/>
-      <c r="EY6" s="125"/>
-      <c r="EZ6" s="125"/>
-      <c r="FA6" s="125"/>
-      <c r="FB6" s="125"/>
-      <c r="FC6" s="125"/>
-      <c r="FD6" s="125"/>
-      <c r="FE6" s="125"/>
-      <c r="FF6" s="125"/>
-      <c r="FG6" s="125"/>
-      <c r="FH6" s="125"/>
-      <c r="FI6" s="125"/>
-      <c r="FJ6" s="125"/>
-      <c r="FK6" s="125"/>
-      <c r="FL6" s="125"/>
-      <c r="FM6" s="125" t="s">
+      <c r="EL6" s="148"/>
+      <c r="EM6" s="148"/>
+      <c r="EN6" s="148"/>
+      <c r="EO6" s="148"/>
+      <c r="EP6" s="148"/>
+      <c r="EQ6" s="148"/>
+      <c r="ER6" s="148"/>
+      <c r="ES6" s="148"/>
+      <c r="ET6" s="148"/>
+      <c r="EU6" s="148"/>
+      <c r="EV6" s="148"/>
+      <c r="EW6" s="148"/>
+      <c r="EX6" s="148"/>
+      <c r="EY6" s="148"/>
+      <c r="EZ6" s="148"/>
+      <c r="FA6" s="148"/>
+      <c r="FB6" s="148"/>
+      <c r="FC6" s="148"/>
+      <c r="FD6" s="148"/>
+      <c r="FE6" s="148"/>
+      <c r="FF6" s="148"/>
+      <c r="FG6" s="148"/>
+      <c r="FH6" s="148"/>
+      <c r="FI6" s="148"/>
+      <c r="FJ6" s="148"/>
+      <c r="FK6" s="148"/>
+      <c r="FL6" s="148"/>
+      <c r="FM6" s="148" t="s">
         <v>51</v>
       </c>
-      <c r="FN6" s="125"/>
-      <c r="FO6" s="125"/>
-      <c r="FP6" s="125"/>
-      <c r="FQ6" s="125"/>
-      <c r="FR6" s="125"/>
-      <c r="FS6" s="125"/>
-      <c r="FT6" s="125"/>
-      <c r="FU6" s="125"/>
-      <c r="FV6" s="125"/>
-      <c r="FW6" s="125"/>
-      <c r="FX6" s="125"/>
-      <c r="FY6" s="125"/>
-      <c r="FZ6" s="125"/>
-      <c r="GA6" s="125"/>
-      <c r="GB6" s="125"/>
-      <c r="GC6" s="126"/>
+      <c r="FN6" s="148"/>
+      <c r="FO6" s="148"/>
+      <c r="FP6" s="148"/>
+      <c r="FQ6" s="148"/>
+      <c r="FR6" s="148"/>
+      <c r="FS6" s="148"/>
+      <c r="FT6" s="148"/>
+      <c r="FU6" s="148"/>
+      <c r="FV6" s="148"/>
+      <c r="FW6" s="148"/>
+      <c r="FX6" s="148"/>
+      <c r="FY6" s="148"/>
+      <c r="FZ6" s="148"/>
+      <c r="GA6" s="148"/>
+      <c r="GB6" s="148"/>
+      <c r="GC6" s="171"/>
     </row>
     <row r="7" spans="1:185" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="137" t="s">
+      <c r="A7" s="156" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="139"/>
+      <c r="B7" s="157"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157"/>
+      <c r="E7" s="158"/>
       <c r="F7" s="149" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="127"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="127"/>
-      <c r="J7" s="127"/>
-      <c r="K7" s="127"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="129" t="s">
+      <c r="G7" s="150"/>
+      <c r="H7" s="150"/>
+      <c r="I7" s="150"/>
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="155"/>
+      <c r="M7" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="127"/>
-      <c r="O7" s="127"/>
-      <c r="P7" s="127"/>
-      <c r="Q7" s="127"/>
-      <c r="R7" s="127"/>
-      <c r="S7" s="130"/>
-      <c r="T7" s="129" t="s">
+      <c r="N7" s="150"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="150"/>
+      <c r="Q7" s="150"/>
+      <c r="R7" s="150"/>
+      <c r="S7" s="155"/>
+      <c r="T7" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="127"/>
-      <c r="V7" s="127"/>
-      <c r="W7" s="127"/>
-      <c r="X7" s="127"/>
-      <c r="Y7" s="127"/>
-      <c r="Z7" s="130"/>
-      <c r="AA7" s="129" t="s">
+      <c r="U7" s="150"/>
+      <c r="V7" s="150"/>
+      <c r="W7" s="150"/>
+      <c r="X7" s="150"/>
+      <c r="Y7" s="150"/>
+      <c r="Z7" s="155"/>
+      <c r="AA7" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="AB7" s="127"/>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="127"/>
-      <c r="AE7" s="127"/>
-      <c r="AF7" s="127"/>
-      <c r="AG7" s="130"/>
-      <c r="AH7" s="129" t="s">
+      <c r="AB7" s="150"/>
+      <c r="AC7" s="150"/>
+      <c r="AD7" s="150"/>
+      <c r="AE7" s="150"/>
+      <c r="AF7" s="150"/>
+      <c r="AG7" s="155"/>
+      <c r="AH7" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="AI7" s="127"/>
-      <c r="AJ7" s="127"/>
-      <c r="AK7" s="127"/>
-      <c r="AL7" s="127"/>
-      <c r="AM7" s="127"/>
-      <c r="AN7" s="130"/>
-      <c r="AO7" s="129" t="s">
+      <c r="AI7" s="150"/>
+      <c r="AJ7" s="150"/>
+      <c r="AK7" s="150"/>
+      <c r="AL7" s="150"/>
+      <c r="AM7" s="150"/>
+      <c r="AN7" s="155"/>
+      <c r="AO7" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="AP7" s="127"/>
-      <c r="AQ7" s="127"/>
-      <c r="AR7" s="127"/>
-      <c r="AS7" s="127"/>
-      <c r="AT7" s="127"/>
-      <c r="AU7" s="130"/>
-      <c r="AV7" s="129" t="s">
+      <c r="AP7" s="150"/>
+      <c r="AQ7" s="150"/>
+      <c r="AR7" s="150"/>
+      <c r="AS7" s="150"/>
+      <c r="AT7" s="150"/>
+      <c r="AU7" s="155"/>
+      <c r="AV7" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="AW7" s="127"/>
-      <c r="AX7" s="127"/>
-      <c r="AY7" s="127"/>
-      <c r="AZ7" s="127"/>
-      <c r="BA7" s="127"/>
-      <c r="BB7" s="130"/>
-      <c r="BC7" s="129" t="s">
+      <c r="AW7" s="150"/>
+      <c r="AX7" s="150"/>
+      <c r="AY7" s="150"/>
+      <c r="AZ7" s="150"/>
+      <c r="BA7" s="150"/>
+      <c r="BB7" s="155"/>
+      <c r="BC7" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="BD7" s="127"/>
-      <c r="BE7" s="127"/>
-      <c r="BF7" s="127"/>
-      <c r="BG7" s="127"/>
-      <c r="BH7" s="127"/>
-      <c r="BI7" s="130"/>
-      <c r="BJ7" s="129" t="s">
+      <c r="BD7" s="150"/>
+      <c r="BE7" s="150"/>
+      <c r="BF7" s="150"/>
+      <c r="BG7" s="150"/>
+      <c r="BH7" s="150"/>
+      <c r="BI7" s="155"/>
+      <c r="BJ7" s="154" t="s">
         <v>13</v>
       </c>
-      <c r="BK7" s="127"/>
-      <c r="BL7" s="127"/>
-      <c r="BM7" s="127"/>
-      <c r="BN7" s="127"/>
-      <c r="BO7" s="127"/>
-      <c r="BP7" s="130"/>
-      <c r="BQ7" s="129" t="s">
+      <c r="BK7" s="150"/>
+      <c r="BL7" s="150"/>
+      <c r="BM7" s="150"/>
+      <c r="BN7" s="150"/>
+      <c r="BO7" s="150"/>
+      <c r="BP7" s="155"/>
+      <c r="BQ7" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="BR7" s="127"/>
-      <c r="BS7" s="127"/>
-      <c r="BT7" s="127"/>
-      <c r="BU7" s="127"/>
-      <c r="BV7" s="127"/>
-      <c r="BW7" s="130"/>
-      <c r="BX7" s="129" t="s">
+      <c r="BR7" s="150"/>
+      <c r="BS7" s="150"/>
+      <c r="BT7" s="150"/>
+      <c r="BU7" s="150"/>
+      <c r="BV7" s="150"/>
+      <c r="BW7" s="155"/>
+      <c r="BX7" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="BY7" s="127"/>
-      <c r="BZ7" s="127"/>
-      <c r="CA7" s="127"/>
-      <c r="CB7" s="127"/>
-      <c r="CC7" s="127"/>
-      <c r="CD7" s="130"/>
-      <c r="CE7" s="129" t="s">
+      <c r="BY7" s="150"/>
+      <c r="BZ7" s="150"/>
+      <c r="CA7" s="150"/>
+      <c r="CB7" s="150"/>
+      <c r="CC7" s="150"/>
+      <c r="CD7" s="155"/>
+      <c r="CE7" s="154" t="s">
         <v>16</v>
       </c>
-      <c r="CF7" s="127"/>
-      <c r="CG7" s="127"/>
-      <c r="CH7" s="127"/>
-      <c r="CI7" s="127"/>
-      <c r="CJ7" s="127"/>
-      <c r="CK7" s="130"/>
-      <c r="CL7" s="129" t="s">
+      <c r="CF7" s="150"/>
+      <c r="CG7" s="150"/>
+      <c r="CH7" s="150"/>
+      <c r="CI7" s="150"/>
+      <c r="CJ7" s="150"/>
+      <c r="CK7" s="155"/>
+      <c r="CL7" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="CM7" s="127"/>
-      <c r="CN7" s="127"/>
-      <c r="CO7" s="127"/>
-      <c r="CP7" s="127"/>
-      <c r="CQ7" s="127"/>
-      <c r="CR7" s="130"/>
-      <c r="CS7" s="129" t="s">
+      <c r="CM7" s="150"/>
+      <c r="CN7" s="150"/>
+      <c r="CO7" s="150"/>
+      <c r="CP7" s="150"/>
+      <c r="CQ7" s="150"/>
+      <c r="CR7" s="155"/>
+      <c r="CS7" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="CT7" s="127"/>
-      <c r="CU7" s="127"/>
-      <c r="CV7" s="127"/>
-      <c r="CW7" s="127"/>
-      <c r="CX7" s="127"/>
-      <c r="CY7" s="130"/>
-      <c r="CZ7" s="129" t="s">
+      <c r="CT7" s="150"/>
+      <c r="CU7" s="150"/>
+      <c r="CV7" s="150"/>
+      <c r="CW7" s="150"/>
+      <c r="CX7" s="150"/>
+      <c r="CY7" s="155"/>
+      <c r="CZ7" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="DA7" s="127"/>
-      <c r="DB7" s="127"/>
-      <c r="DC7" s="127"/>
-      <c r="DD7" s="127"/>
-      <c r="DE7" s="127"/>
-      <c r="DF7" s="127"/>
-      <c r="DG7" s="129" t="s">
+      <c r="DA7" s="150"/>
+      <c r="DB7" s="150"/>
+      <c r="DC7" s="150"/>
+      <c r="DD7" s="150"/>
+      <c r="DE7" s="150"/>
+      <c r="DF7" s="150"/>
+      <c r="DG7" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="DH7" s="127"/>
-      <c r="DI7" s="127"/>
-      <c r="DJ7" s="127"/>
-      <c r="DK7" s="127"/>
-      <c r="DL7" s="127"/>
-      <c r="DM7" s="130"/>
-      <c r="DN7" s="127" t="s">
+      <c r="DH7" s="150"/>
+      <c r="DI7" s="150"/>
+      <c r="DJ7" s="150"/>
+      <c r="DK7" s="150"/>
+      <c r="DL7" s="150"/>
+      <c r="DM7" s="155"/>
+      <c r="DN7" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="DO7" s="127"/>
-      <c r="DP7" s="127"/>
-      <c r="DQ7" s="127"/>
-      <c r="DR7" s="127"/>
-      <c r="DS7" s="127"/>
-      <c r="DT7" s="127"/>
-      <c r="DU7" s="129" t="s">
+      <c r="DO7" s="150"/>
+      <c r="DP7" s="150"/>
+      <c r="DQ7" s="150"/>
+      <c r="DR7" s="150"/>
+      <c r="DS7" s="150"/>
+      <c r="DT7" s="150"/>
+      <c r="DU7" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="DV7" s="127"/>
-      <c r="DW7" s="127"/>
-      <c r="DX7" s="127"/>
-      <c r="DY7" s="127"/>
-      <c r="DZ7" s="127"/>
-      <c r="EA7" s="130"/>
-      <c r="EB7" s="127" t="s">
+      <c r="DV7" s="150"/>
+      <c r="DW7" s="150"/>
+      <c r="DX7" s="150"/>
+      <c r="DY7" s="150"/>
+      <c r="DZ7" s="150"/>
+      <c r="EA7" s="155"/>
+      <c r="EB7" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="EC7" s="127"/>
-      <c r="ED7" s="127"/>
-      <c r="EE7" s="127"/>
-      <c r="EF7" s="127"/>
-      <c r="EG7" s="127"/>
-      <c r="EH7" s="127"/>
-      <c r="EI7" s="129" t="s">
+      <c r="EC7" s="150"/>
+      <c r="ED7" s="150"/>
+      <c r="EE7" s="150"/>
+      <c r="EF7" s="150"/>
+      <c r="EG7" s="150"/>
+      <c r="EH7" s="150"/>
+      <c r="EI7" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="EJ7" s="127"/>
-      <c r="EK7" s="127"/>
-      <c r="EL7" s="127"/>
-      <c r="EM7" s="127"/>
-      <c r="EN7" s="127"/>
-      <c r="EO7" s="130"/>
-      <c r="EP7" s="127" t="s">
+      <c r="EJ7" s="150"/>
+      <c r="EK7" s="150"/>
+      <c r="EL7" s="150"/>
+      <c r="EM7" s="150"/>
+      <c r="EN7" s="150"/>
+      <c r="EO7" s="155"/>
+      <c r="EP7" s="150" t="s">
         <v>55</v>
       </c>
-      <c r="EQ7" s="127"/>
-      <c r="ER7" s="127"/>
-      <c r="ES7" s="127"/>
-      <c r="ET7" s="127"/>
-      <c r="EU7" s="127"/>
-      <c r="EV7" s="127"/>
-      <c r="EW7" s="129" t="s">
+      <c r="EQ7" s="150"/>
+      <c r="ER7" s="150"/>
+      <c r="ES7" s="150"/>
+      <c r="ET7" s="150"/>
+      <c r="EU7" s="150"/>
+      <c r="EV7" s="150"/>
+      <c r="EW7" s="154" t="s">
         <v>56</v>
       </c>
-      <c r="EX7" s="127"/>
-      <c r="EY7" s="127"/>
-      <c r="EZ7" s="127"/>
-      <c r="FA7" s="127"/>
-      <c r="FB7" s="127"/>
-      <c r="FC7" s="130"/>
-      <c r="FD7" s="127" t="s">
+      <c r="EX7" s="150"/>
+      <c r="EY7" s="150"/>
+      <c r="EZ7" s="150"/>
+      <c r="FA7" s="150"/>
+      <c r="FB7" s="150"/>
+      <c r="FC7" s="155"/>
+      <c r="FD7" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="FE7" s="127"/>
-      <c r="FF7" s="127"/>
-      <c r="FG7" s="127"/>
-      <c r="FH7" s="127"/>
-      <c r="FI7" s="127"/>
-      <c r="FJ7" s="127"/>
-      <c r="FK7" s="129" t="s">
+      <c r="FE7" s="150"/>
+      <c r="FF7" s="150"/>
+      <c r="FG7" s="150"/>
+      <c r="FH7" s="150"/>
+      <c r="FI7" s="150"/>
+      <c r="FJ7" s="150"/>
+      <c r="FK7" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="FL7" s="127"/>
-      <c r="FM7" s="127"/>
-      <c r="FN7" s="127"/>
-      <c r="FO7" s="127"/>
-      <c r="FP7" s="127"/>
-      <c r="FQ7" s="130"/>
-      <c r="FR7" s="127" t="s">
+      <c r="FL7" s="150"/>
+      <c r="FM7" s="150"/>
+      <c r="FN7" s="150"/>
+      <c r="FO7" s="150"/>
+      <c r="FP7" s="150"/>
+      <c r="FQ7" s="155"/>
+      <c r="FR7" s="150" t="s">
         <v>59</v>
       </c>
-      <c r="FS7" s="127"/>
-      <c r="FT7" s="127"/>
-      <c r="FU7" s="127"/>
-      <c r="FV7" s="127"/>
-      <c r="FW7" s="127"/>
-      <c r="FX7" s="127"/>
-      <c r="FY7" s="129" t="s">
+      <c r="FS7" s="150"/>
+      <c r="FT7" s="150"/>
+      <c r="FU7" s="150"/>
+      <c r="FV7" s="150"/>
+      <c r="FW7" s="150"/>
+      <c r="FX7" s="150"/>
+      <c r="FY7" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="FZ7" s="127"/>
-      <c r="GA7" s="127"/>
-      <c r="GB7" s="127"/>
-      <c r="GC7" s="128"/>
+      <c r="FZ7" s="150"/>
+      <c r="GA7" s="150"/>
+      <c r="GB7" s="150"/>
+      <c r="GC7" s="172"/>
     </row>
     <row r="8" spans="1:185" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="146" t="s">
+      <c r="A8" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="148"/>
+      <c r="B8" s="152"/>
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="153"/>
       <c r="F8" s="25">
         <v>19</v>
       </c>
@@ -19539,405 +19539,405 @@
         <v>719.99999999999989</v>
       </c>
       <c r="E82" s="121"/>
-      <c r="F82" s="168">
+      <c r="F82" s="131">
         <f>35*C82</f>
         <v>151.80722891566265</v>
       </c>
-      <c r="G82" s="165"/>
-      <c r="H82" s="165"/>
-      <c r="I82" s="165"/>
-      <c r="J82" s="165"/>
-      <c r="K82" s="165"/>
-      <c r="L82" s="165"/>
-      <c r="M82" s="165"/>
-      <c r="N82" s="165"/>
-      <c r="O82" s="165"/>
-      <c r="P82" s="165"/>
-      <c r="Q82" s="165"/>
-      <c r="R82" s="165"/>
-      <c r="S82" s="165"/>
-      <c r="T82" s="165"/>
-      <c r="U82" s="165"/>
-      <c r="V82" s="165"/>
-      <c r="W82" s="165"/>
-      <c r="X82" s="165"/>
-      <c r="Y82" s="165"/>
-      <c r="Z82" s="165"/>
-      <c r="AA82" s="165"/>
-      <c r="AB82" s="165"/>
-      <c r="AC82" s="165"/>
-      <c r="AD82" s="165"/>
-      <c r="AE82" s="165"/>
-      <c r="AF82" s="165"/>
-      <c r="AG82" s="165"/>
-      <c r="AH82" s="165"/>
-      <c r="AI82" s="165"/>
-      <c r="AJ82" s="165"/>
-      <c r="AK82" s="165"/>
-      <c r="AL82" s="165"/>
-      <c r="AM82" s="165"/>
-      <c r="AN82" s="169"/>
-      <c r="AO82" s="170">
+      <c r="G82" s="128"/>
+      <c r="H82" s="128"/>
+      <c r="I82" s="128"/>
+      <c r="J82" s="128"/>
+      <c r="K82" s="128"/>
+      <c r="L82" s="128"/>
+      <c r="M82" s="128"/>
+      <c r="N82" s="128"/>
+      <c r="O82" s="128"/>
+      <c r="P82" s="128"/>
+      <c r="Q82" s="128"/>
+      <c r="R82" s="128"/>
+      <c r="S82" s="128"/>
+      <c r="T82" s="128"/>
+      <c r="U82" s="128"/>
+      <c r="V82" s="128"/>
+      <c r="W82" s="128"/>
+      <c r="X82" s="128"/>
+      <c r="Y82" s="128"/>
+      <c r="Z82" s="128"/>
+      <c r="AA82" s="128"/>
+      <c r="AB82" s="128"/>
+      <c r="AC82" s="128"/>
+      <c r="AD82" s="128"/>
+      <c r="AE82" s="128"/>
+      <c r="AF82" s="128"/>
+      <c r="AG82" s="128"/>
+      <c r="AH82" s="128"/>
+      <c r="AI82" s="128"/>
+      <c r="AJ82" s="128"/>
+      <c r="AK82" s="128"/>
+      <c r="AL82" s="128"/>
+      <c r="AM82" s="128"/>
+      <c r="AN82" s="132"/>
+      <c r="AO82" s="133">
         <f>38*C82</f>
         <v>164.81927710843374</v>
       </c>
-      <c r="AP82" s="165"/>
-      <c r="AQ82" s="165"/>
-      <c r="AR82" s="165"/>
-      <c r="AS82" s="165"/>
-      <c r="AT82" s="165"/>
-      <c r="AU82" s="165"/>
-      <c r="AV82" s="165"/>
-      <c r="AW82" s="165"/>
-      <c r="AX82" s="165"/>
-      <c r="AY82" s="165"/>
-      <c r="AZ82" s="165"/>
-      <c r="BA82" s="165"/>
-      <c r="BB82" s="165"/>
-      <c r="BC82" s="165"/>
-      <c r="BD82" s="165"/>
-      <c r="BE82" s="165"/>
-      <c r="BF82" s="165"/>
-      <c r="BG82" s="165"/>
-      <c r="BH82" s="165"/>
-      <c r="BI82" s="165"/>
-      <c r="BJ82" s="165"/>
-      <c r="BK82" s="165"/>
-      <c r="BL82" s="165"/>
-      <c r="BM82" s="165"/>
-      <c r="BN82" s="165"/>
-      <c r="BO82" s="165"/>
-      <c r="BP82" s="165"/>
-      <c r="BQ82" s="165"/>
-      <c r="BR82" s="165"/>
-      <c r="BS82" s="165"/>
-      <c r="BT82" s="165"/>
-      <c r="BU82" s="165"/>
-      <c r="BV82" s="165"/>
-      <c r="BW82" s="165"/>
-      <c r="BX82" s="165"/>
-      <c r="BY82" s="165"/>
-      <c r="BZ82" s="166"/>
-      <c r="CA82" s="164">
+      <c r="AP82" s="128"/>
+      <c r="AQ82" s="128"/>
+      <c r="AR82" s="128"/>
+      <c r="AS82" s="128"/>
+      <c r="AT82" s="128"/>
+      <c r="AU82" s="128"/>
+      <c r="AV82" s="128"/>
+      <c r="AW82" s="128"/>
+      <c r="AX82" s="128"/>
+      <c r="AY82" s="128"/>
+      <c r="AZ82" s="128"/>
+      <c r="BA82" s="128"/>
+      <c r="BB82" s="128"/>
+      <c r="BC82" s="128"/>
+      <c r="BD82" s="128"/>
+      <c r="BE82" s="128"/>
+      <c r="BF82" s="128"/>
+      <c r="BG82" s="128"/>
+      <c r="BH82" s="128"/>
+      <c r="BI82" s="128"/>
+      <c r="BJ82" s="128"/>
+      <c r="BK82" s="128"/>
+      <c r="BL82" s="128"/>
+      <c r="BM82" s="128"/>
+      <c r="BN82" s="128"/>
+      <c r="BO82" s="128"/>
+      <c r="BP82" s="128"/>
+      <c r="BQ82" s="128"/>
+      <c r="BR82" s="128"/>
+      <c r="BS82" s="128"/>
+      <c r="BT82" s="128"/>
+      <c r="BU82" s="128"/>
+      <c r="BV82" s="128"/>
+      <c r="BW82" s="128"/>
+      <c r="BX82" s="128"/>
+      <c r="BY82" s="128"/>
+      <c r="BZ82" s="129"/>
+      <c r="CA82" s="127">
         <f>21*C82</f>
         <v>91.084337349397586</v>
       </c>
-      <c r="CB82" s="165"/>
-      <c r="CC82" s="165"/>
-      <c r="CD82" s="165"/>
-      <c r="CE82" s="165"/>
-      <c r="CF82" s="165"/>
-      <c r="CG82" s="165"/>
-      <c r="CH82" s="165"/>
-      <c r="CI82" s="165"/>
-      <c r="CJ82" s="165"/>
-      <c r="CK82" s="165"/>
-      <c r="CL82" s="165"/>
-      <c r="CM82" s="165"/>
-      <c r="CN82" s="165"/>
-      <c r="CO82" s="165"/>
-      <c r="CP82" s="165"/>
-      <c r="CQ82" s="165"/>
-      <c r="CR82" s="165"/>
-      <c r="CS82" s="165"/>
-      <c r="CT82" s="165"/>
-      <c r="CU82" s="166"/>
-      <c r="CV82" s="164">
+      <c r="CB82" s="128"/>
+      <c r="CC82" s="128"/>
+      <c r="CD82" s="128"/>
+      <c r="CE82" s="128"/>
+      <c r="CF82" s="128"/>
+      <c r="CG82" s="128"/>
+      <c r="CH82" s="128"/>
+      <c r="CI82" s="128"/>
+      <c r="CJ82" s="128"/>
+      <c r="CK82" s="128"/>
+      <c r="CL82" s="128"/>
+      <c r="CM82" s="128"/>
+      <c r="CN82" s="128"/>
+      <c r="CO82" s="128"/>
+      <c r="CP82" s="128"/>
+      <c r="CQ82" s="128"/>
+      <c r="CR82" s="128"/>
+      <c r="CS82" s="128"/>
+      <c r="CT82" s="128"/>
+      <c r="CU82" s="129"/>
+      <c r="CV82" s="127">
         <f>21*C82</f>
         <v>91.084337349397586</v>
       </c>
-      <c r="CW82" s="165"/>
-      <c r="CX82" s="165"/>
-      <c r="CY82" s="165"/>
-      <c r="CZ82" s="165"/>
-      <c r="DA82" s="165"/>
-      <c r="DB82" s="165"/>
-      <c r="DC82" s="165"/>
-      <c r="DD82" s="165"/>
-      <c r="DE82" s="165"/>
-      <c r="DF82" s="165"/>
-      <c r="DG82" s="165"/>
-      <c r="DH82" s="165"/>
-      <c r="DI82" s="165"/>
-      <c r="DJ82" s="165"/>
-      <c r="DK82" s="165"/>
-      <c r="DL82" s="165"/>
-      <c r="DM82" s="165"/>
-      <c r="DN82" s="165"/>
-      <c r="DO82" s="165"/>
-      <c r="DP82" s="165"/>
-      <c r="DQ82" s="165"/>
-      <c r="DR82" s="165"/>
-      <c r="DS82" s="165"/>
-      <c r="DT82" s="165"/>
-      <c r="DU82" s="165"/>
-      <c r="DV82" s="165"/>
-      <c r="DW82" s="165"/>
-      <c r="DX82" s="165"/>
-      <c r="DY82" s="165"/>
-      <c r="DZ82" s="165"/>
-      <c r="EA82" s="165"/>
-      <c r="EB82" s="165"/>
-      <c r="EC82" s="165"/>
-      <c r="ED82" s="166"/>
-      <c r="EE82" s="164">
+      <c r="CW82" s="128"/>
+      <c r="CX82" s="128"/>
+      <c r="CY82" s="128"/>
+      <c r="CZ82" s="128"/>
+      <c r="DA82" s="128"/>
+      <c r="DB82" s="128"/>
+      <c r="DC82" s="128"/>
+      <c r="DD82" s="128"/>
+      <c r="DE82" s="128"/>
+      <c r="DF82" s="128"/>
+      <c r="DG82" s="128"/>
+      <c r="DH82" s="128"/>
+      <c r="DI82" s="128"/>
+      <c r="DJ82" s="128"/>
+      <c r="DK82" s="128"/>
+      <c r="DL82" s="128"/>
+      <c r="DM82" s="128"/>
+      <c r="DN82" s="128"/>
+      <c r="DO82" s="128"/>
+      <c r="DP82" s="128"/>
+      <c r="DQ82" s="128"/>
+      <c r="DR82" s="128"/>
+      <c r="DS82" s="128"/>
+      <c r="DT82" s="128"/>
+      <c r="DU82" s="128"/>
+      <c r="DV82" s="128"/>
+      <c r="DW82" s="128"/>
+      <c r="DX82" s="128"/>
+      <c r="DY82" s="128"/>
+      <c r="DZ82" s="128"/>
+      <c r="EA82" s="128"/>
+      <c r="EB82" s="128"/>
+      <c r="EC82" s="128"/>
+      <c r="ED82" s="129"/>
+      <c r="EE82" s="127">
         <f>34*C82</f>
         <v>147.46987951807228</v>
       </c>
-      <c r="EF82" s="165"/>
-      <c r="EG82" s="165"/>
-      <c r="EH82" s="165"/>
-      <c r="EI82" s="165"/>
-      <c r="EJ82" s="165"/>
-      <c r="EK82" s="165"/>
-      <c r="EL82" s="165"/>
-      <c r="EM82" s="165"/>
-      <c r="EN82" s="165"/>
-      <c r="EO82" s="165"/>
-      <c r="EP82" s="165"/>
-      <c r="EQ82" s="165"/>
-      <c r="ER82" s="165"/>
-      <c r="ES82" s="165"/>
-      <c r="ET82" s="165"/>
-      <c r="EU82" s="165"/>
-      <c r="EV82" s="165"/>
-      <c r="EW82" s="165"/>
-      <c r="EX82" s="165"/>
-      <c r="EY82" s="165"/>
-      <c r="EZ82" s="165"/>
-      <c r="FA82" s="165"/>
-      <c r="FB82" s="165"/>
-      <c r="FC82" s="165"/>
-      <c r="FD82" s="165"/>
-      <c r="FE82" s="165"/>
-      <c r="FF82" s="165"/>
-      <c r="FG82" s="165"/>
-      <c r="FH82" s="165"/>
-      <c r="FI82" s="165"/>
-      <c r="FJ82" s="165"/>
-      <c r="FK82" s="165"/>
-      <c r="FL82" s="166"/>
-      <c r="FM82" s="164">
+      <c r="EF82" s="128"/>
+      <c r="EG82" s="128"/>
+      <c r="EH82" s="128"/>
+      <c r="EI82" s="128"/>
+      <c r="EJ82" s="128"/>
+      <c r="EK82" s="128"/>
+      <c r="EL82" s="128"/>
+      <c r="EM82" s="128"/>
+      <c r="EN82" s="128"/>
+      <c r="EO82" s="128"/>
+      <c r="EP82" s="128"/>
+      <c r="EQ82" s="128"/>
+      <c r="ER82" s="128"/>
+      <c r="ES82" s="128"/>
+      <c r="ET82" s="128"/>
+      <c r="EU82" s="128"/>
+      <c r="EV82" s="128"/>
+      <c r="EW82" s="128"/>
+      <c r="EX82" s="128"/>
+      <c r="EY82" s="128"/>
+      <c r="EZ82" s="128"/>
+      <c r="FA82" s="128"/>
+      <c r="FB82" s="128"/>
+      <c r="FC82" s="128"/>
+      <c r="FD82" s="128"/>
+      <c r="FE82" s="128"/>
+      <c r="FF82" s="128"/>
+      <c r="FG82" s="128"/>
+      <c r="FH82" s="128"/>
+      <c r="FI82" s="128"/>
+      <c r="FJ82" s="128"/>
+      <c r="FK82" s="128"/>
+      <c r="FL82" s="129"/>
+      <c r="FM82" s="127">
         <f>17*C82</f>
         <v>73.734939759036138</v>
       </c>
-      <c r="FN82" s="165"/>
-      <c r="FO82" s="165"/>
-      <c r="FP82" s="165"/>
-      <c r="FQ82" s="165"/>
-      <c r="FR82" s="165"/>
-      <c r="FS82" s="165"/>
-      <c r="FT82" s="165"/>
-      <c r="FU82" s="165"/>
-      <c r="FV82" s="165"/>
-      <c r="FW82" s="165"/>
-      <c r="FX82" s="165"/>
-      <c r="FY82" s="165"/>
-      <c r="FZ82" s="165"/>
-      <c r="GA82" s="165"/>
-      <c r="GB82" s="165"/>
-      <c r="GC82" s="167"/>
+      <c r="FN82" s="128"/>
+      <c r="FO82" s="128"/>
+      <c r="FP82" s="128"/>
+      <c r="FQ82" s="128"/>
+      <c r="FR82" s="128"/>
+      <c r="FS82" s="128"/>
+      <c r="FT82" s="128"/>
+      <c r="FU82" s="128"/>
+      <c r="FV82" s="128"/>
+      <c r="FW82" s="128"/>
+      <c r="FX82" s="128"/>
+      <c r="FY82" s="128"/>
+      <c r="FZ82" s="128"/>
+      <c r="GA82" s="128"/>
+      <c r="GB82" s="128"/>
+      <c r="GC82" s="130"/>
     </row>
     <row r="83" spans="1:187" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="158" t="s">
+      <c r="A83" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="159"/>
-      <c r="C83" s="159"/>
-      <c r="D83" s="159"/>
-      <c r="E83" s="160"/>
-      <c r="F83" s="161" t="s">
+      <c r="B83" s="139"/>
+      <c r="C83" s="139"/>
+      <c r="D83" s="139"/>
+      <c r="E83" s="140"/>
+      <c r="F83" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="G83" s="155"/>
-      <c r="H83" s="155"/>
-      <c r="I83" s="155"/>
-      <c r="J83" s="155"/>
-      <c r="K83" s="155"/>
-      <c r="L83" s="155"/>
-      <c r="M83" s="155"/>
-      <c r="N83" s="155"/>
-      <c r="O83" s="155"/>
-      <c r="P83" s="155"/>
-      <c r="Q83" s="155"/>
-      <c r="R83" s="155"/>
-      <c r="S83" s="155"/>
-      <c r="T83" s="155"/>
-      <c r="U83" s="155"/>
-      <c r="V83" s="155"/>
-      <c r="W83" s="155"/>
-      <c r="X83" s="155"/>
-      <c r="Y83" s="155"/>
-      <c r="Z83" s="155"/>
-      <c r="AA83" s="155"/>
-      <c r="AB83" s="155"/>
-      <c r="AC83" s="155"/>
-      <c r="AD83" s="155"/>
-      <c r="AE83" s="155"/>
-      <c r="AF83" s="155"/>
-      <c r="AG83" s="155"/>
-      <c r="AH83" s="155"/>
-      <c r="AI83" s="155"/>
-      <c r="AJ83" s="155"/>
-      <c r="AK83" s="155"/>
-      <c r="AL83" s="155"/>
-      <c r="AM83" s="155"/>
-      <c r="AN83" s="162"/>
-      <c r="AO83" s="163" t="s">
+      <c r="G83" s="135"/>
+      <c r="H83" s="135"/>
+      <c r="I83" s="135"/>
+      <c r="J83" s="135"/>
+      <c r="K83" s="135"/>
+      <c r="L83" s="135"/>
+      <c r="M83" s="135"/>
+      <c r="N83" s="135"/>
+      <c r="O83" s="135"/>
+      <c r="P83" s="135"/>
+      <c r="Q83" s="135"/>
+      <c r="R83" s="135"/>
+      <c r="S83" s="135"/>
+      <c r="T83" s="135"/>
+      <c r="U83" s="135"/>
+      <c r="V83" s="135"/>
+      <c r="W83" s="135"/>
+      <c r="X83" s="135"/>
+      <c r="Y83" s="135"/>
+      <c r="Z83" s="135"/>
+      <c r="AA83" s="135"/>
+      <c r="AB83" s="135"/>
+      <c r="AC83" s="135"/>
+      <c r="AD83" s="135"/>
+      <c r="AE83" s="135"/>
+      <c r="AF83" s="135"/>
+      <c r="AG83" s="135"/>
+      <c r="AH83" s="135"/>
+      <c r="AI83" s="135"/>
+      <c r="AJ83" s="135"/>
+      <c r="AK83" s="135"/>
+      <c r="AL83" s="135"/>
+      <c r="AM83" s="135"/>
+      <c r="AN83" s="142"/>
+      <c r="AO83" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="AP83" s="155"/>
-      <c r="AQ83" s="155"/>
-      <c r="AR83" s="155"/>
-      <c r="AS83" s="155"/>
-      <c r="AT83" s="155"/>
-      <c r="AU83" s="155"/>
-      <c r="AV83" s="155"/>
-      <c r="AW83" s="155"/>
-      <c r="AX83" s="155"/>
-      <c r="AY83" s="155"/>
-      <c r="AZ83" s="155"/>
-      <c r="BA83" s="155"/>
-      <c r="BB83" s="155"/>
-      <c r="BC83" s="155"/>
-      <c r="BD83" s="155"/>
-      <c r="BE83" s="155"/>
-      <c r="BF83" s="155"/>
-      <c r="BG83" s="155"/>
-      <c r="BH83" s="155"/>
-      <c r="BI83" s="155"/>
-      <c r="BJ83" s="155"/>
-      <c r="BK83" s="155"/>
-      <c r="BL83" s="155"/>
-      <c r="BM83" s="155"/>
-      <c r="BN83" s="155"/>
-      <c r="BO83" s="155"/>
-      <c r="BP83" s="155"/>
-      <c r="BQ83" s="155"/>
-      <c r="BR83" s="155"/>
-      <c r="BS83" s="155"/>
-      <c r="BT83" s="155"/>
-      <c r="BU83" s="155"/>
-      <c r="BV83" s="155"/>
-      <c r="BW83" s="155"/>
-      <c r="BX83" s="155"/>
-      <c r="BY83" s="155"/>
-      <c r="BZ83" s="156"/>
-      <c r="CA83" s="154" t="s">
+      <c r="AP83" s="135"/>
+      <c r="AQ83" s="135"/>
+      <c r="AR83" s="135"/>
+      <c r="AS83" s="135"/>
+      <c r="AT83" s="135"/>
+      <c r="AU83" s="135"/>
+      <c r="AV83" s="135"/>
+      <c r="AW83" s="135"/>
+      <c r="AX83" s="135"/>
+      <c r="AY83" s="135"/>
+      <c r="AZ83" s="135"/>
+      <c r="BA83" s="135"/>
+      <c r="BB83" s="135"/>
+      <c r="BC83" s="135"/>
+      <c r="BD83" s="135"/>
+      <c r="BE83" s="135"/>
+      <c r="BF83" s="135"/>
+      <c r="BG83" s="135"/>
+      <c r="BH83" s="135"/>
+      <c r="BI83" s="135"/>
+      <c r="BJ83" s="135"/>
+      <c r="BK83" s="135"/>
+      <c r="BL83" s="135"/>
+      <c r="BM83" s="135"/>
+      <c r="BN83" s="135"/>
+      <c r="BO83" s="135"/>
+      <c r="BP83" s="135"/>
+      <c r="BQ83" s="135"/>
+      <c r="BR83" s="135"/>
+      <c r="BS83" s="135"/>
+      <c r="BT83" s="135"/>
+      <c r="BU83" s="135"/>
+      <c r="BV83" s="135"/>
+      <c r="BW83" s="135"/>
+      <c r="BX83" s="135"/>
+      <c r="BY83" s="135"/>
+      <c r="BZ83" s="136"/>
+      <c r="CA83" s="134" t="s">
         <v>92</v>
       </c>
-      <c r="CB83" s="155"/>
-      <c r="CC83" s="155"/>
-      <c r="CD83" s="155"/>
-      <c r="CE83" s="155"/>
-      <c r="CF83" s="155"/>
-      <c r="CG83" s="155"/>
-      <c r="CH83" s="155"/>
-      <c r="CI83" s="155"/>
-      <c r="CJ83" s="155"/>
-      <c r="CK83" s="155"/>
-      <c r="CL83" s="155"/>
-      <c r="CM83" s="155"/>
-      <c r="CN83" s="155"/>
-      <c r="CO83" s="155"/>
-      <c r="CP83" s="155"/>
-      <c r="CQ83" s="155"/>
-      <c r="CR83" s="155"/>
-      <c r="CS83" s="155"/>
-      <c r="CT83" s="155"/>
-      <c r="CU83" s="156"/>
-      <c r="CV83" s="154" t="s">
+      <c r="CB83" s="135"/>
+      <c r="CC83" s="135"/>
+      <c r="CD83" s="135"/>
+      <c r="CE83" s="135"/>
+      <c r="CF83" s="135"/>
+      <c r="CG83" s="135"/>
+      <c r="CH83" s="135"/>
+      <c r="CI83" s="135"/>
+      <c r="CJ83" s="135"/>
+      <c r="CK83" s="135"/>
+      <c r="CL83" s="135"/>
+      <c r="CM83" s="135"/>
+      <c r="CN83" s="135"/>
+      <c r="CO83" s="135"/>
+      <c r="CP83" s="135"/>
+      <c r="CQ83" s="135"/>
+      <c r="CR83" s="135"/>
+      <c r="CS83" s="135"/>
+      <c r="CT83" s="135"/>
+      <c r="CU83" s="136"/>
+      <c r="CV83" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="CW83" s="155"/>
-      <c r="CX83" s="155"/>
-      <c r="CY83" s="155"/>
-      <c r="CZ83" s="155"/>
-      <c r="DA83" s="155"/>
-      <c r="DB83" s="155"/>
-      <c r="DC83" s="155"/>
-      <c r="DD83" s="155"/>
-      <c r="DE83" s="155"/>
-      <c r="DF83" s="155"/>
-      <c r="DG83" s="155"/>
-      <c r="DH83" s="155"/>
-      <c r="DI83" s="155"/>
-      <c r="DJ83" s="155"/>
-      <c r="DK83" s="155"/>
-      <c r="DL83" s="155"/>
-      <c r="DM83" s="155"/>
-      <c r="DN83" s="155"/>
-      <c r="DO83" s="155"/>
-      <c r="DP83" s="155"/>
-      <c r="DQ83" s="155"/>
-      <c r="DR83" s="155"/>
-      <c r="DS83" s="155"/>
-      <c r="DT83" s="155"/>
-      <c r="DU83" s="155"/>
-      <c r="DV83" s="155"/>
-      <c r="DW83" s="155"/>
-      <c r="DX83" s="155"/>
-      <c r="DY83" s="155"/>
-      <c r="DZ83" s="155"/>
-      <c r="EA83" s="155"/>
-      <c r="EB83" s="155"/>
-      <c r="EC83" s="155"/>
-      <c r="ED83" s="156"/>
-      <c r="EE83" s="154" t="s">
+      <c r="CW83" s="135"/>
+      <c r="CX83" s="135"/>
+      <c r="CY83" s="135"/>
+      <c r="CZ83" s="135"/>
+      <c r="DA83" s="135"/>
+      <c r="DB83" s="135"/>
+      <c r="DC83" s="135"/>
+      <c r="DD83" s="135"/>
+      <c r="DE83" s="135"/>
+      <c r="DF83" s="135"/>
+      <c r="DG83" s="135"/>
+      <c r="DH83" s="135"/>
+      <c r="DI83" s="135"/>
+      <c r="DJ83" s="135"/>
+      <c r="DK83" s="135"/>
+      <c r="DL83" s="135"/>
+      <c r="DM83" s="135"/>
+      <c r="DN83" s="135"/>
+      <c r="DO83" s="135"/>
+      <c r="DP83" s="135"/>
+      <c r="DQ83" s="135"/>
+      <c r="DR83" s="135"/>
+      <c r="DS83" s="135"/>
+      <c r="DT83" s="135"/>
+      <c r="DU83" s="135"/>
+      <c r="DV83" s="135"/>
+      <c r="DW83" s="135"/>
+      <c r="DX83" s="135"/>
+      <c r="DY83" s="135"/>
+      <c r="DZ83" s="135"/>
+      <c r="EA83" s="135"/>
+      <c r="EB83" s="135"/>
+      <c r="EC83" s="135"/>
+      <c r="ED83" s="136"/>
+      <c r="EE83" s="134" t="s">
         <v>94</v>
       </c>
-      <c r="EF83" s="155"/>
-      <c r="EG83" s="155"/>
-      <c r="EH83" s="155"/>
-      <c r="EI83" s="155"/>
-      <c r="EJ83" s="155"/>
-      <c r="EK83" s="155"/>
-      <c r="EL83" s="155"/>
-      <c r="EM83" s="155"/>
-      <c r="EN83" s="155"/>
-      <c r="EO83" s="155"/>
-      <c r="EP83" s="155"/>
-      <c r="EQ83" s="155"/>
-      <c r="ER83" s="155"/>
-      <c r="ES83" s="155"/>
-      <c r="ET83" s="155"/>
-      <c r="EU83" s="155"/>
-      <c r="EV83" s="155"/>
-      <c r="EW83" s="155"/>
-      <c r="EX83" s="155"/>
-      <c r="EY83" s="155"/>
-      <c r="EZ83" s="155"/>
-      <c r="FA83" s="155"/>
-      <c r="FB83" s="155"/>
-      <c r="FC83" s="155"/>
-      <c r="FD83" s="155"/>
-      <c r="FE83" s="155"/>
-      <c r="FF83" s="155"/>
-      <c r="FG83" s="155"/>
-      <c r="FH83" s="155"/>
-      <c r="FI83" s="155"/>
-      <c r="FJ83" s="155"/>
-      <c r="FK83" s="155"/>
-      <c r="FL83" s="156"/>
-      <c r="FM83" s="154" t="s">
+      <c r="EF83" s="135"/>
+      <c r="EG83" s="135"/>
+      <c r="EH83" s="135"/>
+      <c r="EI83" s="135"/>
+      <c r="EJ83" s="135"/>
+      <c r="EK83" s="135"/>
+      <c r="EL83" s="135"/>
+      <c r="EM83" s="135"/>
+      <c r="EN83" s="135"/>
+      <c r="EO83" s="135"/>
+      <c r="EP83" s="135"/>
+      <c r="EQ83" s="135"/>
+      <c r="ER83" s="135"/>
+      <c r="ES83" s="135"/>
+      <c r="ET83" s="135"/>
+      <c r="EU83" s="135"/>
+      <c r="EV83" s="135"/>
+      <c r="EW83" s="135"/>
+      <c r="EX83" s="135"/>
+      <c r="EY83" s="135"/>
+      <c r="EZ83" s="135"/>
+      <c r="FA83" s="135"/>
+      <c r="FB83" s="135"/>
+      <c r="FC83" s="135"/>
+      <c r="FD83" s="135"/>
+      <c r="FE83" s="135"/>
+      <c r="FF83" s="135"/>
+      <c r="FG83" s="135"/>
+      <c r="FH83" s="135"/>
+      <c r="FI83" s="135"/>
+      <c r="FJ83" s="135"/>
+      <c r="FK83" s="135"/>
+      <c r="FL83" s="136"/>
+      <c r="FM83" s="134" t="s">
         <v>91</v>
       </c>
-      <c r="FN83" s="155"/>
-      <c r="FO83" s="155"/>
-      <c r="FP83" s="155"/>
-      <c r="FQ83" s="155"/>
-      <c r="FR83" s="155"/>
-      <c r="FS83" s="155"/>
-      <c r="FT83" s="155"/>
-      <c r="FU83" s="155"/>
-      <c r="FV83" s="155"/>
-      <c r="FW83" s="155"/>
-      <c r="FX83" s="155"/>
-      <c r="FY83" s="155"/>
-      <c r="FZ83" s="155"/>
-      <c r="GA83" s="155"/>
-      <c r="GB83" s="155"/>
-      <c r="GC83" s="157"/>
+      <c r="FN83" s="135"/>
+      <c r="FO83" s="135"/>
+      <c r="FP83" s="135"/>
+      <c r="FQ83" s="135"/>
+      <c r="FR83" s="135"/>
+      <c r="FS83" s="135"/>
+      <c r="FT83" s="135"/>
+      <c r="FU83" s="135"/>
+      <c r="FV83" s="135"/>
+      <c r="FW83" s="135"/>
+      <c r="FX83" s="135"/>
+      <c r="FY83" s="135"/>
+      <c r="FZ83" s="135"/>
+      <c r="GA83" s="135"/>
+      <c r="GB83" s="135"/>
+      <c r="GC83" s="137"/>
     </row>
     <row r="85" spans="1:187" x14ac:dyDescent="0.2">
       <c r="GE85" s="117"/>
@@ -19947,53 +19947,6 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="EE82:FL82"/>
-    <mergeCell ref="FM82:GC82"/>
-    <mergeCell ref="F82:AN82"/>
-    <mergeCell ref="AO82:BZ82"/>
-    <mergeCell ref="CA82:CU82"/>
-    <mergeCell ref="CV82:ED82"/>
-    <mergeCell ref="EE83:FL83"/>
-    <mergeCell ref="FM83:GC83"/>
-    <mergeCell ref="A83:E83"/>
-    <mergeCell ref="F83:AN83"/>
-    <mergeCell ref="AO83:BZ83"/>
-    <mergeCell ref="CA83:CU83"/>
-    <mergeCell ref="CV83:ED83"/>
-    <mergeCell ref="F4:AN4"/>
-    <mergeCell ref="AO4:BZ4"/>
-    <mergeCell ref="FM4:GC4"/>
-    <mergeCell ref="CA4:CU4"/>
-    <mergeCell ref="CV4:ED4"/>
-    <mergeCell ref="EE4:FL4"/>
-    <mergeCell ref="F6:Q6"/>
-    <mergeCell ref="R6:AV6"/>
-    <mergeCell ref="AW6:BZ6"/>
-    <mergeCell ref="CA6:DE6"/>
-    <mergeCell ref="F5:DE5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="BQ7:BW7"/>
-    <mergeCell ref="BX7:CD7"/>
-    <mergeCell ref="CE7:CK7"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="M7:S7"/>
-    <mergeCell ref="T7:Z7"/>
-    <mergeCell ref="AA7:AG7"/>
-    <mergeCell ref="CL7:CR7"/>
-    <mergeCell ref="CS7:CY7"/>
-    <mergeCell ref="CZ7:DF7"/>
-    <mergeCell ref="DG7:DM7"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="AH7:AN7"/>
-    <mergeCell ref="AO7:AU7"/>
-    <mergeCell ref="AV7:BB7"/>
-    <mergeCell ref="BC7:BI7"/>
-    <mergeCell ref="BJ7:BP7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A2:E2"/>
     <mergeCell ref="EK6:FL6"/>
     <mergeCell ref="FM6:GC6"/>
     <mergeCell ref="DF5:GC5"/>
@@ -20008,6 +19961,53 @@
     <mergeCell ref="FY7:GC7"/>
     <mergeCell ref="DN7:DT7"/>
     <mergeCell ref="DF6:EJ6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="CL7:CR7"/>
+    <mergeCell ref="CS7:CY7"/>
+    <mergeCell ref="CZ7:DF7"/>
+    <mergeCell ref="DG7:DM7"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="AH7:AN7"/>
+    <mergeCell ref="AO7:AU7"/>
+    <mergeCell ref="AV7:BB7"/>
+    <mergeCell ref="BC7:BI7"/>
+    <mergeCell ref="BJ7:BP7"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="BQ7:BW7"/>
+    <mergeCell ref="BX7:CD7"/>
+    <mergeCell ref="CE7:CK7"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="M7:S7"/>
+    <mergeCell ref="T7:Z7"/>
+    <mergeCell ref="AA7:AG7"/>
+    <mergeCell ref="F6:Q6"/>
+    <mergeCell ref="R6:AV6"/>
+    <mergeCell ref="AW6:BZ6"/>
+    <mergeCell ref="CA6:DE6"/>
+    <mergeCell ref="F5:DE5"/>
+    <mergeCell ref="F4:AN4"/>
+    <mergeCell ref="AO4:BZ4"/>
+    <mergeCell ref="FM4:GC4"/>
+    <mergeCell ref="CA4:CU4"/>
+    <mergeCell ref="CV4:ED4"/>
+    <mergeCell ref="EE4:FL4"/>
+    <mergeCell ref="EE83:FL83"/>
+    <mergeCell ref="FM83:GC83"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="F83:AN83"/>
+    <mergeCell ref="AO83:BZ83"/>
+    <mergeCell ref="CA83:CU83"/>
+    <mergeCell ref="CV83:ED83"/>
+    <mergeCell ref="EE82:FL82"/>
+    <mergeCell ref="FM82:GC82"/>
+    <mergeCell ref="F82:AN82"/>
+    <mergeCell ref="AO82:BZ82"/>
+    <mergeCell ref="CA82:CU82"/>
+    <mergeCell ref="CV82:ED82"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -20020,14 +20020,14 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="124"/>
-    <col min="5" max="5" width="10.83203125" style="172"/>
+    <col min="5" max="5" width="10.83203125" style="126"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20044,7 +20044,7 @@
       <c r="D1" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="171" t="s">
+      <c r="E1" s="125" t="s">
         <v>166</v>
       </c>
       <c r="F1" s="122" t="s">
@@ -20065,7 +20065,7 @@
       <c r="D2" s="124">
         <v>57</v>
       </c>
-      <c r="E2" s="172">
+      <c r="E2" s="126">
         <v>51</v>
       </c>
       <c r="F2" t="s">
@@ -20086,7 +20086,7 @@
       <c r="D3" s="124">
         <v>71</v>
       </c>
-      <c r="E3" s="172">
+      <c r="E3" s="126">
         <v>77</v>
       </c>
       <c r="F3" t="s">
@@ -20107,7 +20107,7 @@
       <c r="D4" s="124">
         <v>45</v>
       </c>
-      <c r="E4" s="172">
+      <c r="E4" s="126">
         <v>52</v>
       </c>
       <c r="F4" t="s">
@@ -20128,7 +20128,7 @@
       <c r="D5" s="124">
         <v>54</v>
       </c>
-      <c r="E5" s="172">
+      <c r="E5" s="126">
         <v>23</v>
       </c>
       <c r="F5" t="s">
@@ -20149,7 +20149,7 @@
       <c r="D6" s="124">
         <v>87</v>
       </c>
-      <c r="E6" s="172">
+      <c r="E6" s="126">
         <v>120</v>
       </c>
       <c r="F6" t="s">
@@ -20170,7 +20170,7 @@
       <c r="D7" s="124">
         <v>71</v>
       </c>
-      <c r="E7" s="172">
+      <c r="E7" s="126">
         <v>68</v>
       </c>
       <c r="F7" t="s">

</xml_diff>